<commit_message>
Bug fixes and slight moveset tweaks
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Microsoft\Excel\Pokemon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2471D2-193A-456F-9FD1-F73233B1B757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13515A-A193-474C-85F8-AA815FE7937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2403" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="1156">
   <si>
     <t>Leafer</t>
   </si>
@@ -3425,9 +3425,6 @@
     <t>Reckless</t>
   </si>
   <si>
-    <t>Glimmora</t>
-  </si>
-  <si>
     <t>Pigoga+</t>
   </si>
   <si>
@@ -3441,6 +3438,72 @@
   </si>
   <si>
     <t>Poison Heal</t>
+  </si>
+  <si>
+    <t>1. Glimmora</t>
+  </si>
+  <si>
+    <t>2. Roserade</t>
+  </si>
+  <si>
+    <t>3. Zurroaratr-S</t>
+  </si>
+  <si>
+    <t>4. Arbok</t>
+  </si>
+  <si>
+    <t>1. Magron</t>
+  </si>
+  <si>
+    <t>2. Megawatt</t>
+  </si>
+  <si>
+    <t>3. Hast</t>
+  </si>
+  <si>
+    <t>4. Soldrota</t>
+  </si>
+  <si>
+    <t>1. Dragave</t>
+  </si>
+  <si>
+    <t>2. Treewin</t>
+  </si>
+  <si>
+    <t>3. Raptorex</t>
+  </si>
+  <si>
+    <t>4. Pyrator</t>
+  </si>
+  <si>
+    <t>5. Pyrator-S</t>
+  </si>
+  <si>
+    <t>6. Soldrota-E</t>
+  </si>
+  <si>
+    <t>7. Conkeldurr</t>
+  </si>
+  <si>
+    <t>8. Scraftagon</t>
+  </si>
+  <si>
+    <t>Dragave: Spikes/Wave Crash/Summit Strike</t>
+  </si>
+  <si>
+    <t>Magron: Eruption/Fire Blast/Spikes/Stealth Rock/Molten Steelspike/Steel Beam</t>
+  </si>
+  <si>
+    <t>Glimmora: Rocks/Sludge Wave/Toxic/Earth Power/Energy Ball/Power Gem/Spiky Shield/Toxic</t>
+  </si>
+  <si>
+    <t>Roserade: Spikes/Venom Drench/Leech Seed/Toxic/Protect/Magical Leaf/Leaf Storm/Sludge Bomb/Sleep Powder/Synthesis</t>
+  </si>
+  <si>
+    <t>Arbok: Coil/Sucker Punch/Gunk Shot/Magic Fang/Thunder Fang</t>
+  </si>
+  <si>
+    <t>Zurroaratr-S: Nasty Plot/Venom Drench/Dark Pulse/Giga Drain/Silver Wind/Star Storm</t>
   </si>
 </sst>
 </file>
@@ -4186,13 +4249,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AT622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L217" sqref="L217"/>
+    <sheetView tabSelected="1" topLeftCell="I29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
     <col min="5" max="5" width="11" style="3" customWidth="1"/>
@@ -4202,20 +4265,20 @@
     <col min="9" max="9" width="11" style="6" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" customWidth="1"/>
     <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" customWidth="1"/>
-    <col min="26" max="28" width="10.85546875" customWidth="1"/>
-    <col min="29" max="31" width="7.7109375" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" customWidth="1"/>
-    <col min="33" max="46" width="7.7109375" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" customWidth="1"/>
+    <col min="26" max="28" width="10.88671875" customWidth="1"/>
+    <col min="29" max="31" width="7.6640625" customWidth="1"/>
+    <col min="32" max="32" width="11.44140625" customWidth="1"/>
+    <col min="33" max="46" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>-1</v>
       </c>
@@ -4333,7 +4396,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -4401,7 +4464,7 @@
       <c r="AQ2" s="18"/>
       <c r="AS2" s="17"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-3</v>
       </c>
@@ -4474,7 +4537,7 @@
       <c r="AQ3" s="17"/>
       <c r="AT3" s="19"/>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-4</v>
       </c>
@@ -4542,7 +4605,7 @@
       <c r="AM4" s="17"/>
       <c r="AO4" s="18"/>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>-5</v>
       </c>
@@ -4615,7 +4678,7 @@
       <c r="AR5" s="17"/>
       <c r="AT5" s="18"/>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>-6</v>
       </c>
@@ -4682,7 +4745,7 @@
       <c r="AO6" s="18"/>
       <c r="AQ6" s="17"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>-7</v>
       </c>
@@ -4749,7 +4812,7 @@
       <c r="AO7" s="17"/>
       <c r="AQ7" s="18"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>-8</v>
       </c>
@@ -4820,7 +4883,7 @@
       <c r="AS8" s="18"/>
       <c r="AT8" s="18"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>-9</v>
       </c>
@@ -4889,7 +4952,7 @@
       <c r="AQ9" s="19"/>
       <c r="AS9" s="17"/>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>-10</v>
       </c>
@@ -4953,7 +5016,7 @@
       <c r="AQ10" s="17"/>
       <c r="AT10" s="18"/>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>-11</v>
       </c>
@@ -5014,7 +5077,7 @@
       <c r="AQ11" s="18"/>
       <c r="AT11" s="17"/>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>-12</v>
       </c>
@@ -5074,7 +5137,7 @@
       <c r="AP12" s="19"/>
       <c r="AS12" s="18"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>-13</v>
       </c>
@@ -5140,7 +5203,7 @@
       <c r="AR13" s="17"/>
       <c r="AT13" s="18"/>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>-14</v>
       </c>
@@ -5197,7 +5260,7 @@
       <c r="AQ14" s="18"/>
       <c r="AT14" s="17"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>-15</v>
       </c>
@@ -5252,7 +5315,7 @@
       <c r="AP15" s="18"/>
       <c r="AR15" s="18"/>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>-16</v>
       </c>
@@ -5304,7 +5367,7 @@
       <c r="AQ16" s="18"/>
       <c r="AS16" s="19"/>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>-17</v>
       </c>
@@ -5364,7 +5427,7 @@
       <c r="AP17" s="18"/>
       <c r="AR17" s="18"/>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>-18</v>
       </c>
@@ -5430,7 +5493,7 @@
       <c r="AR18" s="17"/>
       <c r="AS18" s="18"/>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>-19</v>
       </c>
@@ -5494,7 +5557,7 @@
       <c r="AR19" s="18"/>
       <c r="AT19" s="17"/>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>-20</v>
       </c>
@@ -5555,7 +5618,7 @@
       <c r="AQ20" s="17"/>
       <c r="AS20" s="18"/>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>-21</v>
       </c>
@@ -5608,7 +5671,7 @@
       <c r="AQ21" s="18"/>
       <c r="AR21" s="18"/>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>-22</v>
       </c>
@@ -5657,7 +5720,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>-23</v>
       </c>
@@ -5705,7 +5768,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>-24</v>
       </c>
@@ -5753,7 +5816,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>-25</v>
       </c>
@@ -5801,7 +5864,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>-26</v>
       </c>
@@ -5846,7 +5909,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>-27</v>
       </c>
@@ -5891,7 +5954,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>-28</v>
       </c>
@@ -5936,7 +5999,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>-29</v>
       </c>
@@ -6008,7 +6071,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>-30</v>
       </c>
@@ -6075,7 +6138,7 @@
         <v>1.66E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>-31</v>
       </c>
@@ -6142,7 +6205,7 @@
         <v>1.41E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>-32</v>
       </c>
@@ -6215,7 +6278,7 @@
         <v>1.41E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>-33</v>
       </c>
@@ -6297,7 +6360,7 @@
         <v>1.2800000000000001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>-34</v>
       </c>
@@ -6332,14 +6395,14 @@
       <c r="M34" t="s">
         <v>19</v>
       </c>
-      <c r="N34" t="s">
-        <v>511</v>
+      <c r="N34" s="39" t="s">
+        <v>1134</v>
       </c>
       <c r="O34" t="s">
-        <v>1087</v>
+        <v>1138</v>
       </c>
       <c r="P34" t="s">
-        <v>397</v>
+        <v>1142</v>
       </c>
       <c r="T34" t="s">
         <v>208</v>
@@ -6376,7 +6439,7 @@
         <v>1.2800000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>-35</v>
       </c>
@@ -6412,13 +6475,13 @@
         <v>486</v>
       </c>
       <c r="N35" t="s">
-        <v>1090</v>
+        <v>1135</v>
       </c>
       <c r="O35" t="s">
-        <v>483</v>
+        <v>1139</v>
       </c>
       <c r="P35" t="s">
-        <v>12</v>
+        <v>1143</v>
       </c>
       <c r="T35" t="s">
         <v>210</v>
@@ -6455,7 +6518,7 @@
         <v>1.2800000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>-36</v>
       </c>
@@ -6491,13 +6554,13 @@
         <v>508</v>
       </c>
       <c r="N36" t="s">
-        <v>803</v>
+        <v>1136</v>
       </c>
       <c r="O36" t="s">
-        <v>1092</v>
+        <v>1140</v>
       </c>
       <c r="P36" t="s">
-        <v>1094</v>
+        <v>1144</v>
       </c>
       <c r="T36" t="s">
         <v>212</v>
@@ -6534,7 +6597,7 @@
         <v>1.15E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>-37</v>
       </c>
@@ -6570,13 +6633,13 @@
         <v>70</v>
       </c>
       <c r="N37" t="s">
-        <v>1091</v>
+        <v>1137</v>
       </c>
       <c r="O37" t="s">
-        <v>38</v>
+        <v>1141</v>
       </c>
       <c r="P37" t="s">
-        <v>434</v>
+        <v>1145</v>
       </c>
       <c r="W37" s="11" t="s">
         <v>176</v>
@@ -6610,7 +6673,7 @@
         <v>1.15E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>-38</v>
       </c>
@@ -6646,13 +6709,13 @@
         <v>520</v>
       </c>
       <c r="N38" t="s">
-        <v>415</v>
+        <v>1090</v>
       </c>
       <c r="O38" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="P38" t="s">
-        <v>1131</v>
+        <v>1146</v>
       </c>
       <c r="W38" t="s">
         <v>214</v>
@@ -6686,7 +6749,7 @@
         <v>1.15E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>-39</v>
       </c>
@@ -6722,13 +6785,13 @@
         <v>523</v>
       </c>
       <c r="N39" t="s">
-        <v>1074</v>
+        <v>1091</v>
       </c>
       <c r="O39" t="s">
-        <v>94</v>
+        <v>1129</v>
       </c>
       <c r="P39" t="s">
-        <v>443</v>
+        <v>1147</v>
       </c>
       <c r="W39" t="s">
         <v>215</v>
@@ -6762,7 +6825,7 @@
         <v>1.15E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>-40</v>
       </c>
@@ -6797,14 +6860,14 @@
       <c r="M40" t="s">
         <v>556</v>
       </c>
-      <c r="N40" s="39" t="s">
-        <v>1129</v>
+      <c r="N40" t="s">
+        <v>1074</v>
       </c>
       <c r="O40" t="s">
-        <v>394</v>
+        <v>1087</v>
       </c>
       <c r="P40" t="s">
-        <v>1098</v>
+        <v>1148</v>
       </c>
       <c r="W40" s="10" t="s">
         <v>216</v>
@@ -6838,7 +6901,7 @@
         <v>1.15E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>-41</v>
       </c>
@@ -6874,10 +6937,10 @@
         <v>1095</v>
       </c>
       <c r="O41" t="s">
-        <v>1130</v>
+        <v>1093</v>
       </c>
       <c r="P41" t="s">
-        <v>472</v>
+        <v>1149</v>
       </c>
       <c r="W41" t="s">
         <v>217</v>
@@ -6911,7 +6974,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>-42</v>
       </c>
@@ -6946,8 +7009,11 @@
       <c r="M42" t="s">
         <v>1084</v>
       </c>
+      <c r="N42" t="s">
+        <v>1152</v>
+      </c>
       <c r="P42" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="W42" s="10" t="s">
         <v>218</v>
@@ -6981,7 +7047,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>-43</v>
       </c>
@@ -7016,8 +7082,14 @@
       <c r="M43" t="s">
         <v>1085</v>
       </c>
+      <c r="N43" t="s">
+        <v>1153</v>
+      </c>
+      <c r="O43" t="s">
+        <v>1151</v>
+      </c>
       <c r="P43" t="s">
-        <v>518</v>
+        <v>1097</v>
       </c>
       <c r="W43" t="s">
         <v>219</v>
@@ -7051,7 +7123,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>-44</v>
       </c>
@@ -7086,8 +7158,11 @@
       <c r="M44" t="s">
         <v>1086</v>
       </c>
+      <c r="N44" t="s">
+        <v>1155</v>
+      </c>
       <c r="P44" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="W44" s="10" t="s">
         <v>220</v>
@@ -7121,7 +7196,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>-45</v>
       </c>
@@ -7153,8 +7228,11 @@
       <c r="J45">
         <v>505</v>
       </c>
+      <c r="N45" t="s">
+        <v>1154</v>
+      </c>
       <c r="P45" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="W45" s="10" t="s">
         <v>221</v>
@@ -7188,7 +7266,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>-46</v>
       </c>
@@ -7221,7 +7299,7 @@
         <v>330</v>
       </c>
       <c r="P46" t="s">
-        <v>538</v>
+        <v>1096</v>
       </c>
       <c r="W46" t="s">
         <v>222</v>
@@ -7255,7 +7333,7 @@
         <v>1.0200000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>-47</v>
       </c>
@@ -7288,7 +7366,7 @@
         <v>492</v>
       </c>
       <c r="P47" t="s">
-        <v>561</v>
+        <v>443</v>
       </c>
       <c r="W47" t="s">
         <v>223</v>
@@ -7322,7 +7400,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>-48</v>
       </c>
@@ -7355,7 +7433,7 @@
         <v>315</v>
       </c>
       <c r="P48" t="s">
-        <v>807</v>
+        <v>1131</v>
       </c>
       <c r="W48" s="10" t="s">
         <v>224</v>
@@ -7389,7 +7467,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>-49</v>
       </c>
@@ -7453,7 +7531,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>-50</v>
       </c>
@@ -7485,6 +7563,9 @@
       <c r="J50">
         <v>545</v>
       </c>
+      <c r="P50" t="s">
+        <v>1150</v>
+      </c>
       <c r="W50" s="10" t="s">
         <v>226</v>
       </c>
@@ -7517,7 +7598,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>-51</v>
       </c>
@@ -7581,7 +7662,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>-52</v>
       </c>
@@ -7645,7 +7726,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>-53</v>
       </c>
@@ -7709,7 +7790,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>-54</v>
       </c>
@@ -7797,7 +7878,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>-55</v>
       </c>
@@ -7885,7 +7966,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>-56</v>
       </c>
@@ -7973,7 +8054,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>-57</v>
       </c>
@@ -8064,7 +8145,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>-58</v>
       </c>
@@ -8152,7 +8233,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>-59</v>
       </c>
@@ -8240,7 +8321,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>-60</v>
       </c>
@@ -8331,7 +8412,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>-61</v>
       </c>
@@ -8419,7 +8500,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>-62</v>
       </c>
@@ -8507,7 +8588,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>-63</v>
       </c>
@@ -8595,7 +8676,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>-64</v>
       </c>
@@ -8683,7 +8764,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>-65</v>
       </c>
@@ -8771,7 +8852,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>-66</v>
       </c>
@@ -8859,7 +8940,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>-67</v>
       </c>
@@ -8947,7 +9028,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>-68</v>
       </c>
@@ -9035,7 +9116,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>-69</v>
       </c>
@@ -9123,7 +9204,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>-70</v>
       </c>
@@ -9211,7 +9292,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>-71</v>
       </c>
@@ -9299,7 +9380,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>-72</v>
       </c>
@@ -9387,7 +9468,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>-73</v>
       </c>
@@ -9475,7 +9556,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>-74</v>
       </c>
@@ -9563,7 +9644,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>-75</v>
       </c>
@@ -9658,7 +9739,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>-76</v>
       </c>
@@ -9722,7 +9803,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>-77</v>
       </c>
@@ -9786,7 +9867,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>-78</v>
       </c>
@@ -9850,7 +9931,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>-79</v>
       </c>
@@ -9914,7 +9995,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>-80</v>
       </c>
@@ -9978,7 +10059,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>-81</v>
       </c>
@@ -10042,7 +10123,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>-82</v>
       </c>
@@ -10106,7 +10187,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>-83</v>
       </c>
@@ -10170,7 +10251,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>-84</v>
       </c>
@@ -10234,7 +10315,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>-85</v>
       </c>
@@ -10301,7 +10382,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>-86</v>
       </c>
@@ -10365,7 +10446,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>-87</v>
       </c>
@@ -10429,7 +10510,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>-88</v>
       </c>
@@ -10493,7 +10574,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>-89</v>
       </c>
@@ -10557,7 +10638,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>-90</v>
       </c>
@@ -10621,7 +10702,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>-91</v>
       </c>
@@ -10685,7 +10766,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>-92</v>
       </c>
@@ -10749,7 +10830,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>-93</v>
       </c>
@@ -10813,7 +10894,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>-94</v>
       </c>
@@ -10877,7 +10958,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>-95</v>
       </c>
@@ -10941,7 +11022,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>-96</v>
       </c>
@@ -11005,7 +11086,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>-97</v>
       </c>
@@ -11069,7 +11150,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>-98</v>
       </c>
@@ -11133,7 +11214,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>-99</v>
       </c>
@@ -11197,7 +11278,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>-100</v>
       </c>
@@ -11261,7 +11342,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>-101</v>
       </c>
@@ -11325,7 +11406,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>-102</v>
       </c>
@@ -11389,7 +11470,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>-103</v>
       </c>
@@ -11456,7 +11537,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>-104</v>
       </c>
@@ -11520,7 +11601,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>-105</v>
       </c>
@@ -11584,7 +11665,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>-106</v>
       </c>
@@ -11648,7 +11729,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>-107</v>
       </c>
@@ -11712,7 +11793,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>-108</v>
       </c>
@@ -11776,7 +11857,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>-109</v>
       </c>
@@ -11840,7 +11921,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>-110</v>
       </c>
@@ -11904,7 +11985,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>-111</v>
       </c>
@@ -11968,7 +12049,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>-112</v>
       </c>
@@ -12032,7 +12113,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>-113</v>
       </c>
@@ -12096,7 +12177,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>-114</v>
       </c>
@@ -12160,7 +12241,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>-115</v>
       </c>
@@ -12224,7 +12305,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>-116</v>
       </c>
@@ -12288,7 +12369,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>-117</v>
       </c>
@@ -12352,7 +12433,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>-118</v>
       </c>
@@ -12416,7 +12497,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>-119</v>
       </c>
@@ -12480,7 +12561,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>-120</v>
       </c>
@@ -12544,7 +12625,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>-121</v>
       </c>
@@ -12608,7 +12689,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>-122</v>
       </c>
@@ -12672,7 +12753,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>-123</v>
       </c>
@@ -12736,7 +12817,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>-124</v>
       </c>
@@ -12800,7 +12881,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>-125</v>
       </c>
@@ -12864,7 +12945,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>-126</v>
       </c>
@@ -12928,7 +13009,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>-127</v>
       </c>
@@ -12992,7 +13073,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>-128</v>
       </c>
@@ -13056,7 +13137,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>-129</v>
       </c>
@@ -13120,7 +13201,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>-130</v>
       </c>
@@ -13184,7 +13265,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>-131</v>
       </c>
@@ -13248,7 +13329,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>-132</v>
       </c>
@@ -13312,7 +13393,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>-133</v>
       </c>
@@ -13376,7 +13457,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>-134</v>
       </c>
@@ -13440,7 +13521,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>-135</v>
       </c>
@@ -13504,7 +13585,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>-136</v>
       </c>
@@ -13568,7 +13649,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>-137</v>
       </c>
@@ -13632,7 +13713,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>-138</v>
       </c>
@@ -13699,7 +13780,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>-139</v>
       </c>
@@ -13763,7 +13844,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>-140</v>
       </c>
@@ -13827,7 +13908,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>-141</v>
       </c>
@@ -13898,7 +13979,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>-142</v>
       </c>
@@ -13972,7 +14053,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>-143</v>
       </c>
@@ -14043,7 +14124,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>-144</v>
       </c>
@@ -14123,7 +14204,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:34" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
         <v>585</v>
       </c>
@@ -14193,7 +14274,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>1</v>
       </c>
@@ -14288,7 +14369,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2</v>
       </c>
@@ -14383,7 +14464,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>3</v>
       </c>
@@ -14475,7 +14556,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>4</v>
       </c>
@@ -14568,7 +14649,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>5</v>
       </c>
@@ -14661,7 +14742,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>6</v>
       </c>
@@ -14751,7 +14832,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>7</v>
       </c>
@@ -14849,7 +14930,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>8</v>
       </c>
@@ -14944,7 +15025,7 @@
         <v>3.8E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>9</v>
       </c>
@@ -15036,7 +15117,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>10</v>
       </c>
@@ -15131,7 +15212,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>11</v>
       </c>
@@ -15226,7 +15307,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>12</v>
       </c>
@@ -15318,7 +15399,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>13</v>
       </c>
@@ -15411,7 +15492,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>14</v>
       </c>
@@ -15504,7 +15585,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>15</v>
       </c>
@@ -15596,7 +15677,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>16</v>
       </c>
@@ -15691,7 +15772,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>17</v>
       </c>
@@ -15786,7 +15867,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>18</v>
       </c>
@@ -15881,7 +15962,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>19</v>
       </c>
@@ -15974,7 +16055,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>20</v>
       </c>
@@ -16067,7 +16148,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>21</v>
       </c>
@@ -16157,7 +16238,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>22</v>
       </c>
@@ -16250,7 +16331,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>23</v>
       </c>
@@ -16343,7 +16424,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>24</v>
       </c>
@@ -16376,7 +16457,7 @@
         <v>505</v>
       </c>
       <c r="K169" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="L169" t="s">
         <v>654</v>
@@ -16433,7 +16514,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>25</v>
       </c>
@@ -16526,7 +16607,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>26</v>
       </c>
@@ -16619,7 +16700,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>27</v>
       </c>
@@ -16709,7 +16790,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>28</v>
       </c>
@@ -16796,7 +16877,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>29</v>
       </c>
@@ -16888,7 +16969,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>30</v>
       </c>
@@ -16980,7 +17061,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>31</v>
       </c>
@@ -17069,7 +17150,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>32</v>
       </c>
@@ -17159,7 +17240,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>33</v>
       </c>
@@ -17249,7 +17330,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>34</v>
       </c>
@@ -17336,7 +17417,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>35</v>
       </c>
@@ -17426,7 +17507,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="181" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>36</v>
       </c>
@@ -17516,7 +17597,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>37</v>
       </c>
@@ -17603,7 +17684,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>38</v>
       </c>
@@ -17692,7 +17773,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="184" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>39</v>
       </c>
@@ -17787,7 +17868,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>40</v>
       </c>
@@ -17879,7 +17960,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>41</v>
       </c>
@@ -17969,7 +18050,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>42</v>
       </c>
@@ -18059,7 +18140,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>43</v>
       </c>
@@ -18146,7 +18227,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>44</v>
       </c>
@@ -18236,7 +18317,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>45</v>
       </c>
@@ -18326,7 +18407,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>46</v>
       </c>
@@ -18407,7 +18488,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>47</v>
       </c>
@@ -18488,7 +18569,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>48</v>
       </c>
@@ -18574,7 +18655,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>49</v>
       </c>
@@ -18666,7 +18747,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="195" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>50</v>
       </c>
@@ -18755,7 +18836,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>51</v>
       </c>
@@ -18847,7 +18928,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>52</v>
       </c>
@@ -18937,7 +19018,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>53</v>
       </c>
@@ -19027,7 +19108,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>54</v>
       </c>
@@ -19114,7 +19195,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>55</v>
       </c>
@@ -19206,7 +19287,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="201" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>56</v>
       </c>
@@ -19295,7 +19376,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="202" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>57</v>
       </c>
@@ -19384,7 +19465,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>58</v>
       </c>
@@ -19470,7 +19551,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>59</v>
       </c>
@@ -19559,7 +19640,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>60</v>
       </c>
@@ -19645,7 +19726,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="206" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>61</v>
       </c>
@@ -19731,7 +19812,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>62</v>
       </c>
@@ -19820,7 +19901,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="208" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>63</v>
       </c>
@@ -19903,7 +19984,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="209" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>64</v>
       </c>
@@ -19987,7 +20068,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="210" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>65</v>
       </c>
@@ -20068,7 +20149,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="211" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>66</v>
       </c>
@@ -20154,7 +20235,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>67</v>
       </c>
@@ -20237,7 +20318,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="213" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>68</v>
       </c>
@@ -20323,7 +20404,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="214" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>69</v>
       </c>
@@ -20409,7 +20490,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="215" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>70</v>
       </c>
@@ -20492,7 +20573,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="216" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>71</v>
       </c>
@@ -20578,7 +20659,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="217" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>72</v>
       </c>
@@ -20661,7 +20742,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="218" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>73</v>
       </c>
@@ -20700,7 +20781,7 @@
         <v>682</v>
       </c>
       <c r="M218" s="20" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="N218" s="17" t="s">
         <v>756</v>
@@ -20750,7 +20831,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="219" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>74</v>
       </c>
@@ -20789,7 +20870,7 @@
         <v>682</v>
       </c>
       <c r="M219" s="20" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="N219" s="10" t="s">
         <v>696</v>
@@ -20836,7 +20917,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="220" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>75</v>
       </c>
@@ -20922,7 +21003,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="221" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>76</v>
       </c>
@@ -21008,7 +21089,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="222" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>77</v>
       </c>
@@ -21091,7 +21172,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="223" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>78</v>
       </c>
@@ -21180,7 +21261,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="224" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>79</v>
       </c>
@@ -21263,7 +21344,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="225" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>80</v>
       </c>
@@ -21347,7 +21428,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>81</v>
       </c>
@@ -21428,7 +21509,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="227" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>82</v>
       </c>
@@ -21511,7 +21592,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>83</v>
       </c>
@@ -21597,7 +21678,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="229" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>84</v>
       </c>
@@ -21695,7 +21776,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>85</v>
       </c>
@@ -21788,7 +21869,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="231" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>86</v>
       </c>
@@ -21881,7 +21962,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>87</v>
       </c>
@@ -21973,7 +22054,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="233" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>88</v>
       </c>
@@ -22068,7 +22149,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>89</v>
       </c>
@@ -22160,7 +22241,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="235" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>90</v>
       </c>
@@ -22255,7 +22336,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>91</v>
       </c>
@@ -22347,7 +22428,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>92</v>
       </c>
@@ -22442,7 +22523,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>93</v>
       </c>
@@ -22534,7 +22615,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="239" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>94</v>
       </c>
@@ -22627,7 +22708,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="240" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>95</v>
       </c>
@@ -22720,7 +22801,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="241" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>96</v>
       </c>
@@ -22810,7 +22891,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="242" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>97</v>
       </c>
@@ -22899,7 +22980,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>98</v>
       </c>
@@ -22990,7 +23071,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="244" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>99</v>
       </c>
@@ -23080,7 +23161,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="245" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>100</v>
       </c>
@@ -23167,7 +23248,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="246" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>101</v>
       </c>
@@ -23259,7 +23340,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="247" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>102</v>
       </c>
@@ -23351,7 +23432,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="248" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>103</v>
       </c>
@@ -23440,7 +23521,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>104</v>
       </c>
@@ -23535,7 +23616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>105</v>
       </c>
@@ -23627,7 +23708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>106</v>
       </c>
@@ -23719,7 +23800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>107</v>
       </c>
@@ -23808,7 +23889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>108</v>
       </c>
@@ -23889,7 +23970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>109</v>
       </c>
@@ -23976,7 +24057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>110</v>
       </c>
@@ -24066,7 +24147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>111</v>
       </c>
@@ -24158,7 +24239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>112</v>
       </c>
@@ -24250,7 +24331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>113</v>
       </c>
@@ -24339,7 +24420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>114</v>
       </c>
@@ -24429,7 +24510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>115</v>
       </c>
@@ -24519,7 +24600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>116</v>
       </c>
@@ -24606,7 +24687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>117</v>
       </c>
@@ -24696,7 +24777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>118</v>
       </c>
@@ -24786,7 +24867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>119</v>
       </c>
@@ -24876,7 +24957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>120</v>
       </c>
@@ -24969,7 +25050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>121</v>
       </c>
@@ -25062,7 +25143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>122</v>
       </c>
@@ -25152,7 +25233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>123</v>
       </c>
@@ -25242,7 +25323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>124</v>
       </c>
@@ -25332,7 +25413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>125</v>
       </c>
@@ -25394,7 +25475,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="271" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>126</v>
       </c>
@@ -25459,7 +25540,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="272" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>127</v>
       </c>
@@ -25512,7 +25593,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>128</v>
       </c>
@@ -25562,7 +25643,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>129</v>
       </c>
@@ -25615,7 +25696,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>130</v>
       </c>
@@ -25665,7 +25746,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>131</v>
       </c>
@@ -25724,7 +25805,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>132</v>
       </c>
@@ -25786,7 +25867,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>133</v>
       </c>
@@ -25845,7 +25926,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>134</v>
       </c>
@@ -25907,7 +25988,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>135</v>
       </c>
@@ -25966,7 +26047,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>136</v>
       </c>
@@ -26025,7 +26106,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>137</v>
       </c>
@@ -26087,7 +26168,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>138</v>
       </c>
@@ -26146,7 +26227,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>139</v>
       </c>
@@ -26205,7 +26286,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>140</v>
       </c>
@@ -26261,7 +26342,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>141</v>
       </c>
@@ -26320,7 +26401,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>142</v>
       </c>
@@ -26376,7 +26457,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>143</v>
       </c>
@@ -26435,7 +26516,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="289" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>144</v>
       </c>
@@ -26494,7 +26575,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="290" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>145</v>
       </c>
@@ -26550,7 +26631,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="291" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>146</v>
       </c>
@@ -26609,7 +26690,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="292" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>147</v>
       </c>
@@ -26665,7 +26746,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="293" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>148</v>
       </c>
@@ -26724,7 +26805,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="294" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>149</v>
       </c>
@@ -26780,7 +26861,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="295" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>150</v>
       </c>
@@ -26836,7 +26917,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="296" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>151</v>
       </c>
@@ -26900,7 +26981,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="297" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>152</v>
       </c>
@@ -26961,7 +27042,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="298" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>153</v>
       </c>
@@ -27025,7 +27106,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="299" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>154</v>
       </c>
@@ -27089,7 +27170,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="300" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>155</v>
       </c>
@@ -27150,7 +27231,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="301" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>156</v>
       </c>
@@ -27214,7 +27295,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="302" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>157</v>
       </c>
@@ -27275,7 +27356,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="303" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>158</v>
       </c>
@@ -27337,7 +27418,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="304" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>159</v>
       </c>
@@ -27396,7 +27477,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="305" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>160</v>
       </c>
@@ -27455,7 +27536,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="306" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>161</v>
       </c>
@@ -27514,7 +27595,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="307" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>162</v>
       </c>
@@ -27573,7 +27654,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="308" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>163</v>
       </c>
@@ -27632,7 +27713,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="309" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>164</v>
       </c>
@@ -27691,7 +27772,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="310" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>165</v>
       </c>
@@ -27747,7 +27828,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="311" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>166</v>
       </c>
@@ -27808,7 +27889,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="312" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>167</v>
       </c>
@@ -27869,7 +27950,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="313" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>168</v>
       </c>
@@ -27927,7 +28008,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="314" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>169</v>
       </c>
@@ -27986,7 +28067,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="315" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>170</v>
       </c>
@@ -28042,7 +28123,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="316" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>171</v>
       </c>
@@ -28101,7 +28182,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="317" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>172</v>
       </c>
@@ -28160,7 +28241,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="318" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>173</v>
       </c>
@@ -28216,7 +28297,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="319" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>174</v>
       </c>
@@ -28275,7 +28356,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="320" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>175</v>
       </c>
@@ -28334,7 +28415,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="321" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>176</v>
       </c>
@@ -28390,7 +28471,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="322" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>177</v>
       </c>
@@ -28449,7 +28530,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="323" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>178</v>
       </c>
@@ -28505,7 +28586,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="324" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>179</v>
       </c>
@@ -28564,7 +28645,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="325" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>180</v>
       </c>
@@ -28620,7 +28701,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="326" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>181</v>
       </c>
@@ -28676,7 +28757,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="327" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>182</v>
       </c>
@@ -28735,7 +28816,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="328" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>183</v>
       </c>
@@ -28794,7 +28875,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="329" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>184</v>
       </c>
@@ -28850,7 +28931,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="330" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>185</v>
       </c>
@@ -28906,7 +28987,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="331" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>186</v>
       </c>
@@ -28962,7 +29043,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="332" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>187</v>
       </c>
@@ -29021,7 +29102,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="333" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>188</v>
       </c>
@@ -29080,7 +29161,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="334" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>189</v>
       </c>
@@ -29133,7 +29214,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="335" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>190</v>
       </c>
@@ -29183,7 +29264,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="336" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>191</v>
       </c>
@@ -29233,7 +29314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>192</v>
       </c>
@@ -29280,7 +29361,7 @@
         <v>Galactasolder</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>193</v>
       </c>
@@ -29332,7 +29413,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>194</v>
       </c>
@@ -29381,7 +29462,7 @@
         <v>Cosmocrash</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>195</v>
       </c>
@@ -29431,7 +29512,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>196</v>
       </c>
@@ -29478,7 +29559,7 @@
         <v>Stellarock</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>197</v>
       </c>
@@ -29530,7 +29611,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>198</v>
       </c>
@@ -29579,7 +29660,7 @@
         <v>Hast-E</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>199</v>
       </c>
@@ -29629,7 +29710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>200</v>
       </c>
@@ -29679,7 +29760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>201</v>
       </c>
@@ -29726,7 +29807,7 @@
         <v>Soldrota-E</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>202</v>
       </c>
@@ -29776,7 +29857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>203</v>
       </c>
@@ -29826,7 +29907,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>204</v>
       </c>
@@ -29873,7 +29954,7 @@
         <v>Blastflames-E</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>205</v>
       </c>
@@ -29923,7 +30004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>206</v>
       </c>
@@ -29973,7 +30054,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>207</v>
       </c>
@@ -30020,7 +30101,7 @@
         <v>Blaster-E</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>208</v>
       </c>
@@ -30070,7 +30151,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>209</v>
       </c>
@@ -30120,7 +30201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>210</v>
       </c>
@@ -30170,7 +30251,7 @@
         <v>Gyarados-E</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>211</v>
       </c>
@@ -30217,7 +30298,7 @@
         <v>Shockfang</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>212</v>
       </c>
@@ -30267,7 +30348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>213</v>
       </c>
@@ -30314,7 +30395,7 @@
         <v>Nightrex</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>214</v>
       </c>
@@ -30364,7 +30445,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>215</v>
       </c>
@@ -30411,7 +30492,7 @@
         <v>Durfish-S</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>216</v>
       </c>
@@ -30461,7 +30542,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>217</v>
       </c>
@@ -30507,7 +30588,7 @@
         <v>Wormite-S</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>218</v>
       </c>
@@ -30556,7 +30637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>219</v>
       </c>
@@ -30605,7 +30686,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>220</v>
       </c>
@@ -30651,7 +30732,7 @@
         <v>Cluuz-S</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>221</v>
       </c>
@@ -30700,7 +30781,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>222</v>
       </c>
@@ -30749,7 +30830,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>223</v>
       </c>
@@ -30801,7 +30882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>224</v>
       </c>
@@ -30853,7 +30934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>225</v>
       </c>
@@ -30902,7 +30983,7 @@
         <v>Pyrator-S</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>226</v>
       </c>
@@ -30952,7 +31033,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>227</v>
       </c>
@@ -30999,7 +31080,7 @@
         <v>Arbok-S</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>228</v>
       </c>
@@ -31046,7 +31127,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>229</v>
       </c>
@@ -31093,7 +31174,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>230</v>
       </c>
@@ -31140,7 +31221,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>231</v>
       </c>
@@ -31187,7 +31268,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>232</v>
       </c>
@@ -31234,7 +31315,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>233</v>
       </c>
@@ -31281,7 +31362,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>234</v>
       </c>
@@ -31328,7 +31409,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>235</v>
       </c>
@@ -31375,7 +31456,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>236</v>
       </c>
@@ -31422,7 +31503,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>237</v>
       </c>
@@ -31465,7 +31546,7 @@
         <v>Kissyfishy-D</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>238</v>
       </c>
@@ -31507,7 +31588,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>239</v>
       </c>
@@ -31549,7 +31630,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>240</v>
       </c>
@@ -31591,15 +31672,15 @@
         <v>623</v>
       </c>
     </row>
-    <row r="622" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="622" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B622">
         <f>MAX(B385:B620)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L1:N20">
-    <sortCondition descending="1" ref="L1:L20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P34:P48">
+    <sortCondition ref="P48"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="M1:M21">

</xml_diff>

<commit_message>
Implementation changes getting ready for hidden abilities
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF13515A-A193-474C-85F8-AA815FE7937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2EEEDB-F0DB-49AC-BA99-05A2AB30E72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="1161">
   <si>
     <t>Leafer</t>
   </si>
@@ -3504,6 +3504,21 @@
   </si>
   <si>
     <t>Zurroaratr-S: Nasty Plot/Venom Drench/Dark Pulse/Giga Drain/Silver Wind/Star Storm</t>
+  </si>
+  <si>
+    <t>Defiant/Swift Swim</t>
+  </si>
+  <si>
+    <t>Corrosion</t>
+  </si>
+  <si>
+    <t>Prankster?</t>
+  </si>
+  <si>
+    <t>Mold Breaker</t>
+  </si>
+  <si>
+    <t>Full Force(Unburden for Attack)</t>
   </si>
 </sst>
 </file>
@@ -4249,8 +4264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AT622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M329" sqref="M329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14594,7 +14609,9 @@
       <c r="L149" t="s">
         <v>871</v>
       </c>
-      <c r="M149" s="20"/>
+      <c r="M149" s="20" t="s">
+        <v>647</v>
+      </c>
       <c r="N149" s="17" t="s">
         <v>732</v>
       </c>
@@ -14687,7 +14704,9 @@
       <c r="L150" t="s">
         <v>871</v>
       </c>
-      <c r="M150" s="20"/>
+      <c r="M150" s="20" t="s">
+        <v>647</v>
+      </c>
       <c r="N150" s="17" t="s">
         <v>733</v>
       </c>
@@ -14780,7 +14799,9 @@
       <c r="L151" t="s">
         <v>871</v>
       </c>
-      <c r="M151" s="20"/>
+      <c r="M151" s="20" t="s">
+        <v>647</v>
+      </c>
       <c r="N151" s="17" t="s">
         <v>741</v>
       </c>
@@ -14871,7 +14892,7 @@
         <v>677</v>
       </c>
       <c r="M152" s="20" t="s">
-        <v>166</v>
+        <v>1156</v>
       </c>
       <c r="N152" s="17" t="s">
         <v>747</v>
@@ -14969,7 +14990,7 @@
         <v>677</v>
       </c>
       <c r="M153" s="20" t="s">
-        <v>166</v>
+        <v>1156</v>
       </c>
       <c r="N153" s="17" t="s">
         <v>734</v>
@@ -15064,7 +15085,7 @@
         <v>677</v>
       </c>
       <c r="M154" s="20" t="s">
-        <v>166</v>
+        <v>1156</v>
       </c>
       <c r="N154" s="17" t="s">
         <v>735</v>
@@ -15437,7 +15458,9 @@
       <c r="L158" t="s">
         <v>597</v>
       </c>
-      <c r="M158" s="20"/>
+      <c r="M158" s="20" t="s">
+        <v>658</v>
+      </c>
       <c r="N158" s="10" t="s">
         <v>687</v>
       </c>
@@ -15530,7 +15553,9 @@
       <c r="L159" t="s">
         <v>597</v>
       </c>
-      <c r="M159" s="20"/>
+      <c r="M159" s="20" t="s">
+        <v>658</v>
+      </c>
       <c r="N159" s="17" t="s">
         <v>737</v>
       </c>
@@ -16916,7 +16941,7 @@
         <v>605</v>
       </c>
       <c r="M174" s="20" t="s">
-        <v>1112</v>
+        <v>1157</v>
       </c>
       <c r="N174" s="17" t="s">
         <v>765</v>
@@ -17008,7 +17033,7 @@
         <v>605</v>
       </c>
       <c r="M175" s="20" t="s">
-        <v>1112</v>
+        <v>1157</v>
       </c>
       <c r="N175" s="17" t="s">
         <v>708</v>
@@ -17100,7 +17125,7 @@
         <v>605</v>
       </c>
       <c r="M176" s="20" t="s">
-        <v>1112</v>
+        <v>1157</v>
       </c>
       <c r="N176" s="17" t="s">
         <v>748</v>
@@ -26265,7 +26290,9 @@
       <c r="L284" t="s">
         <v>605</v>
       </c>
-      <c r="M284" s="20"/>
+      <c r="M284" s="20" t="s">
+        <v>660</v>
+      </c>
       <c r="O284">
         <v>139</v>
       </c>
@@ -26324,7 +26351,9 @@
       <c r="L285" t="s">
         <v>605</v>
       </c>
-      <c r="M285" s="20"/>
+      <c r="M285" s="20" t="s">
+        <v>660</v>
+      </c>
       <c r="O285">
         <v>140</v>
       </c>
@@ -27081,7 +27110,7 @@
         <v>663</v>
       </c>
       <c r="M298" s="20" t="s">
-        <v>1112</v>
+        <v>1158</v>
       </c>
       <c r="O298">
         <v>153</v>
@@ -27145,7 +27174,7 @@
         <v>663</v>
       </c>
       <c r="M299" s="20" t="s">
-        <v>1112</v>
+        <v>1158</v>
       </c>
       <c r="O299">
         <v>154</v>
@@ -27209,7 +27238,7 @@
         <v>663</v>
       </c>
       <c r="M300" s="20" t="s">
-        <v>1112</v>
+        <v>1158</v>
       </c>
       <c r="O300">
         <v>155</v>
@@ -27270,7 +27299,7 @@
         <v>610</v>
       </c>
       <c r="M301" s="20" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="O301">
         <v>156</v>
@@ -27394,7 +27423,9 @@
       <c r="L303" t="s">
         <v>604</v>
       </c>
-      <c r="M303" s="20"/>
+      <c r="M303" s="20" t="s">
+        <v>1127</v>
+      </c>
       <c r="O303">
         <v>158</v>
       </c>
@@ -27456,7 +27487,9 @@
       <c r="L304" t="s">
         <v>604</v>
       </c>
-      <c r="M304" s="20"/>
+      <c r="M304" s="20" t="s">
+        <v>1127</v>
+      </c>
       <c r="O304">
         <v>159</v>
       </c>
@@ -28046,7 +28079,9 @@
       <c r="L314" t="s">
         <v>653</v>
       </c>
-      <c r="M314" s="20"/>
+      <c r="M314" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O314">
         <v>169</v>
       </c>
@@ -28105,7 +28140,9 @@
       <c r="L315" t="s">
         <v>653</v>
       </c>
-      <c r="M315" s="20"/>
+      <c r="M315" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O315">
         <v>170</v>
       </c>
@@ -28161,7 +28198,9 @@
       <c r="L316" t="s">
         <v>648</v>
       </c>
-      <c r="M316" s="20"/>
+      <c r="M316" s="20" t="s">
+        <v>1107</v>
+      </c>
       <c r="O316">
         <v>171</v>
       </c>
@@ -28220,7 +28259,9 @@
       <c r="L317" t="s">
         <v>648</v>
       </c>
-      <c r="M317" s="20"/>
+      <c r="M317" s="20" t="s">
+        <v>1107</v>
+      </c>
       <c r="O317">
         <v>172</v>
       </c>
@@ -28279,7 +28320,9 @@
       <c r="L318" t="s">
         <v>601</v>
       </c>
-      <c r="M318" s="20"/>
+      <c r="M318" s="20" t="s">
+        <v>1107</v>
+      </c>
       <c r="O318">
         <v>173</v>
       </c>
@@ -28739,7 +28782,9 @@
       <c r="L326" t="s">
         <v>663</v>
       </c>
-      <c r="M326" s="20"/>
+      <c r="M326" s="20" t="s">
+        <v>1160</v>
+      </c>
       <c r="O326">
         <v>181</v>
       </c>
@@ -28795,7 +28840,9 @@
       <c r="L327" t="s">
         <v>663</v>
       </c>
-      <c r="M327" s="20"/>
+      <c r="M327" s="20" t="s">
+        <v>1160</v>
+      </c>
       <c r="O327">
         <v>182</v>
       </c>
@@ -28854,7 +28901,9 @@
       <c r="L328" t="s">
         <v>663</v>
       </c>
-      <c r="M328" s="20"/>
+      <c r="M328" s="20" t="s">
+        <v>1160</v>
+      </c>
       <c r="O328">
         <v>183</v>
       </c>
@@ -29252,7 +29301,9 @@
       <c r="L335" t="s">
         <v>610</v>
       </c>
-      <c r="M335" s="20"/>
+      <c r="M335" s="20" t="s">
+        <v>1107</v>
+      </c>
       <c r="O335">
         <v>190</v>
       </c>
@@ -29302,7 +29353,9 @@
       <c r="L336" t="s">
         <v>683</v>
       </c>
-      <c r="M336" s="20"/>
+      <c r="M336" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O336">
         <v>191</v>
       </c>
@@ -29352,7 +29405,9 @@
       <c r="L337" t="s">
         <v>683</v>
       </c>
-      <c r="M337" s="20"/>
+      <c r="M337" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O337">
         <v>192</v>
       </c>
@@ -29500,7 +29555,9 @@
       <c r="L340" t="s">
         <v>650</v>
       </c>
-      <c r="M340" s="20"/>
+      <c r="M340" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O340">
         <v>195</v>
       </c>
@@ -29550,7 +29607,9 @@
       <c r="L341" t="s">
         <v>650</v>
       </c>
-      <c r="M341" s="20"/>
+      <c r="M341" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O341">
         <v>196</v>
       </c>
@@ -29698,7 +29757,9 @@
       <c r="L344" t="s">
         <v>671</v>
       </c>
-      <c r="M344" s="20"/>
+      <c r="M344" s="20" t="s">
+        <v>1160</v>
+      </c>
       <c r="O344">
         <v>199</v>
       </c>
@@ -29748,7 +29809,9 @@
       <c r="L345" t="s">
         <v>671</v>
       </c>
-      <c r="M345" s="20"/>
+      <c r="M345" s="20" t="s">
+        <v>1160</v>
+      </c>
       <c r="O345">
         <v>200</v>
       </c>
@@ -29798,7 +29861,9 @@
       <c r="L346" t="s">
         <v>671</v>
       </c>
-      <c r="M346" s="20"/>
+      <c r="M346" s="20" t="s">
+        <v>1160</v>
+      </c>
       <c r="O346">
         <v>201</v>
       </c>
@@ -31021,7 +31086,9 @@
       <c r="L371" t="s">
         <v>674</v>
       </c>
-      <c r="M371" s="20"/>
+      <c r="M371" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O371">
         <v>226</v>
       </c>
@@ -31071,7 +31138,9 @@
       <c r="L372" t="s">
         <v>674</v>
       </c>
-      <c r="M372" s="20"/>
+      <c r="M372" s="20" t="s">
+        <v>1159</v>
+      </c>
       <c r="O372">
         <v>227</v>
       </c>

</xml_diff>

<commit_message>
Finished TN Splinkty base implementation, and added hidden abilities
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56023BE4-28A6-41CC-B784-7CF892FE31BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBC995E-455C-4E37-8FF2-EADB7CAF7DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2470" uniqueCount="1186">
   <si>
     <t>Leafer</t>
   </si>
@@ -3528,6 +3528,72 @@
   </si>
   <si>
     <t>Scrappy</t>
+  </si>
+  <si>
+    <t>Unburden</t>
+  </si>
+  <si>
+    <t>Abra</t>
+  </si>
+  <si>
+    <t>Kadabra</t>
+  </si>
+  <si>
+    <t>Alakazam</t>
+  </si>
+  <si>
+    <t>Flamigo</t>
+  </si>
+  <si>
+    <t>Sneasel</t>
+  </si>
+  <si>
+    <t>Sneasler</t>
+  </si>
+  <si>
+    <t>Weavile</t>
+  </si>
+  <si>
+    <t>Sneasel-H</t>
+  </si>
+  <si>
+    <t>Solosis</t>
+  </si>
+  <si>
+    <t>Duosion</t>
+  </si>
+  <si>
+    <t>Reuniclus</t>
+  </si>
+  <si>
+    <t>Solosis-X</t>
+  </si>
+  <si>
+    <t>Duosion-X</t>
+  </si>
+  <si>
+    <t>Reuniclus-X</t>
+  </si>
+  <si>
+    <t>Seviper</t>
+  </si>
+  <si>
+    <t>Hissimitar</t>
+  </si>
+  <si>
+    <t>Gulpin</t>
+  </si>
+  <si>
+    <t>Swalot</t>
+  </si>
+  <si>
+    <t>Gulpin-X</t>
+  </si>
+  <si>
+    <t>Swalot-X</t>
+  </si>
+  <si>
+    <t>Plasamp</t>
   </si>
 </sst>
 </file>
@@ -3537,7 +3603,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3616,8 +3682,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3752,6 +3825,36 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3775,7 +3878,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -3820,6 +3923,15 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -3900,8 +4012,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}" name="Table3" displayName="Table3" ref="B145:J385" totalsRowShown="0" tableBorderDxfId="4">
-  <autoFilter ref="B145:J385" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}" name="Table3" displayName="Table3" ref="B145:J409" totalsRowShown="0" tableBorderDxfId="4">
+  <autoFilter ref="B145:J409" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{954E08A8-D138-4D6D-97C7-F47E4324725D}" name="Name"/>
     <tableColumn id="2" xr3:uid="{F9097124-9DD8-47D1-881E-F9976C72C702}" name="Total" dataCellStyle="60% - Accent4">
@@ -4271,10 +4383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
-  <dimension ref="A1:AT622"/>
+  <dimension ref="A1:AT621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="N196" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W212" sqref="W212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18663,7 +18775,7 @@
       <c r="Q193">
         <v>22</v>
       </c>
-      <c r="W193" s="10" t="s">
+      <c r="W193" s="46" t="s">
         <v>362</v>
       </c>
       <c r="Y193">
@@ -20326,7 +20438,7 @@
         <f t="shared" si="14"/>
         <v>Tricercil</v>
       </c>
-      <c r="W212" s="10" t="s">
+      <c r="W212" s="46" t="s">
         <v>204</v>
       </c>
       <c r="Y212">
@@ -21422,7 +21534,9 @@
       <c r="L225" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="M225" s="20"/>
+      <c r="M225" s="20" t="s">
+        <v>1164</v>
+      </c>
       <c r="N225" s="10" t="s">
         <v>700</v>
       </c>
@@ -21506,7 +21620,9 @@
       <c r="L226" s="10" t="s">
         <v>621</v>
       </c>
-      <c r="M226" s="20"/>
+      <c r="M226" s="20" t="s">
+        <v>1164</v>
+      </c>
       <c r="N226" s="10" t="s">
         <v>701</v>
       </c>
@@ -22693,7 +22809,9 @@
       <c r="L239" t="s">
         <v>642</v>
       </c>
-      <c r="M239" s="20"/>
+      <c r="M239" s="20" t="s">
+        <v>1164</v>
+      </c>
       <c r="N239" s="32" t="s">
         <v>769</v>
       </c>
@@ -22786,7 +22904,9 @@
       <c r="L240" t="s">
         <v>671</v>
       </c>
-      <c r="M240" s="20"/>
+      <c r="M240" s="20" t="s">
+        <v>1164</v>
+      </c>
       <c r="N240" s="10" t="s">
         <v>695</v>
       </c>
@@ -22879,7 +22999,9 @@
       <c r="L241" t="s">
         <v>671</v>
       </c>
-      <c r="M241" s="21"/>
+      <c r="M241" s="40" t="s">
+        <v>1164</v>
+      </c>
       <c r="N241" s="32" t="s">
         <v>727</v>
       </c>
@@ -31780,9 +31902,651 @@
         <v>623</v>
       </c>
     </row>
-    <row r="622" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B622">
-        <f>MAX(B385:B620)</f>
+    <row r="386" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>241</v>
+      </c>
+      <c r="B386" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C386" s="1">
+        <f>SUM(D386:I386)</f>
+        <v>350</v>
+      </c>
+      <c r="D386" s="2">
+        <v>48</v>
+      </c>
+      <c r="E386" s="3">
+        <v>35</v>
+      </c>
+      <c r="F386" s="4">
+        <v>42</v>
+      </c>
+      <c r="G386" s="5">
+        <v>105</v>
+      </c>
+      <c r="H386" s="4">
+        <v>60</v>
+      </c>
+      <c r="I386" s="6">
+        <v>60</v>
+      </c>
+      <c r="J386">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="387" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>242</v>
+      </c>
+      <c r="B387" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C387" s="1">
+        <f>SUM(D387:I387)</f>
+        <v>525</v>
+      </c>
+      <c r="D387" s="2">
+        <v>83</v>
+      </c>
+      <c r="E387" s="3">
+        <v>55</v>
+      </c>
+      <c r="F387" s="4">
+        <v>90</v>
+      </c>
+      <c r="G387" s="5">
+        <v>130</v>
+      </c>
+      <c r="H387" s="4">
+        <v>81</v>
+      </c>
+      <c r="I387" s="6">
+        <v>86</v>
+      </c>
+      <c r="J387">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="388" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>243</v>
+      </c>
+      <c r="B388" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C388" s="1">
+        <f>SUM(D388:I388)</f>
+        <v>310</v>
+      </c>
+      <c r="D388" s="2">
+        <v>25</v>
+      </c>
+      <c r="E388" s="3">
+        <v>20</v>
+      </c>
+      <c r="F388" s="4">
+        <v>15</v>
+      </c>
+      <c r="G388" s="5">
+        <v>105</v>
+      </c>
+      <c r="H388" s="4">
+        <v>55</v>
+      </c>
+      <c r="I388" s="6">
+        <v>90</v>
+      </c>
+      <c r="J388">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="389" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>244</v>
+      </c>
+      <c r="B389" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C389" s="1">
+        <f>SUM(D389:I389)</f>
+        <v>400</v>
+      </c>
+      <c r="D389" s="2">
+        <v>40</v>
+      </c>
+      <c r="E389" s="3">
+        <v>35</v>
+      </c>
+      <c r="F389" s="4">
+        <v>30</v>
+      </c>
+      <c r="G389" s="5">
+        <v>120</v>
+      </c>
+      <c r="H389" s="4">
+        <v>70</v>
+      </c>
+      <c r="I389" s="6">
+        <v>105</v>
+      </c>
+      <c r="J389">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="390" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>245</v>
+      </c>
+      <c r="B390" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C390" s="1">
+        <f>SUM(D390:I390)</f>
+        <v>500</v>
+      </c>
+      <c r="D390" s="2">
+        <v>55</v>
+      </c>
+      <c r="E390" s="3">
+        <v>50</v>
+      </c>
+      <c r="F390" s="4">
+        <v>45</v>
+      </c>
+      <c r="G390" s="5">
+        <v>135</v>
+      </c>
+      <c r="H390" s="4">
+        <v>95</v>
+      </c>
+      <c r="I390" s="6">
+        <v>120</v>
+      </c>
+      <c r="J390">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="391" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>246</v>
+      </c>
+      <c r="B391" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C391" s="1">
+        <f>SUM(D391:I391)</f>
+        <v>500</v>
+      </c>
+      <c r="D391" s="2">
+        <v>82</v>
+      </c>
+      <c r="E391" s="3">
+        <v>115</v>
+      </c>
+      <c r="F391" s="4">
+        <v>74</v>
+      </c>
+      <c r="G391" s="5">
+        <v>75</v>
+      </c>
+      <c r="H391" s="4">
+        <v>64</v>
+      </c>
+      <c r="I391" s="6">
+        <v>90</v>
+      </c>
+      <c r="J391">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="392" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>247</v>
+      </c>
+      <c r="B392" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C392" s="1">
+        <f>SUM(D392:I392)</f>
+        <v>430</v>
+      </c>
+      <c r="D392" s="2">
+        <v>55</v>
+      </c>
+      <c r="E392" s="3">
+        <v>95</v>
+      </c>
+      <c r="F392" s="4">
+        <v>55</v>
+      </c>
+      <c r="G392" s="5">
+        <v>35</v>
+      </c>
+      <c r="H392" s="4">
+        <v>75</v>
+      </c>
+      <c r="I392" s="6">
+        <v>115</v>
+      </c>
+      <c r="J392">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="393" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>248</v>
+      </c>
+      <c r="B393" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C393" s="1">
+        <f t="shared" ref="C393:C396" si="20">SUM(D393:I393)</f>
+        <v>510</v>
+      </c>
+      <c r="D393" s="2">
+        <v>70</v>
+      </c>
+      <c r="E393" s="3">
+        <v>120</v>
+      </c>
+      <c r="F393" s="4">
+        <v>65</v>
+      </c>
+      <c r="G393" s="5">
+        <v>45</v>
+      </c>
+      <c r="H393" s="4">
+        <v>85</v>
+      </c>
+      <c r="I393" s="6">
+        <v>125</v>
+      </c>
+      <c r="J393">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="394" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>249</v>
+      </c>
+      <c r="B394" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C394" s="1">
+        <f t="shared" si="20"/>
+        <v>430</v>
+      </c>
+      <c r="D394" s="41">
+        <v>55</v>
+      </c>
+      <c r="E394" s="42">
+        <v>95</v>
+      </c>
+      <c r="F394" s="43">
+        <v>55</v>
+      </c>
+      <c r="G394" s="44">
+        <v>35</v>
+      </c>
+      <c r="H394" s="43">
+        <v>75</v>
+      </c>
+      <c r="I394" s="45">
+        <v>115</v>
+      </c>
+      <c r="J394">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="395" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>250</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C395" s="1">
+        <f t="shared" si="20"/>
+        <v>510</v>
+      </c>
+      <c r="D395" s="2">
+        <v>80</v>
+      </c>
+      <c r="E395" s="3">
+        <v>130</v>
+      </c>
+      <c r="F395" s="4">
+        <v>60</v>
+      </c>
+      <c r="G395" s="5">
+        <v>40</v>
+      </c>
+      <c r="H395" s="4">
+        <v>80</v>
+      </c>
+      <c r="I395" s="6">
+        <v>120</v>
+      </c>
+      <c r="J395">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="396" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>251</v>
+      </c>
+      <c r="B396" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C396" s="1">
+        <f t="shared" si="20"/>
+        <v>290</v>
+      </c>
+      <c r="D396" s="2">
+        <v>45</v>
+      </c>
+      <c r="E396" s="3">
+        <v>30</v>
+      </c>
+      <c r="F396" s="4">
+        <v>40</v>
+      </c>
+      <c r="G396" s="5">
+        <v>105</v>
+      </c>
+      <c r="H396" s="4">
+        <v>50</v>
+      </c>
+      <c r="I396" s="6">
+        <v>20</v>
+      </c>
+      <c r="J396">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="397" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>252</v>
+      </c>
+      <c r="B397" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C397" s="1">
+        <f>SUM(D397:I397)</f>
+        <v>370</v>
+      </c>
+      <c r="D397" s="2">
+        <v>65</v>
+      </c>
+      <c r="E397" s="3">
+        <v>40</v>
+      </c>
+      <c r="F397" s="4">
+        <v>50</v>
+      </c>
+      <c r="G397" s="5">
+        <v>125</v>
+      </c>
+      <c r="H397" s="4">
+        <v>60</v>
+      </c>
+      <c r="I397" s="6">
+        <v>30</v>
+      </c>
+      <c r="J397">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="398" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>253</v>
+      </c>
+      <c r="B398" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C398" s="1">
+        <f>SUM(D398:I398)</f>
+        <v>490</v>
+      </c>
+      <c r="D398" s="2">
+        <v>110</v>
+      </c>
+      <c r="E398" s="3">
+        <v>65</v>
+      </c>
+      <c r="F398" s="4">
+        <v>75</v>
+      </c>
+      <c r="G398" s="5">
+        <v>125</v>
+      </c>
+      <c r="H398" s="4">
+        <v>85</v>
+      </c>
+      <c r="I398" s="6">
+        <v>30</v>
+      </c>
+      <c r="J398">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="399" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>254</v>
+      </c>
+      <c r="B399" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C399" s="1">
+        <f>SUM(D399:I399)</f>
+        <v>0</v>
+      </c>
+      <c r="J399">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="400" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>255</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C400" s="1">
+        <f>SUM(D400:I400)</f>
+        <v>0</v>
+      </c>
+      <c r="J400">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>256</v>
+      </c>
+      <c r="B401" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C401" s="1">
+        <f>SUM(D401:I401)</f>
+        <v>0</v>
+      </c>
+      <c r="J401">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>257</v>
+      </c>
+      <c r="B402" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C402" s="1">
+        <f>SUM(D402:I402)</f>
+        <v>458</v>
+      </c>
+      <c r="D402" s="2">
+        <v>73</v>
+      </c>
+      <c r="E402" s="3">
+        <v>100</v>
+      </c>
+      <c r="F402" s="4">
+        <v>60</v>
+      </c>
+      <c r="G402" s="5">
+        <v>100</v>
+      </c>
+      <c r="H402" s="4">
+        <v>60</v>
+      </c>
+      <c r="I402" s="6">
+        <v>65</v>
+      </c>
+      <c r="J402">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>258</v>
+      </c>
+      <c r="B403" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C403" s="1">
+        <f>SUM(D403:I403)</f>
+        <v>0</v>
+      </c>
+      <c r="J403">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>259</v>
+      </c>
+      <c r="B404" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C404" s="1">
+        <f>SUM(D404:I404)</f>
+        <v>312</v>
+      </c>
+      <c r="D404" s="2">
+        <v>80</v>
+      </c>
+      <c r="E404" s="3">
+        <v>43</v>
+      </c>
+      <c r="F404" s="4">
+        <v>53</v>
+      </c>
+      <c r="G404" s="5">
+        <v>43</v>
+      </c>
+      <c r="H404" s="4">
+        <v>53</v>
+      </c>
+      <c r="I404" s="6">
+        <v>40</v>
+      </c>
+      <c r="J404">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>260</v>
+      </c>
+      <c r="B405" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C405" s="1">
+        <f>SUM(D405:I405)</f>
+        <v>487</v>
+      </c>
+      <c r="D405" s="2">
+        <v>120</v>
+      </c>
+      <c r="E405" s="3">
+        <v>73</v>
+      </c>
+      <c r="F405" s="4">
+        <v>83</v>
+      </c>
+      <c r="G405" s="5">
+        <v>73</v>
+      </c>
+      <c r="H405" s="4">
+        <v>83</v>
+      </c>
+      <c r="I405" s="6">
+        <v>55</v>
+      </c>
+      <c r="J405">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>261</v>
+      </c>
+      <c r="B406" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C406" s="1">
+        <f>SUM(D406:I406)</f>
+        <v>0</v>
+      </c>
+      <c r="J406">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>262</v>
+      </c>
+      <c r="B407" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C407" s="1">
+        <f>SUM(D407:I407)</f>
+        <v>0</v>
+      </c>
+      <c r="J407">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>263</v>
+      </c>
+      <c r="B408" t="s">
+        <v>864</v>
+      </c>
+      <c r="C408" s="1">
+        <f>SUM(D408:I408)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>264</v>
+      </c>
+      <c r="B409" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C409" s="1">
+        <f>SUM(D409:I409)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B621">
+        <f>MAX(B385:B619)</f>
         <v>0</v>
       </c>
     </row>
@@ -31904,7 +32668,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C1:C140 C146:C385" formulaRange="1"/>
+    <ignoredError sqref="C1:C140 C146:C407" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="4">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
New sprites and added a bunch more Pokemon
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83258CCB-F06A-4DBE-B902-93DB88FCA78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE918B2-ECB3-4909-93F5-EE56AFEDCAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2497" uniqueCount="1188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="1192">
   <si>
     <t>Leafer</t>
   </si>
@@ -3600,6 +3600,18 @@
   </si>
   <si>
     <t>Seviper-X</t>
+  </si>
+  <si>
+    <t>Bronzor</t>
+  </si>
+  <si>
+    <t>Bronzong</t>
+  </si>
+  <si>
+    <t>Bronzor-X</t>
+  </si>
+  <si>
+    <t>Bronzong-X</t>
   </si>
 </sst>
 </file>
@@ -4017,8 +4029,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}" name="Table3" displayName="Table3" ref="B145:J419" totalsRowShown="0" tableBorderDxfId="4">
-  <autoFilter ref="B145:J419" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}" name="Table3" displayName="Table3" ref="B145:J423" totalsRowShown="0" tableBorderDxfId="4">
+  <autoFilter ref="B145:J423" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{954E08A8-D138-4D6D-97C7-F47E4324725D}" name="Name"/>
     <tableColumn id="2" xr3:uid="{F9097124-9DD8-47D1-881E-F9976C72C702}" name="Total" dataCellStyle="60% - Accent4">
@@ -4390,8 +4402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AT621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A393" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G415" sqref="G415"/>
+    <sheetView tabSelected="1" topLeftCell="A389" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C421" sqref="C421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32808,6 +32820,54 @@
       </c>
       <c r="C419" s="1">
         <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>275</v>
+      </c>
+      <c r="B420" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C420" s="1">
+        <f>SUM(D420:I420)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>276</v>
+      </c>
+      <c r="B421" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C421" s="1">
+        <f>SUM(D421:I421)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>277</v>
+      </c>
+      <c r="B422" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C422" s="1">
+        <f>SUM(D422:I422)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>278</v>
+      </c>
+      <c r="B423" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C423" s="1">
+        <f>SUM(D423:I423)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New sprites, and a couple items checked off on the TODO list
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE918B2-ECB3-4909-93F5-EE56AFEDCAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229CF193-5781-4B10-8C89-859759AA84AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -4402,8 +4402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AT621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C421" sqref="C421"/>
+    <sheetView tabSelected="1" topLeftCell="I256" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O194" sqref="O194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18708,7 +18708,7 @@
       <c r="M192" s="20" t="s">
         <v>871</v>
       </c>
-      <c r="N192" t="s">
+      <c r="N192" s="17" t="s">
         <v>776</v>
       </c>
       <c r="O192">

</xml_diff>

<commit_message>
Prepping for trainer classes
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229CF193-5781-4B10-8C89-859759AA84AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13589B1D-C1C1-495B-924E-CD3E7289D7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="1192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="1193">
   <si>
     <t>Leafer</t>
   </si>
@@ -3612,6 +3612,9 @@
   </si>
   <si>
     <t>Bronzong-X</t>
+  </si>
+  <si>
+    <t>Arthra uses</t>
   </si>
 </sst>
 </file>
@@ -4402,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AT621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I256" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O194" sqref="O194"/>
+    <sheetView tabSelected="1" topLeftCell="A391" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K417" sqref="K417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32766,7 +32769,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>272</v>
       </c>
@@ -32799,7 +32802,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>273</v>
       </c>
@@ -32811,7 +32814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>274</v>
       </c>
@@ -32822,8 +32825,11 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K419" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>275</v>
       </c>
@@ -32835,7 +32841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>276</v>
       </c>
@@ -32847,7 +32853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>277</v>
       </c>
@@ -32859,7 +32865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>278</v>
       </c>
@@ -32869,6 +32875,9 @@
       <c r="C423" s="1">
         <f>SUM(D423:I423)</f>
         <v>0</v>
+      </c>
+      <c r="K423" t="s">
+        <v>1192</v>
       </c>
     </row>
     <row r="621" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New sprites and implemented new abilities
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38484908-279C-4B10-AB84-A70BBAC13C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663EEED9-B162-4BD0-BF85-C66499078E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="1213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2546" uniqueCount="1218">
   <si>
     <t>Leafer</t>
   </si>
@@ -3675,6 +3675,21 @@
   </si>
   <si>
     <t>Analytic</t>
+  </si>
+  <si>
+    <t>Bichirville</t>
+  </si>
+  <si>
+    <t>Flowerhorn Grove</t>
+  </si>
+  <si>
+    <t>Skipjack City</t>
+  </si>
+  <si>
+    <t>Sheephead Village</t>
+  </si>
+  <si>
+    <t>Arowana City</t>
   </si>
 </sst>
 </file>
@@ -3771,7 +3786,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3902,12 +3917,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE2EFDA"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -3934,6 +3943,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E1F2"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4005,16 +4044,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -4615,8 +4654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AU620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J430" sqref="J430"/>
+    <sheetView tabSelected="1" topLeftCell="O136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W167" sqref="W167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8278,28 +8317,28 @@
         <v>390</v>
       </c>
       <c r="M55" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="N55">
-        <v>66.7</v>
+        <v>74.5</v>
       </c>
       <c r="O55">
-        <v>63.8</v>
+        <v>93.5</v>
       </c>
       <c r="P55">
-        <v>70.7</v>
+        <v>67.3</v>
       </c>
       <c r="Q55">
-        <v>64.900000000000006</v>
+        <v>74.2</v>
       </c>
       <c r="R55">
-        <v>75.8</v>
+        <v>72</v>
       </c>
       <c r="S55">
-        <v>66.2</v>
+        <v>85.8</v>
       </c>
       <c r="T55">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X55" s="10" t="s">
         <v>231</v>
@@ -8366,28 +8405,28 @@
         <v>465</v>
       </c>
       <c r="M56" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N56">
-        <v>70.099999999999994</v>
+        <v>66.7</v>
       </c>
       <c r="O56">
-        <v>82.3</v>
+        <v>63.8</v>
       </c>
       <c r="P56">
-        <v>70.599999999999994</v>
+        <v>70.7</v>
       </c>
       <c r="Q56">
-        <v>72.2</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="R56">
-        <v>68.2</v>
+        <v>75.8</v>
       </c>
       <c r="S56">
-        <v>73.099999999999994</v>
+        <v>66.2</v>
       </c>
       <c r="T56">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X56" s="12" t="s">
         <v>178</v>
@@ -8545,28 +8584,28 @@
         <v>419</v>
       </c>
       <c r="M58" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="N58">
-        <v>63.8</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="O58">
-        <v>62.4</v>
+        <v>82.3</v>
       </c>
       <c r="P58">
-        <v>62.6</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="Q58">
-        <v>89</v>
+        <v>72.2</v>
       </c>
       <c r="R58">
-        <v>80.900000000000006</v>
+        <v>68.2</v>
       </c>
       <c r="S58">
-        <v>61.2</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="T58">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="X58" s="10" t="s">
         <v>233</v>
@@ -8636,25 +8675,25 @@
         <v>208</v>
       </c>
       <c r="N59">
-        <v>62.4</v>
+        <v>65.2</v>
       </c>
       <c r="O59">
-        <v>55.1</v>
+        <v>61.5</v>
       </c>
       <c r="P59">
-        <v>57.3</v>
+        <v>60.7</v>
       </c>
       <c r="Q59">
-        <v>80.400000000000006</v>
+        <v>85.7</v>
       </c>
       <c r="R59">
-        <v>79.900000000000006</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="S59">
-        <v>69.7</v>
+        <v>73.7</v>
       </c>
       <c r="T59">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="X59" s="10" t="s">
         <v>234</v>
@@ -8721,28 +8760,28 @@
         <v>500</v>
       </c>
       <c r="M60" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="N60">
-        <v>79.8</v>
+        <v>63.8</v>
       </c>
       <c r="O60">
-        <v>82.2</v>
+        <v>62.4</v>
       </c>
       <c r="P60">
-        <v>97</v>
+        <v>62.6</v>
       </c>
       <c r="Q60">
-        <v>65.2</v>
+        <v>89</v>
       </c>
       <c r="R60">
-        <v>76</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="S60">
-        <v>52.1</v>
+        <v>61.2</v>
       </c>
       <c r="T60">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X60" s="12" t="s">
         <v>235</v>
@@ -8812,25 +8851,25 @@
         <v>390</v>
       </c>
       <c r="M61" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="N61">
-        <v>71.7</v>
+        <v>79.8</v>
       </c>
       <c r="O61">
-        <v>87.9</v>
+        <v>82.2</v>
       </c>
       <c r="P61">
-        <v>63.6</v>
+        <v>97</v>
       </c>
       <c r="Q61">
-        <v>67.3</v>
+        <v>65.2</v>
       </c>
       <c r="R61">
-        <v>71.2</v>
+        <v>76</v>
       </c>
       <c r="S61">
-        <v>82.3</v>
+        <v>52.1</v>
       </c>
       <c r="T61">
         <v>29</v>
@@ -8900,28 +8939,28 @@
         <v>486</v>
       </c>
       <c r="M62" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="N62">
-        <v>85.1</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="O62">
-        <v>80.7</v>
+        <v>76.5</v>
       </c>
       <c r="P62">
-        <v>76.5</v>
+        <v>70.7</v>
       </c>
       <c r="Q62">
-        <v>78.5</v>
+        <v>75.3</v>
       </c>
       <c r="R62">
-        <v>81.400000000000006</v>
+        <v>73.5</v>
       </c>
       <c r="S62">
-        <v>70.400000000000006</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="T62">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X62" s="10" t="s">
         <v>238</v>
@@ -8991,25 +9030,25 @@
         <v>176</v>
       </c>
       <c r="N63">
-        <v>74.900000000000006</v>
+        <v>75.3</v>
       </c>
       <c r="O63">
-        <v>67.099999999999994</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="P63">
         <v>71.5</v>
       </c>
       <c r="Q63">
-        <v>87</v>
+        <v>88.7</v>
       </c>
       <c r="R63">
-        <v>74.2</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="S63">
-        <v>71.3</v>
+        <v>72.2</v>
       </c>
       <c r="T63">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X63" s="12" t="s">
         <v>239</v>
@@ -9076,28 +9115,28 @@
         <v>471</v>
       </c>
       <c r="M64" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="N64">
-        <v>60.1</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="O64">
-        <v>82.4</v>
+        <v>91.6</v>
       </c>
       <c r="P64">
-        <v>71</v>
+        <v>69.2</v>
       </c>
       <c r="Q64">
-        <v>55.8</v>
+        <v>86.6</v>
       </c>
       <c r="R64">
-        <v>62.3</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="S64">
-        <v>73.599999999999994</v>
+        <v>81.8</v>
       </c>
       <c r="T64">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="X64" s="10" t="s">
         <v>240</v>
@@ -9164,28 +9203,28 @@
         <v>400</v>
       </c>
       <c r="M65" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="N65">
-        <v>67.599999999999994</v>
+        <v>85</v>
       </c>
       <c r="O65">
-        <v>89.8</v>
+        <v>82</v>
       </c>
       <c r="P65">
-        <v>68.8</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="Q65">
-        <v>87.5</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="R65">
-        <v>80.2</v>
+        <v>80.8</v>
       </c>
       <c r="S65">
-        <v>81.2</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="T65">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X65" t="s">
         <v>241</v>
@@ -9252,28 +9291,28 @@
         <v>495</v>
       </c>
       <c r="M66" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="N66">
-        <v>61.3</v>
+        <v>61</v>
       </c>
       <c r="O66">
-        <v>79</v>
+        <v>83.7</v>
       </c>
       <c r="P66">
-        <v>86</v>
+        <v>71.2</v>
       </c>
       <c r="Q66">
-        <v>54.6</v>
+        <v>56.5</v>
       </c>
       <c r="R66">
-        <v>58</v>
+        <v>62.3</v>
       </c>
       <c r="S66">
-        <v>55.5</v>
+        <v>74.2</v>
       </c>
       <c r="T66">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X66" s="10" t="s">
         <v>242</v>
@@ -9340,28 +9379,28 @@
         <v>330</v>
       </c>
       <c r="M67" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="N67">
-        <v>66.3</v>
+        <v>61.3</v>
       </c>
       <c r="O67">
-        <v>69.3</v>
+        <v>79</v>
       </c>
       <c r="P67">
-        <v>71.599999999999994</v>
+        <v>86</v>
       </c>
       <c r="Q67">
-        <v>72.2</v>
+        <v>54.6</v>
       </c>
       <c r="R67">
-        <v>76.5</v>
+        <v>58</v>
       </c>
       <c r="S67">
-        <v>62.9</v>
+        <v>55.5</v>
       </c>
       <c r="T67">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="X67" s="10" t="s">
         <v>243</v>
@@ -9537,7 +9576,7 @@
         <v>83.9</v>
       </c>
       <c r="T69">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X69" s="10" t="s">
         <v>245</v>
@@ -9607,25 +9646,25 @@
         <v>200</v>
       </c>
       <c r="N70">
-        <v>66.2</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="O70">
-        <v>70.8</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="P70">
-        <v>70.8</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="Q70">
-        <v>80</v>
+        <v>79.8</v>
       </c>
       <c r="R70">
-        <v>71.900000000000006</v>
+        <v>71.5</v>
       </c>
       <c r="S70">
-        <v>70.2</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="T70">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="X70" t="s">
         <v>246</v>
@@ -9783,25 +9822,25 @@
         <v>206</v>
       </c>
       <c r="N72">
-        <v>71.400000000000006</v>
+        <v>72</v>
       </c>
       <c r="O72">
-        <v>92.3</v>
+        <v>93.5</v>
       </c>
       <c r="P72">
-        <v>90.1</v>
+        <v>89.2</v>
       </c>
       <c r="Q72">
-        <v>68.8</v>
+        <v>69.2</v>
       </c>
       <c r="R72">
-        <v>76.400000000000006</v>
+        <v>75.7</v>
       </c>
       <c r="S72">
-        <v>72.8</v>
+        <v>73.7</v>
       </c>
       <c r="T72">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X72" s="10" t="s">
         <v>248</v>
@@ -9871,22 +9910,22 @@
         <v>184</v>
       </c>
       <c r="N73">
-        <v>74.7</v>
+        <v>75.5</v>
       </c>
       <c r="O73">
-        <v>85.6</v>
+        <v>88.7</v>
       </c>
       <c r="P73">
-        <v>72.099999999999994</v>
+        <v>72.3</v>
       </c>
       <c r="Q73">
-        <v>74</v>
+        <v>74.099999999999994</v>
       </c>
       <c r="R73">
-        <v>83.4</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="S73">
-        <v>70.099999999999994</v>
+        <v>72.2</v>
       </c>
       <c r="T73">
         <v>19</v>
@@ -10048,31 +10087,31 @@
       </c>
       <c r="N75" s="45">
         <f>SUBTOTAL(101,Table1[HP])</f>
-        <v>70.50500000000001</v>
+        <v>71.09</v>
       </c>
       <c r="O75" s="46">
         <f>SUBTOTAL(101,Table1[Atk])</f>
-        <v>78.74499999999999</v>
+        <v>80.470000000000013</v>
       </c>
       <c r="P75" s="47">
         <f>SUBTOTAL(101,Table1[Def])</f>
-        <v>73.524999999999991</v>
+        <v>73.830000000000013</v>
       </c>
       <c r="Q75" s="48">
         <f>SUBTOTAL(101,Table1[SpA])</f>
-        <v>72.709999999999994</v>
+        <v>73.559999999999988</v>
       </c>
       <c r="R75" s="47">
         <f>SUBTOTAL(101,Table1[SpD])</f>
-        <v>74.680000000000021</v>
+        <v>74.335000000000008</v>
       </c>
       <c r="S75" s="49">
         <f>SUBTOTAL(101,Table1[Spe])</f>
-        <v>71.16</v>
+        <v>72.03</v>
       </c>
       <c r="T75" s="33">
         <f>SUBTOTAL(101,Table1[Amt])</f>
-        <v>25.7</v>
+        <v>26.3</v>
       </c>
       <c r="X75" s="10" t="s">
         <v>250</v>
@@ -14539,6 +14578,9 @@
       <c r="V144" t="s">
         <v>857</v>
       </c>
+      <c r="W144" t="s">
+        <v>808</v>
+      </c>
       <c r="X144" s="10" t="s">
         <v>318</v>
       </c>
@@ -14707,6 +14749,9 @@
       <c r="V146" t="s">
         <v>858</v>
       </c>
+      <c r="W146" t="s">
+        <v>1213</v>
+      </c>
       <c r="X146" t="s">
         <v>320</v>
       </c>
@@ -14900,6 +14945,9 @@
       <c r="V148" t="s">
         <v>858</v>
       </c>
+      <c r="W148" t="s">
+        <v>1214</v>
+      </c>
       <c r="X148" t="s">
         <v>322</v>
       </c>
@@ -15776,6 +15824,9 @@
       <c r="V157" t="s">
         <v>859</v>
       </c>
+      <c r="W157" t="s">
+        <v>1216</v>
+      </c>
       <c r="X157" s="10" t="s">
         <v>330</v>
       </c>
@@ -16459,6 +16510,9 @@
       <c r="V164" t="s">
         <v>859</v>
       </c>
+      <c r="W164" t="s">
+        <v>1217</v>
+      </c>
       <c r="X164" t="s">
         <v>336</v>
       </c>
@@ -17225,6 +17279,9 @@
       </c>
       <c r="U172" t="s">
         <v>835</v>
+      </c>
+      <c r="W172" t="s">
+        <v>1215</v>
       </c>
       <c r="X172" s="10" t="s">
         <v>194</v>
@@ -33262,7 +33319,25 @@
       </c>
       <c r="D399" s="1">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>290</v>
+      </c>
+      <c r="E399" s="2">
+        <v>45</v>
+      </c>
+      <c r="F399" s="3">
+        <v>20</v>
+      </c>
+      <c r="G399" s="4">
+        <v>45</v>
+      </c>
+      <c r="H399" s="5">
+        <v>105</v>
+      </c>
+      <c r="I399" s="4">
+        <v>55</v>
+      </c>
+      <c r="J399" s="6">
+        <v>20</v>
       </c>
       <c r="K399">
         <v>290</v>
@@ -33676,7 +33751,7 @@
       </c>
       <c r="D416" s="1">
         <f t="shared" si="21"/>
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="E416" s="2">
         <v>60</v>
@@ -33688,7 +33763,7 @@
         <v>50</v>
       </c>
       <c r="H416" s="5">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="I416" s="4">
         <v>80</v>
@@ -33697,7 +33772,7 @@
         <v>70</v>
       </c>
       <c r="K416">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="417" spans="1:15" x14ac:dyDescent="0.25">
@@ -33742,7 +33817,28 @@
       </c>
       <c r="D419" s="1">
         <f t="shared" ref="D419:D436" si="22">SUM(E419:J419)</f>
-        <v>0</v>
+        <v>300</v>
+      </c>
+      <c r="E419" s="2">
+        <v>57</v>
+      </c>
+      <c r="F419" s="3">
+        <v>24</v>
+      </c>
+      <c r="G419" s="4">
+        <v>86</v>
+      </c>
+      <c r="H419" s="5">
+        <v>24</v>
+      </c>
+      <c r="I419" s="4">
+        <v>86</v>
+      </c>
+      <c r="J419" s="6">
+        <v>23</v>
+      </c>
+      <c r="K419">
+        <v>300</v>
       </c>
     </row>
     <row r="420" spans="1:15" x14ac:dyDescent="0.25">
@@ -33754,7 +33850,28 @@
       </c>
       <c r="D420" s="1">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>500</v>
+      </c>
+      <c r="E420" s="2">
+        <v>67</v>
+      </c>
+      <c r="F420" s="3">
+        <v>89</v>
+      </c>
+      <c r="G420" s="4">
+        <v>116</v>
+      </c>
+      <c r="H420" s="5">
+        <v>79</v>
+      </c>
+      <c r="I420" s="4">
+        <v>116</v>
+      </c>
+      <c r="J420" s="6">
+        <v>33</v>
+      </c>
+      <c r="K420">
+        <v>500</v>
       </c>
     </row>
     <row r="421" spans="1:15" x14ac:dyDescent="0.25">
@@ -33771,6 +33888,9 @@
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
+      <c r="K421">
+        <v>300</v>
+      </c>
     </row>
     <row r="422" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A422">
@@ -33785,6 +33905,9 @@
       <c r="D422" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
+      </c>
+      <c r="K422">
+        <v>500</v>
       </c>
       <c r="L422" t="s">
         <v>1191</v>

</xml_diff>

<commit_message>
Worked on first floor for lab - going to need partial collision tiles
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E10BE9-45C7-41FF-A8F2-CA4B2CBDC956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAFF5A8-04AE-4A0A-B79D-3A7EED447634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2552" uniqueCount="1219">
   <si>
     <t>Leafer</t>
   </si>
@@ -4084,122 +4084,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="9" builtinId="5"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF595959"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF595959"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -4387,6 +4272,9 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="double">
           <color rgb="FF3F3F3F"/>
@@ -4413,7 +4301,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}" name="Table3" displayName="Table3" ref="A145:K436" totalsRowShown="0" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}" name="Table3" displayName="Table3" ref="A145:K436" totalsRowShown="0" tableBorderDxfId="11">
   <autoFilter ref="A145:K436" xr:uid="{12DD2A8C-1E55-4C6C-8CEC-614080B9B737}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A146:K436">
     <sortCondition ref="B145:B436"/>
@@ -4422,7 +4310,7 @@
     <tableColumn id="10" xr3:uid="{BCD684F9-91A2-458E-B61B-0E2FC6A62D0D}" name="Pkdx #"/>
     <tableColumn id="11" xr3:uid="{C8B5C43A-CE53-443E-8C1D-AC00B102DB7C}" name="ID"/>
     <tableColumn id="1" xr3:uid="{954E08A8-D138-4D6D-97C7-F47E4324725D}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{F9097124-9DD8-47D1-881E-F9976C72C702}" name="Total" dataDxfId="1" dataCellStyle="60% - Accent4">
+    <tableColumn id="2" xr3:uid="{F9097124-9DD8-47D1-881E-F9976C72C702}" name="Total" dataDxfId="10" dataCellStyle="60% - Accent4">
       <calculatedColumnFormula>SUM($E146:$J146)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{D7056670-07AC-4C55-9FE2-A9E5FE4DB2A1}" name="HP" dataCellStyle="20% - Accent6"/>
@@ -4445,13 +4333,13 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5ECD7C50-12C2-4722-BB43-4A5392C844D3}" name="Type" totalsRowLabel="TOTAL"/>
-    <tableColumn id="2" xr3:uid="{1FEEF44A-9297-470E-B8C5-DB2860F63B26}" name="HP" totalsRowFunction="average" totalsRowDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{C4F64A03-884E-4ABF-863F-FB93EB9C48D7}" name="Atk" totalsRowFunction="average" totalsRowDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7D26ECE6-FEFB-43CC-9954-6A7B9A9B1FFF}" name="Def" totalsRowFunction="average" totalsRowDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{5E7CA636-F06B-46EF-9E88-779A1C949192}" name="SpA" totalsRowFunction="average" totalsRowDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{21E01ACA-9002-4C73-9BFF-AF400041F7E7}" name="SpD" totalsRowFunction="average" totalsRowDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{717E4770-D119-4D0A-BD0F-58E3D3ADFE4C}" name="Spe" totalsRowFunction="average" totalsRowDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{8B8669EB-BDCE-49F8-84EE-CA277552CD38}" name="Amt" totalsRowFunction="average" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{1FEEF44A-9297-470E-B8C5-DB2860F63B26}" name="HP" totalsRowFunction="average" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{C4F64A03-884E-4ABF-863F-FB93EB9C48D7}" name="Atk" totalsRowFunction="average" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{7D26ECE6-FEFB-43CC-9954-6A7B9A9B1FFF}" name="Def" totalsRowFunction="average" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5E7CA636-F06B-46EF-9E88-779A1C949192}" name="SpA" totalsRowFunction="average" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{21E01ACA-9002-4C73-9BFF-AF400041F7E7}" name="SpD" totalsRowFunction="average" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{717E4770-D119-4D0A-BD0F-58E3D3ADFE4C}" name="Spe" totalsRowFunction="average" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{8B8669EB-BDCE-49F8-84EE-CA277552CD38}" name="Amt" totalsRowFunction="average" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4467,8 +4355,8 @@
     <tableColumn id="5" xr3:uid="{D4240EEB-6B7E-4513-81CD-64F028AE015F}" name="Num"/>
     <tableColumn id="1" xr3:uid="{927F8053-02EB-4DE4-A9C2-E39369A9D18C}" name="Species"/>
     <tableColumn id="2" xr3:uid="{88EA7429-2A79-45C2-9DAD-432E911FB847}" name="Amount"/>
-    <tableColumn id="3" xr3:uid="{31049355-8917-406D-A961-EA9E609C094C}" name="Average" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{9EB8DBFF-5E4E-4D13-B06A-8EEDCAE0D250}" name="Total" dataDxfId="16" dataCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{31049355-8917-406D-A961-EA9E609C094C}" name="Average" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{9EB8DBFF-5E4E-4D13-B06A-8EEDCAE0D250}" name="Total" dataDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>AC30*AB30</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4486,7 +4374,7 @@
     <tableColumn id="1" xr3:uid="{71084C9A-5E75-4048-82AA-70A2D1CBD776}" name="Num"/>
     <tableColumn id="2" xr3:uid="{7A1103DC-DAF9-41EF-BBD3-0883ED909130}" name="Pokemon"/>
     <tableColumn id="3" xr3:uid="{A641B1E3-DC03-463F-B2D8-CE49F38612E2}" name="Amt"/>
-    <tableColumn id="4" xr3:uid="{8554C379-EE33-4C0B-B30E-A04B1C29BF4E}" name="%" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{8554C379-EE33-4C0B-B30E-A04B1C29BF4E}" name="%" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4791,8 +4679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AU620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33:P41"/>
+    <sheetView tabSelected="1" topLeftCell="A403" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M387" sqref="M387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31587,33 +31475,35 @@
         <v>430</v>
       </c>
       <c r="E356" s="2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F356" s="3">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="G356" s="4">
         <v>65</v>
       </c>
       <c r="H356" s="5">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="I356" s="4">
         <v>65</v>
       </c>
       <c r="J356" s="6">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K356">
         <v>430</v>
       </c>
       <c r="L356" s="9" t="s">
-        <v>658</v>
+        <v>609</v>
       </c>
       <c r="M356" t="s">
-        <v>623</v>
-      </c>
-      <c r="N356" s="20"/>
+        <v>659</v>
+      </c>
+      <c r="N356" s="20" t="s">
+        <v>1170</v>
+      </c>
       <c r="P356">
         <v>211</v>
       </c>
@@ -31637,33 +31527,35 @@
         <v>530</v>
       </c>
       <c r="E357" s="2">
+        <v>90</v>
+      </c>
+      <c r="F357" s="3">
         <v>75</v>
       </c>
-      <c r="F357" s="3">
-        <v>124</v>
-      </c>
       <c r="G357" s="4">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="H357" s="5">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="I357" s="4">
         <v>70</v>
       </c>
       <c r="J357" s="6">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="K357">
         <v>530</v>
       </c>
       <c r="L357" s="9" t="s">
-        <v>658</v>
+        <v>609</v>
       </c>
       <c r="M357" t="s">
-        <v>623</v>
-      </c>
-      <c r="N357" s="20"/>
+        <v>659</v>
+      </c>
+      <c r="N357" s="20" t="s">
+        <v>1170</v>
+      </c>
       <c r="P357">
         <v>212</v>
       </c>
@@ -31716,7 +31608,9 @@
       <c r="M358" t="s">
         <v>166</v>
       </c>
-      <c r="N358" s="20"/>
+      <c r="N358" s="20" t="s">
+        <v>1112</v>
+      </c>
       <c r="P358">
         <v>213</v>
       </c>
@@ -31766,7 +31660,9 @@
       <c r="M359" t="s">
         <v>166</v>
       </c>
-      <c r="N359" s="20"/>
+      <c r="N359" s="20" t="s">
+        <v>1112</v>
+      </c>
       <c r="P359">
         <v>214</v>
       </c>
@@ -33051,10 +32947,10 @@
       </c>
       <c r="D385" s="1">
         <f>SUM($E385:$J385)</f>
-        <v>570</v>
+        <v>555</v>
       </c>
       <c r="E385" s="2">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F385" s="3">
         <v>110</v>
@@ -33063,16 +32959,16 @@
         <v>120</v>
       </c>
       <c r="H385" s="5">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="I385" s="4">
         <v>120</v>
       </c>
       <c r="J385" s="6">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="K385">
-        <v>570</v>
+        <v>555</v>
       </c>
       <c r="L385" t="s">
         <v>807</v>

</xml_diff>

<commit_message>
Programmed a Game Tools program and added a new package for it!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057D88D9-8236-409C-A7BA-4DF539D71E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3022D7F6-D368-496C-B4BE-1F4DC224D2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-12915" windowWidth="16440" windowHeight="28440" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2552" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="1220">
   <si>
     <t>Leafer</t>
   </si>
@@ -3693,6 +3693,9 @@
   </si>
   <si>
     <t>Pkdx #</t>
+  </si>
+  <si>
+    <t>Route 45</t>
   </si>
 </sst>
 </file>
@@ -4679,8 +4682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AU620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U148" sqref="U148"/>
+    <sheetView tabSelected="1" topLeftCell="H165" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U174" sqref="U174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19074,6 +19077,12 @@
       <c r="Q191" t="str">
         <f t="shared" si="11"/>
         <v>Ludicolo</v>
+      </c>
+      <c r="T191">
+        <v>47</v>
+      </c>
+      <c r="U191" t="s">
+        <v>1219</v>
       </c>
       <c r="X191" s="12" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
Worked on research part of Gym 2 split
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3022D7F6-D368-496C-B4BE-1F4DC224D2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8951B9-5772-4109-90D0-1CC4FFA714B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -4682,8 +4682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AU620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H165" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U174" sqref="U174"/>
+    <sheetView tabSelected="1" topLeftCell="A396" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H419" sqref="H419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34027,7 +34027,28 @@
       </c>
       <c r="D417" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>210</v>
+      </c>
+      <c r="E417" s="2">
+        <v>50</v>
+      </c>
+      <c r="F417" s="3">
+        <v>20</v>
+      </c>
+      <c r="G417" s="4">
+        <v>50</v>
+      </c>
+      <c r="H417" s="5">
+        <v>35</v>
+      </c>
+      <c r="I417" s="4">
+        <v>30</v>
+      </c>
+      <c r="J417" s="6">
+        <v>25</v>
+      </c>
+      <c r="K417">
+        <v>210</v>
       </c>
     </row>
     <row r="418" spans="1:15" x14ac:dyDescent="0.25">
@@ -34042,7 +34063,28 @@
       </c>
       <c r="D418" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>405</v>
+      </c>
+      <c r="E418" s="2">
+        <v>60</v>
+      </c>
+      <c r="F418" s="3">
+        <v>20</v>
+      </c>
+      <c r="G418" s="4">
+        <v>55</v>
+      </c>
+      <c r="H418" s="5">
+        <v>105</v>
+      </c>
+      <c r="I418" s="4">
+        <v>90</v>
+      </c>
+      <c r="J418" s="6">
+        <v>75</v>
+      </c>
+      <c r="K418">
+        <v>405</v>
       </c>
       <c r="L418" t="s">
         <v>1191</v>

</xml_diff>

<commit_message>
New sprites and new Pokemon TM and moveset work
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCC8458-D074-4BB7-AF3B-CCDF6A462627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6944891F-66BC-478B-AB43-E46CF716B2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="165" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4036,7 +4036,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -4088,20 +4088,6 @@
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4718,8 +4704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AU620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E427" sqref="E427"/>
+    <sheetView tabSelected="1" topLeftCell="A295" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D309" sqref="D309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14754,7 +14740,7 @@
       </c>
     </row>
     <row r="146" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A146" s="58">
+      <c r="A146" s="10">
         <v>-18</v>
       </c>
       <c r="B146">
@@ -14855,7 +14841,7 @@
       </c>
     </row>
     <row r="147" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A147" s="64">
+      <c r="A147" s="50">
         <v>-18</v>
       </c>
       <c r="B147">
@@ -14953,7 +14939,7 @@
       </c>
     </row>
     <row r="148" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A148" s="58">
+      <c r="A148" s="10">
         <v>-17</v>
       </c>
       <c r="B148">
@@ -15051,7 +15037,7 @@
       </c>
     </row>
     <row r="149" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A149" s="64">
+      <c r="A149" s="50">
         <v>-17</v>
       </c>
       <c r="B149">
@@ -15149,7 +15135,7 @@
       </c>
     </row>
     <row r="150" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A150" s="58">
+      <c r="A150" s="10">
         <v>-16</v>
       </c>
       <c r="B150">
@@ -15247,7 +15233,7 @@
       </c>
     </row>
     <row r="151" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A151" s="64">
+      <c r="A151" s="50">
         <v>-16</v>
       </c>
       <c r="B151">
@@ -15342,7 +15328,7 @@
       </c>
     </row>
     <row r="152" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A152" s="58">
+      <c r="A152" s="10">
         <v>-15</v>
       </c>
       <c r="B152">
@@ -15443,7 +15429,7 @@
       </c>
     </row>
     <row r="153" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A153" s="64">
+      <c r="A153" s="50">
         <v>-15</v>
       </c>
       <c r="B153">
@@ -15541,7 +15527,7 @@
       </c>
     </row>
     <row r="154" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A154" s="58">
+      <c r="A154" s="10">
         <v>-14</v>
       </c>
       <c r="B154">
@@ -15636,7 +15622,7 @@
       </c>
     </row>
     <row r="155" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A155" s="64">
+      <c r="A155" s="50">
         <v>-14</v>
       </c>
       <c r="B155">
@@ -15734,7 +15720,7 @@
       </c>
     </row>
     <row r="156" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A156" s="64">
+      <c r="A156" s="50">
         <v>-13</v>
       </c>
       <c r="B156">
@@ -15832,7 +15818,7 @@
       </c>
     </row>
     <row r="157" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A157" s="58">
+      <c r="A157" s="10">
         <v>-13</v>
       </c>
       <c r="B157">
@@ -15909,7 +15895,7 @@
       </c>
     </row>
     <row r="158" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A158" s="64">
+      <c r="A158" s="50">
         <v>-12</v>
       </c>
       <c r="B158">
@@ -16007,7 +15993,7 @@
       </c>
     </row>
     <row r="159" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A159" s="58">
+      <c r="A159" s="10">
         <v>-12</v>
       </c>
       <c r="B159">
@@ -16084,7 +16070,7 @@
       </c>
     </row>
     <row r="160" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A160" s="58">
+      <c r="A160" s="10">
         <v>-11</v>
       </c>
       <c r="B160">
@@ -16179,7 +16165,7 @@
       </c>
     </row>
     <row r="161" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A161" s="64">
+      <c r="A161" s="50">
         <v>-11</v>
       </c>
       <c r="B161">
@@ -16190,7 +16176,25 @@
       </c>
       <c r="D161" s="1">
         <f>SUM($E161:$J161)</f>
-        <v>0</v>
+        <v>550</v>
+      </c>
+      <c r="E161" s="2">
+        <v>84</v>
+      </c>
+      <c r="F161" s="3">
+        <v>118</v>
+      </c>
+      <c r="G161" s="4">
+        <v>75</v>
+      </c>
+      <c r="H161" s="5">
+        <v>108</v>
+      </c>
+      <c r="I161" s="4">
+        <v>75</v>
+      </c>
+      <c r="J161" s="6">
+        <v>90</v>
       </c>
       <c r="K161">
         <v>550</v>
@@ -16259,7 +16263,7 @@
       </c>
     </row>
     <row r="162" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A162" s="58">
+      <c r="A162" s="10">
         <v>-10</v>
       </c>
       <c r="B162">
@@ -16357,7 +16361,7 @@
       </c>
     </row>
     <row r="163" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A163" s="64">
+      <c r="A163" s="50">
         <v>-10</v>
       </c>
       <c r="B163">
@@ -16368,7 +16372,25 @@
       </c>
       <c r="D163" s="1">
         <f>SUM($E163:$J163)</f>
-        <v>0</v>
+        <v>486</v>
+      </c>
+      <c r="E163" s="2">
+        <v>65</v>
+      </c>
+      <c r="F163" s="3">
+        <v>113</v>
+      </c>
+      <c r="G163" s="4">
+        <v>60</v>
+      </c>
+      <c r="H163" s="5">
+        <v>103</v>
+      </c>
+      <c r="I163" s="4">
+        <v>65</v>
+      </c>
+      <c r="J163" s="6">
+        <v>80</v>
       </c>
       <c r="K163">
         <v>486</v>
@@ -16437,7 +16459,7 @@
       </c>
     </row>
     <row r="164" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A164" s="58">
+      <c r="A164" s="10">
         <v>-9</v>
       </c>
       <c r="B164">
@@ -16538,7 +16560,7 @@
       </c>
     </row>
     <row r="165" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A165" s="65">
+      <c r="A165" s="51">
         <v>-9</v>
       </c>
       <c r="B165">
@@ -16636,7 +16658,7 @@
       </c>
     </row>
     <row r="166" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A166" s="64">
+      <c r="A166" s="50">
         <v>-9</v>
       </c>
       <c r="B166">
@@ -16647,7 +16669,25 @@
       </c>
       <c r="D166" s="1">
         <f>SUM($E166:$J166)</f>
-        <v>0</v>
+        <v>304</v>
+      </c>
+      <c r="E166" s="2">
+        <v>45</v>
+      </c>
+      <c r="F166" s="3">
+        <v>67</v>
+      </c>
+      <c r="G166" s="4">
+        <v>40</v>
+      </c>
+      <c r="H166" s="5">
+        <v>47</v>
+      </c>
+      <c r="I166" s="4">
+        <v>40</v>
+      </c>
+      <c r="J166" s="6">
+        <v>65</v>
       </c>
       <c r="K166">
         <v>304</v>
@@ -16713,7 +16753,7 @@
       </c>
     </row>
     <row r="167" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A167" s="58">
+      <c r="A167" s="10">
         <v>-8</v>
       </c>
       <c r="B167">
@@ -16809,7 +16849,7 @@
       </c>
     </row>
     <row r="168" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A168" s="64">
+      <c r="A168" s="50">
         <v>-8</v>
       </c>
       <c r="B168">
@@ -16905,7 +16945,7 @@
       </c>
     </row>
     <row r="169" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A169" s="65">
+      <c r="A169" s="51">
         <v>-8</v>
       </c>
       <c r="B169">
@@ -17000,7 +17040,7 @@
       </c>
     </row>
     <row r="170" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A170" s="58">
+      <c r="A170" s="10">
         <v>-7</v>
       </c>
       <c r="B170">
@@ -17098,7 +17138,7 @@
       </c>
     </row>
     <row r="171" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A171" s="64">
+      <c r="A171" s="50">
         <v>-7</v>
       </c>
       <c r="B171">
@@ -17194,7 +17234,7 @@
       </c>
     </row>
     <row r="172" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A172" s="65">
+      <c r="A172" s="51">
         <v>-7</v>
       </c>
       <c r="B172">
@@ -17290,7 +17330,7 @@
       </c>
     </row>
     <row r="173" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A173" s="58">
+      <c r="A173" s="10">
         <v>-6</v>
       </c>
       <c r="B173">
@@ -17380,7 +17420,7 @@
       </c>
     </row>
     <row r="174" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A174" s="64">
+      <c r="A174" s="50">
         <v>-6</v>
       </c>
       <c r="B174">
@@ -17475,7 +17515,7 @@
       </c>
     </row>
     <row r="175" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A175" s="65">
+      <c r="A175" s="51">
         <v>-6</v>
       </c>
       <c r="B175">
@@ -17570,7 +17610,7 @@
       </c>
     </row>
     <row r="176" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A176" s="58">
+      <c r="A176" s="10">
         <v>-5</v>
       </c>
       <c r="B176">
@@ -17662,7 +17702,7 @@
       </c>
     </row>
     <row r="177" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A177" s="64">
+      <c r="A177" s="50">
         <v>-5</v>
       </c>
       <c r="B177">
@@ -17755,7 +17795,7 @@
       </c>
     </row>
     <row r="178" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A178" s="65">
+      <c r="A178" s="51">
         <v>-5</v>
       </c>
       <c r="B178">
@@ -17848,7 +17888,7 @@
       </c>
     </row>
     <row r="179" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A179" s="58">
+      <c r="A179" s="10">
         <v>-4</v>
       </c>
       <c r="B179">
@@ -17938,7 +17978,7 @@
       </c>
     </row>
     <row r="180" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A180" s="64">
+      <c r="A180" s="50">
         <v>-4</v>
       </c>
       <c r="B180">
@@ -18031,7 +18071,7 @@
       </c>
     </row>
     <row r="181" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A181" s="65">
+      <c r="A181" s="51">
         <v>-4</v>
       </c>
       <c r="B181">
@@ -18124,7 +18164,7 @@
       </c>
     </row>
     <row r="182" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A182" s="58">
+      <c r="A182" s="10">
         <v>-3</v>
       </c>
       <c r="B182">
@@ -18214,7 +18254,7 @@
       </c>
     </row>
     <row r="183" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A183" s="64">
+      <c r="A183" s="50">
         <v>-3</v>
       </c>
       <c r="B183">
@@ -18306,7 +18346,7 @@
       </c>
     </row>
     <row r="184" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A184" s="65">
+      <c r="A184" s="51">
         <v>-3</v>
       </c>
       <c r="B184">
@@ -18404,7 +18444,7 @@
       </c>
     </row>
     <row r="185" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A185" s="58">
+      <c r="A185" s="10">
         <v>-2</v>
       </c>
       <c r="B185">
@@ -18499,7 +18539,7 @@
       </c>
     </row>
     <row r="186" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A186" s="64">
+      <c r="A186" s="50">
         <v>-2</v>
       </c>
       <c r="B186">
@@ -18594,7 +18634,7 @@
       </c>
     </row>
     <row r="187" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A187" s="65">
+      <c r="A187" s="51">
         <v>-2</v>
       </c>
       <c r="B187">
@@ -18689,7 +18729,7 @@
       </c>
     </row>
     <row r="188" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A188" s="58">
+      <c r="A188" s="10">
         <v>-1</v>
       </c>
       <c r="B188">
@@ -18781,7 +18821,7 @@
       </c>
     </row>
     <row r="189" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A189" s="64">
+      <c r="A189" s="50">
         <v>-1</v>
       </c>
       <c r="B189">
@@ -18874,7 +18914,7 @@
       </c>
     </row>
     <row r="190" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A190" s="65">
+      <c r="A190" s="51">
         <v>-1</v>
       </c>
       <c r="B190">
@@ -27751,7 +27791,7 @@
       <c r="C294" t="s">
         <v>1220</v>
       </c>
-      <c r="D294" s="66">
+      <c r="D294" s="52">
         <f>SUM($E294:$J294)</f>
         <v>190</v>
       </c>
@@ -27810,7 +27850,7 @@
       <c r="C295" t="s">
         <v>1221</v>
       </c>
-      <c r="D295" s="66">
+      <c r="D295" s="52">
         <f>SUM($E295:$J295)</f>
         <v>250</v>
       </c>
@@ -27869,7 +27909,7 @@
       <c r="C296" t="s">
         <v>1222</v>
       </c>
-      <c r="D296" s="66">
+      <c r="D296" s="52">
         <f>SUM($E296:$J296)</f>
         <v>420</v>
       </c>
@@ -27936,7 +27976,7 @@
       <c r="C297" t="s">
         <v>428</v>
       </c>
-      <c r="D297" s="52">
+      <c r="D297" s="1">
         <f>SUM($E297:$J297)</f>
         <v>410</v>
       </c>
@@ -28067,7 +28107,7 @@
       <c r="C299" t="s">
         <v>430</v>
       </c>
-      <c r="D299" s="52">
+      <c r="D299" s="1">
         <f>SUM($E299:$J299)</f>
         <v>535</v>
       </c>
@@ -28256,7 +28296,7 @@
       </c>
     </row>
     <row r="302" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A302" s="51">
+      <c r="A302">
         <v>112</v>
       </c>
       <c r="B302">
@@ -28320,7 +28360,7 @@
       </c>
     </row>
     <row r="303" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A303" s="51">
+      <c r="A303">
         <v>113</v>
       </c>
       <c r="B303">
@@ -28369,7 +28409,7 @@
       </c>
     </row>
     <row r="304" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A304" s="51">
+      <c r="A304">
         <v>114</v>
       </c>
       <c r="B304">
@@ -28415,7 +28455,7 @@
       </c>
     </row>
     <row r="305" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A305" s="51">
+      <c r="A305">
         <v>115</v>
       </c>
       <c r="B305">
@@ -28477,7 +28517,7 @@
       </c>
     </row>
     <row r="306" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A306" s="51">
+      <c r="A306">
         <v>116</v>
       </c>
       <c r="B306">
@@ -28539,7 +28579,7 @@
       </c>
     </row>
     <row r="307" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A307" s="51">
+      <c r="A307">
         <v>117</v>
       </c>
       <c r="B307">
@@ -28601,7 +28641,7 @@
       </c>
     </row>
     <row r="308" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A308" s="51">
+      <c r="A308">
         <v>118</v>
       </c>
       <c r="B308">
@@ -28663,7 +28703,7 @@
       </c>
     </row>
     <row r="309" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A309" s="51">
+      <c r="A309">
         <v>119</v>
       </c>
       <c r="B309">
@@ -28725,7 +28765,7 @@
       </c>
     </row>
     <row r="310" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A310" s="51">
+      <c r="A310">
         <v>120</v>
       </c>
       <c r="B310">
@@ -28784,7 +28824,7 @@
       </c>
     </row>
     <row r="311" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A311" s="51">
+      <c r="A311">
         <v>121</v>
       </c>
       <c r="B311">
@@ -28848,7 +28888,7 @@
       </c>
     </row>
     <row r="312" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A312" s="51">
+      <c r="A312">
         <v>122</v>
       </c>
       <c r="B312">
@@ -28912,7 +28952,7 @@
       </c>
     </row>
     <row r="313" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A313" s="51">
+      <c r="A313">
         <v>123</v>
       </c>
       <c r="B313">
@@ -28973,7 +29013,7 @@
       </c>
     </row>
     <row r="314" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A314" s="51">
+      <c r="A314">
         <v>124</v>
       </c>
       <c r="B314">
@@ -29037,7 +29077,7 @@
       </c>
     </row>
     <row r="315" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A315" s="51">
+      <c r="A315">
         <v>125</v>
       </c>
       <c r="B315">
@@ -29098,7 +29138,7 @@
       </c>
     </row>
     <row r="316" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A316" s="51">
+      <c r="A316">
         <v>126</v>
       </c>
       <c r="B316">
@@ -29162,7 +29202,7 @@
       </c>
     </row>
     <row r="317" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A317" s="51">
+      <c r="A317">
         <v>127</v>
       </c>
       <c r="B317">
@@ -29226,7 +29266,7 @@
       </c>
     </row>
     <row r="318" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A318" s="51">
+      <c r="A318">
         <v>128</v>
       </c>
       <c r="B318">
@@ -29287,7 +29327,7 @@
       </c>
     </row>
     <row r="319" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A319" s="51">
+      <c r="A319">
         <v>129</v>
       </c>
       <c r="B319">
@@ -29349,7 +29389,7 @@
       </c>
     </row>
     <row r="320" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A320" s="51">
+      <c r="A320">
         <v>130</v>
       </c>
       <c r="B320">
@@ -29411,7 +29451,7 @@
       </c>
     </row>
     <row r="321" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A321" s="51">
+      <c r="A321">
         <v>131</v>
       </c>
       <c r="B321">
@@ -29541,7 +29581,7 @@
       <c r="C323" t="s">
         <v>459</v>
       </c>
-      <c r="D323" s="52">
+      <c r="D323" s="1">
         <f>SUM($E323:$J323)</f>
         <v>400</v>
       </c>
@@ -29662,7 +29702,7 @@
       <c r="C325" t="s">
         <v>1225</v>
       </c>
-      <c r="D325" s="66">
+      <c r="D325" s="52">
         <f>SUM($E325:$J325)</f>
         <v>290</v>
       </c>
@@ -29721,7 +29761,7 @@
       <c r="C326" t="s">
         <v>1226</v>
       </c>
-      <c r="D326" s="66">
+      <c r="D326" s="52">
         <f>SUM($E326:$J326)</f>
         <v>485</v>
       </c>
@@ -29846,7 +29886,7 @@
       <c r="C328" t="s">
         <v>467</v>
       </c>
-      <c r="D328" s="52">
+      <c r="D328" s="1">
         <f>SUM($E328:$J328)</f>
         <v>482</v>
       </c>
@@ -30313,7 +30353,7 @@
       </c>
     </row>
     <row r="336" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A336" s="51">
+      <c r="A336">
         <v>146</v>
       </c>
       <c r="B336">
@@ -30368,7 +30408,7 @@
       </c>
     </row>
     <row r="337" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A337" s="51">
+      <c r="A337">
         <v>147</v>
       </c>
       <c r="B337">
@@ -30420,7 +30460,7 @@
       </c>
     </row>
     <row r="338" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A338" s="51">
+      <c r="A338">
         <v>148</v>
       </c>
       <c r="B338">
@@ -30475,7 +30515,7 @@
       </c>
     </row>
     <row r="339" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A339" s="51">
+      <c r="A339">
         <v>149</v>
       </c>
       <c r="B339">
@@ -30527,7 +30567,7 @@
       </c>
     </row>
     <row r="340" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A340" s="51">
+      <c r="A340">
         <v>150</v>
       </c>
       <c r="B340">
@@ -30582,7 +30622,7 @@
       </c>
     </row>
     <row r="341" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A341" s="51">
+      <c r="A341">
         <v>151</v>
       </c>
       <c r="B341">
@@ -30634,7 +30674,7 @@
       </c>
     </row>
     <row r="342" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A342" s="51">
+      <c r="A342">
         <v>152</v>
       </c>
       <c r="B342">
@@ -30689,7 +30729,7 @@
       </c>
     </row>
     <row r="343" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A343" s="51">
+      <c r="A343">
         <v>153</v>
       </c>
       <c r="B343">
@@ -30741,7 +30781,7 @@
       </c>
     </row>
     <row r="344" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A344" s="51">
+      <c r="A344">
         <v>154</v>
       </c>
       <c r="B344">
@@ -30796,7 +30836,7 @@
       </c>
     </row>
     <row r="345" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A345" s="51">
+      <c r="A345">
         <v>155</v>
       </c>
       <c r="B345">
@@ -30851,7 +30891,7 @@
       </c>
     </row>
     <row r="346" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A346" s="51">
+      <c r="A346">
         <v>156</v>
       </c>
       <c r="B346">
@@ -30903,7 +30943,7 @@
       </c>
     </row>
     <row r="347" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A347" s="51">
+      <c r="A347">
         <v>157</v>
       </c>
       <c r="B347">
@@ -30956,7 +30996,7 @@
       </c>
     </row>
     <row r="348" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A348" s="51">
+      <c r="A348">
         <v>158</v>
       </c>
       <c r="B348">
@@ -31009,7 +31049,7 @@
       </c>
     </row>
     <row r="349" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A349" s="51">
+      <c r="A349">
         <v>159</v>
       </c>
       <c r="B349">
@@ -31059,7 +31099,7 @@
       </c>
     </row>
     <row r="350" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A350" s="51">
+      <c r="A350">
         <v>160</v>
       </c>
       <c r="B350">
@@ -31112,7 +31152,7 @@
       </c>
     </row>
     <row r="351" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A351" s="51">
+      <c r="A351">
         <v>161</v>
       </c>
       <c r="B351">
@@ -31165,7 +31205,7 @@
       </c>
     </row>
     <row r="352" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A352" s="51">
+      <c r="A352">
         <v>162</v>
       </c>
       <c r="B352">
@@ -31215,7 +31255,7 @@
       </c>
     </row>
     <row r="353" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A353" s="51">
+      <c r="A353">
         <v>163</v>
       </c>
       <c r="B353">
@@ -31268,7 +31308,7 @@
       </c>
     </row>
     <row r="354" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A354" s="51">
+      <c r="A354">
         <v>164</v>
       </c>
       <c r="B354">
@@ -31321,7 +31361,7 @@
       </c>
     </row>
     <row r="355" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A355" s="51">
+      <c r="A355">
         <v>165</v>
       </c>
       <c r="B355">
@@ -31374,7 +31414,7 @@
       </c>
     </row>
     <row r="356" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A356" s="51">
+      <c r="A356">
         <v>166</v>
       </c>
       <c r="B356">
@@ -31426,7 +31466,7 @@
       </c>
     </row>
     <row r="357" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A357" s="51">
+      <c r="A357">
         <v>167</v>
       </c>
       <c r="B357">
@@ -31481,7 +31521,7 @@
       </c>
     </row>
     <row r="358" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A358" s="51">
+      <c r="A358">
         <v>168</v>
       </c>
       <c r="B358">
@@ -31533,7 +31573,7 @@
       </c>
     </row>
     <row r="359" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A359" s="51">
+      <c r="A359">
         <v>169</v>
       </c>
       <c r="B359">
@@ -31588,7 +31628,7 @@
       </c>
     </row>
     <row r="360" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A360" s="51">
+      <c r="A360">
         <v>170</v>
       </c>
       <c r="B360">
@@ -31638,7 +31678,7 @@
       </c>
     </row>
     <row r="361" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A361" s="51">
+      <c r="A361">
         <v>171</v>
       </c>
       <c r="B361">
@@ -31691,7 +31731,7 @@
       </c>
     </row>
     <row r="362" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A362" s="51">
+      <c r="A362">
         <v>172</v>
       </c>
       <c r="B362">
@@ -31740,7 +31780,7 @@
       </c>
     </row>
     <row r="363" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A363" s="51">
+      <c r="A363">
         <v>173</v>
       </c>
       <c r="B363">
@@ -31774,7 +31814,7 @@
       </c>
     </row>
     <row r="364" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A364" s="51">
+      <c r="A364">
         <v>174</v>
       </c>
       <c r="B364">
@@ -31826,7 +31866,7 @@
       </c>
     </row>
     <row r="365" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A365" s="51">
+      <c r="A365">
         <v>175</v>
       </c>
       <c r="B365">
@@ -31875,7 +31915,7 @@
       </c>
     </row>
     <row r="366" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A366" s="51">
+      <c r="A366">
         <v>176</v>
       </c>
       <c r="B366">
@@ -31927,7 +31967,7 @@
       </c>
     </row>
     <row r="367" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A367" s="51">
+      <c r="A367">
         <v>177</v>
       </c>
       <c r="B367">
@@ -31979,7 +32019,7 @@
       </c>
     </row>
     <row r="368" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A368" s="51">
+      <c r="A368">
         <v>178</v>
       </c>
       <c r="B368">
@@ -32034,7 +32074,7 @@
       </c>
     </row>
     <row r="369" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A369" s="51">
+      <c r="A369">
         <v>179</v>
       </c>
       <c r="B369">
@@ -32089,7 +32129,7 @@
       </c>
     </row>
     <row r="370" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A370" s="51">
+      <c r="A370">
         <v>180</v>
       </c>
       <c r="B370">
@@ -32141,7 +32181,7 @@
       </c>
     </row>
     <row r="371" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A371" s="51">
+      <c r="A371">
         <v>181</v>
       </c>
       <c r="B371">
@@ -32196,7 +32236,7 @@
       </c>
     </row>
     <row r="372" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A372" s="51">
+      <c r="A372">
         <v>182</v>
       </c>
       <c r="B372">
@@ -32248,7 +32288,7 @@
       </c>
     </row>
     <row r="373" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A373" s="51">
+      <c r="A373">
         <v>183</v>
       </c>
       <c r="B373">
@@ -32298,7 +32338,7 @@
       </c>
     </row>
     <row r="374" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A374" s="51">
+      <c r="A374">
         <v>184</v>
       </c>
       <c r="B374">
@@ -32348,7 +32388,7 @@
       </c>
     </row>
     <row r="375" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A375" s="51">
+      <c r="A375">
         <v>185</v>
       </c>
       <c r="B375">
@@ -32398,7 +32438,7 @@
       </c>
     </row>
     <row r="376" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A376" s="51">
+      <c r="A376">
         <v>186</v>
       </c>
       <c r="B376">
@@ -32448,7 +32488,7 @@
       </c>
     </row>
     <row r="377" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A377" s="51">
+      <c r="A377">
         <v>187</v>
       </c>
       <c r="B377">
@@ -32498,7 +32538,7 @@
       </c>
     </row>
     <row r="378" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A378" s="51">
+      <c r="A378">
         <v>188</v>
       </c>
       <c r="B378">
@@ -32548,7 +32588,7 @@
       </c>
     </row>
     <row r="379" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A379" s="51">
+      <c r="A379">
         <v>189</v>
       </c>
       <c r="B379">
@@ -32598,7 +32638,7 @@
       </c>
     </row>
     <row r="380" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A380" s="51">
+      <c r="A380">
         <v>190</v>
       </c>
       <c r="B380">
@@ -32648,7 +32688,7 @@
       </c>
     </row>
     <row r="381" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A381" s="51">
+      <c r="A381">
         <v>191</v>
       </c>
       <c r="B381">
@@ -32698,7 +32738,7 @@
       </c>
     </row>
     <row r="382" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A382" s="51">
+      <c r="A382">
         <v>192</v>
       </c>
       <c r="B382">
@@ -32744,7 +32784,7 @@
       </c>
     </row>
     <row r="383" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A383" s="51">
+      <c r="A383">
         <v>193</v>
       </c>
       <c r="B383">
@@ -32789,7 +32829,7 @@
       </c>
     </row>
     <row r="384" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A384" s="51">
+      <c r="A384">
         <v>194</v>
       </c>
       <c r="B384">
@@ -32834,7 +32874,7 @@
       </c>
     </row>
     <row r="385" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A385" s="51">
+      <c r="A385">
         <v>195</v>
       </c>
       <c r="B385">
@@ -32879,7 +32919,7 @@
       </c>
     </row>
     <row r="386" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A386" s="51">
+      <c r="A386">
         <v>196</v>
       </c>
       <c r="B386">
@@ -32915,7 +32955,7 @@
       </c>
     </row>
     <row r="387" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A387" s="51">
+      <c r="A387">
         <v>197</v>
       </c>
       <c r="B387">
@@ -32928,22 +32968,22 @@
         <f>SUM($E387:$J387)</f>
         <v>499</v>
       </c>
-      <c r="E387" s="53">
+      <c r="E387" s="2">
         <v>115</v>
       </c>
-      <c r="F387" s="54">
+      <c r="F387" s="3">
         <v>105</v>
       </c>
-      <c r="G387" s="55">
+      <c r="G387" s="4">
         <v>55</v>
       </c>
-      <c r="H387" s="56">
+      <c r="H387" s="5">
         <v>105</v>
       </c>
-      <c r="I387" s="55">
+      <c r="I387" s="4">
         <v>60</v>
       </c>
-      <c r="J387" s="57">
+      <c r="J387" s="6">
         <v>59</v>
       </c>
       <c r="K387">
@@ -32951,7 +32991,7 @@
       </c>
     </row>
     <row r="388" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A388" s="51">
+      <c r="A388">
         <v>198</v>
       </c>
       <c r="B388">
@@ -32987,7 +33027,7 @@
       </c>
     </row>
     <row r="389" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A389" s="51">
+      <c r="A389">
         <v>199</v>
       </c>
       <c r="B389">
@@ -33000,22 +33040,22 @@
         <f>SUM($E389:$J389)</f>
         <v>525</v>
       </c>
-      <c r="E389" s="53">
+      <c r="E389" s="2">
         <v>83</v>
       </c>
-      <c r="F389" s="54">
+      <c r="F389" s="3">
         <v>55</v>
       </c>
-      <c r="G389" s="55">
+      <c r="G389" s="4">
         <v>90</v>
       </c>
-      <c r="H389" s="56">
+      <c r="H389" s="5">
         <v>130</v>
       </c>
-      <c r="I389" s="55">
+      <c r="I389" s="4">
         <v>81</v>
       </c>
-      <c r="J389" s="57">
+      <c r="J389" s="6">
         <v>86</v>
       </c>
       <c r="K389">
@@ -33023,7 +33063,7 @@
       </c>
     </row>
     <row r="390" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A390" s="51">
+      <c r="A390">
         <v>200</v>
       </c>
       <c r="B390">
@@ -33059,7 +33099,7 @@
       </c>
     </row>
     <row r="391" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A391" s="51">
+      <c r="A391">
         <v>201</v>
       </c>
       <c r="B391">
@@ -33095,7 +33135,7 @@
       </c>
     </row>
     <row r="392" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A392" s="51">
+      <c r="A392">
         <v>202</v>
       </c>
       <c r="B392">
@@ -33108,22 +33148,22 @@
         <f>SUM($E392:$J392)</f>
         <v>430</v>
       </c>
-      <c r="E392" s="59">
+      <c r="E392" s="45">
         <v>55</v>
       </c>
-      <c r="F392" s="60">
+      <c r="F392" s="46">
         <v>95</v>
       </c>
-      <c r="G392" s="61">
+      <c r="G392" s="47">
         <v>55</v>
       </c>
-      <c r="H392" s="62">
+      <c r="H392" s="48">
         <v>35</v>
       </c>
-      <c r="I392" s="61">
+      <c r="I392" s="47">
         <v>75</v>
       </c>
-      <c r="J392" s="63">
+      <c r="J392" s="49">
         <v>115</v>
       </c>
       <c r="K392">
@@ -33131,7 +33171,7 @@
       </c>
     </row>
     <row r="393" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A393" s="51">
+      <c r="A393">
         <v>203</v>
       </c>
       <c r="B393">
@@ -33167,7 +33207,7 @@
       </c>
     </row>
     <row r="394" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A394" s="51">
+      <c r="A394">
         <v>204</v>
       </c>
       <c r="B394">
@@ -33180,22 +33220,22 @@
         <f>SUM($E394:$J394)</f>
         <v>435</v>
       </c>
-      <c r="E394" s="53">
+      <c r="E394" s="2">
         <v>90</v>
       </c>
-      <c r="F394" s="54">
+      <c r="F394" s="3">
         <v>64</v>
       </c>
-      <c r="G394" s="55">
+      <c r="G394" s="4">
         <v>67</v>
       </c>
-      <c r="H394" s="56">
+      <c r="H394" s="5">
         <v>85</v>
       </c>
-      <c r="I394" s="55">
+      <c r="I394" s="4">
         <v>71</v>
       </c>
-      <c r="J394" s="57">
+      <c r="J394" s="6">
         <v>58</v>
       </c>
       <c r="K394">
@@ -33203,7 +33243,7 @@
       </c>
     </row>
     <row r="395" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A395" s="51">
+      <c r="A395">
         <v>205</v>
       </c>
       <c r="B395">
@@ -33239,7 +33279,7 @@
       </c>
     </row>
     <row r="396" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A396" s="51">
+      <c r="A396">
         <v>206</v>
       </c>
       <c r="B396">
@@ -33275,7 +33315,7 @@
       </c>
     </row>
     <row r="397" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A397" s="51">
+      <c r="A397">
         <v>207</v>
       </c>
       <c r="B397">
@@ -33311,7 +33351,7 @@
       </c>
     </row>
     <row r="398" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A398" s="51">
+      <c r="A398">
         <v>208</v>
       </c>
       <c r="B398">
@@ -33347,7 +33387,7 @@
       </c>
     </row>
     <row r="399" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A399" s="51">
+      <c r="A399">
         <v>209</v>
       </c>
       <c r="B399">
@@ -33383,7 +33423,7 @@
       </c>
     </row>
     <row r="400" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A400" s="51">
+      <c r="A400">
         <v>210</v>
       </c>
       <c r="B400">
@@ -33419,7 +33459,7 @@
       </c>
     </row>
     <row r="401" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A401" s="51">
+      <c r="A401">
         <v>211</v>
       </c>
       <c r="B401">
@@ -33455,7 +33495,7 @@
       </c>
     </row>
     <row r="402" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A402" s="51">
+      <c r="A402">
         <v>212</v>
       </c>
       <c r="B402">
@@ -33491,7 +33531,7 @@
       </c>
     </row>
     <row r="403" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A403" s="51">
+      <c r="A403">
         <v>213</v>
       </c>
       <c r="B403">
@@ -33527,7 +33567,7 @@
       </c>
     </row>
     <row r="404" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A404" s="51">
+      <c r="A404">
         <v>214</v>
       </c>
       <c r="B404">
@@ -33563,7 +33603,7 @@
       </c>
     </row>
     <row r="405" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A405" s="51">
+      <c r="A405">
         <v>215</v>
       </c>
       <c r="B405">
@@ -33599,7 +33639,7 @@
       </c>
     </row>
     <row r="406" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A406" s="51">
+      <c r="A406">
         <v>216</v>
       </c>
       <c r="B406">
@@ -33635,7 +33675,7 @@
       </c>
     </row>
     <row r="407" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A407" s="51">
+      <c r="A407">
         <v>217</v>
       </c>
       <c r="B407">
@@ -33671,7 +33711,7 @@
       </c>
     </row>
     <row r="408" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A408" s="51">
+      <c r="A408">
         <v>218</v>
       </c>
       <c r="B408">
@@ -33707,7 +33747,7 @@
       </c>
     </row>
     <row r="409" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A409" s="51">
+      <c r="A409">
         <v>219</v>
       </c>
       <c r="B409">
@@ -33743,7 +33783,7 @@
       </c>
     </row>
     <row r="410" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A410" s="51">
+      <c r="A410">
         <v>220</v>
       </c>
       <c r="B410">
@@ -33785,7 +33825,7 @@
       </c>
     </row>
     <row r="411" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A411" s="51">
+      <c r="A411">
         <v>221</v>
       </c>
       <c r="B411">
@@ -33806,7 +33846,7 @@
       </c>
     </row>
     <row r="412" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A412" s="51">
+      <c r="A412">
         <v>222</v>
       </c>
       <c r="B412">
@@ -33821,7 +33861,7 @@
       </c>
     </row>
     <row r="413" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A413" s="51">
+      <c r="A413">
         <v>223</v>
       </c>
       <c r="B413">
@@ -33857,7 +33897,7 @@
       </c>
     </row>
     <row r="414" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A414" s="51">
+      <c r="A414">
         <v>224</v>
       </c>
       <c r="B414">
@@ -33893,7 +33933,7 @@
       </c>
     </row>
     <row r="415" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A415" s="51">
+      <c r="A415">
         <v>225</v>
       </c>
       <c r="B415">
@@ -33929,7 +33969,7 @@
       </c>
     </row>
     <row r="416" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A416" s="51">
+      <c r="A416">
         <v>226</v>
       </c>
       <c r="B416">
@@ -33965,7 +34005,7 @@
       </c>
     </row>
     <row r="417" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A417" s="51">
+      <c r="A417">
         <v>227</v>
       </c>
       <c r="B417">
@@ -34001,7 +34041,7 @@
       </c>
     </row>
     <row r="418" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A418" s="51">
+      <c r="A418">
         <v>228</v>
       </c>
       <c r="B418">
@@ -34040,7 +34080,7 @@
       </c>
     </row>
     <row r="419" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A419" s="51">
+      <c r="A419">
         <v>229</v>
       </c>
       <c r="B419">
@@ -34076,7 +34116,7 @@
       </c>
     </row>
     <row r="420" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A420" s="51">
+      <c r="A420">
         <v>230</v>
       </c>
       <c r="B420">
@@ -34112,7 +34152,7 @@
       </c>
     </row>
     <row r="421" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A421" s="51">
+      <c r="A421">
         <v>231</v>
       </c>
       <c r="B421">
@@ -34148,7 +34188,7 @@
       </c>
     </row>
     <row r="422" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A422" s="51">
+      <c r="A422">
         <v>232</v>
       </c>
       <c r="B422">
@@ -34187,7 +34227,7 @@
       </c>
     </row>
     <row r="423" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A423" s="51">
+      <c r="A423">
         <v>233</v>
       </c>
       <c r="B423">
@@ -34232,7 +34272,7 @@
       </c>
     </row>
     <row r="424" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A424" s="51">
+      <c r="A424">
         <v>234</v>
       </c>
       <c r="B424">
@@ -34277,7 +34317,7 @@
       </c>
     </row>
     <row r="425" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A425" s="51">
+      <c r="A425">
         <v>235</v>
       </c>
       <c r="B425">
@@ -34307,7 +34347,7 @@
       </c>
     </row>
     <row r="426" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A426" s="51">
+      <c r="A426">
         <v>236</v>
       </c>
       <c r="B426">
@@ -34334,7 +34374,7 @@
       </c>
     </row>
     <row r="427" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A427" s="51">
+      <c r="A427">
         <v>237</v>
       </c>
       <c r="B427">
@@ -34361,7 +34401,7 @@
       </c>
     </row>
     <row r="428" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A428" s="51">
+      <c r="A428">
         <v>238</v>
       </c>
       <c r="B428">
@@ -34391,7 +34431,7 @@
       </c>
     </row>
     <row r="429" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A429" s="51">
+      <c r="A429">
         <v>239</v>
       </c>
       <c r="B429">
@@ -34409,7 +34449,7 @@
       </c>
     </row>
     <row r="430" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A430" s="51">
+      <c r="A430">
         <v>240</v>
       </c>
       <c r="B430">
@@ -34445,7 +34485,7 @@
       </c>
     </row>
     <row r="431" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A431" s="51">
+      <c r="A431">
         <v>241</v>
       </c>
       <c r="B431">
@@ -34481,7 +34521,7 @@
       </c>
     </row>
     <row r="432" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A432" s="51">
+      <c r="A432">
         <v>242</v>
       </c>
       <c r="B432">
@@ -34517,7 +34557,7 @@
       </c>
     </row>
     <row r="433" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A433" s="51">
+      <c r="A433">
         <v>243</v>
       </c>
       <c r="B433">
@@ -34553,7 +34593,7 @@
       </c>
     </row>
     <row r="434" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A434" s="51">
+      <c r="A434">
         <v>244</v>
       </c>
       <c r="B434">
@@ -34589,7 +34629,7 @@
       </c>
     </row>
     <row r="435" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A435" s="51">
+      <c r="A435">
         <v>245</v>
       </c>
       <c r="B435">
@@ -34625,7 +34665,7 @@
       </c>
     </row>
     <row r="436" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A436" s="51">
+      <c r="A436">
         <v>246</v>
       </c>
       <c r="B436">
@@ -34661,7 +34701,7 @@
       </c>
     </row>
     <row r="437" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A437" s="51">
+      <c r="A437">
         <v>247</v>
       </c>
       <c r="B437">
@@ -34670,7 +34710,7 @@
       <c r="C437" t="s">
         <v>570</v>
       </c>
-      <c r="D437" s="52">
+      <c r="D437" s="1">
         <f>SUM($E437:$J437)</f>
         <v>700</v>
       </c>
@@ -34706,7 +34746,7 @@
       </c>
     </row>
     <row r="438" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A438" s="51">
+      <c r="A438">
         <v>248</v>
       </c>
       <c r="B438">
@@ -34715,7 +34755,7 @@
       <c r="C438" t="s">
         <v>1198</v>
       </c>
-      <c r="D438" s="52">
+      <c r="D438" s="1">
         <f>SUM($E438:$J438)</f>
         <v>680</v>
       </c>
@@ -34751,7 +34791,7 @@
       </c>
     </row>
     <row r="439" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A439" s="51">
+      <c r="A439">
         <v>249</v>
       </c>
       <c r="B439">
@@ -34760,7 +34800,7 @@
       <c r="C439" t="s">
         <v>571</v>
       </c>
-      <c r="D439" s="52">
+      <c r="D439" s="1">
         <f>SUM($E439:$J439)</f>
         <v>670</v>
       </c>
@@ -34799,41 +34839,41 @@
       <c r="B440">
         <v>237</v>
       </c>
-      <c r="C440" s="51" t="s">
+      <c r="C440" t="s">
         <v>576</v>
       </c>
-      <c r="D440" s="52">
+      <c r="D440" s="1">
         <f>SUM($E440:$J440)</f>
         <v>550</v>
       </c>
-      <c r="E440" s="46">
+      <c r="E440" s="2">
         <v>110</v>
       </c>
-      <c r="F440" s="47">
+      <c r="F440" s="3">
         <v>100</v>
       </c>
-      <c r="G440" s="48">
+      <c r="G440" s="4">
         <v>75</v>
       </c>
-      <c r="H440" s="49">
+      <c r="H440" s="5">
         <v>100</v>
       </c>
-      <c r="I440" s="48">
+      <c r="I440" s="4">
         <v>75</v>
       </c>
-      <c r="J440" s="50">
+      <c r="J440" s="6">
         <v>90</v>
       </c>
-      <c r="K440" s="45">
+      <c r="K440">
         <v>550</v>
       </c>
-      <c r="L440" s="45" t="s">
+      <c r="L440" t="s">
         <v>661</v>
       </c>
-      <c r="M440" s="45" t="s">
+      <c r="M440" t="s">
         <v>1223</v>
       </c>
-      <c r="N440" s="45" t="s">
+      <c r="N440" t="s">
         <v>1148</v>
       </c>
     </row>
@@ -34841,41 +34881,41 @@
       <c r="B441">
         <v>291</v>
       </c>
-      <c r="C441" s="51" t="s">
+      <c r="C441" t="s">
         <v>1199</v>
       </c>
-      <c r="D441" s="52">
+      <c r="D441" s="1">
         <f>SUM($E441:$J441)</f>
         <v>754</v>
       </c>
-      <c r="E441" s="46">
+      <c r="E441" s="2">
         <v>97</v>
       </c>
-      <c r="F441" s="47">
+      <c r="F441" s="3">
         <v>147</v>
       </c>
-      <c r="G441" s="48">
+      <c r="G441" s="4">
         <v>97</v>
       </c>
-      <c r="H441" s="49">
+      <c r="H441" s="5">
         <v>187</v>
       </c>
-      <c r="I441" s="48">
+      <c r="I441" s="4">
         <v>97</v>
       </c>
-      <c r="J441" s="50">
+      <c r="J441" s="6">
         <v>129</v>
       </c>
-      <c r="K441" s="45">
+      <c r="K441">
         <v>754</v>
       </c>
-      <c r="L441" s="45" t="s">
+      <c r="L441" t="s">
         <v>661</v>
       </c>
-      <c r="M441" s="45" t="s">
+      <c r="M441" t="s">
         <v>1224</v>
       </c>
-      <c r="N441" s="45" t="s">
+      <c r="N441" t="s">
         <v>1148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug fixes and moveset/tm learnset implementations
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8324F6-77A0-4063-879C-8D69ABD4B276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD27B472-5558-4534-BD7A-33009B5BB83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="28680" yWindow="-12510" windowWidth="16440" windowHeight="28440" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4728,13 +4729,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AU620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI59" sqref="AI59"/>
+    <sheetView tabSelected="1" topLeftCell="A374" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G413" sqref="G413"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
     <col min="6" max="6" width="11" style="3" customWidth="1"/>
@@ -4744,21 +4745,21 @@
     <col min="10" max="10" width="11" style="6" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
     <col min="21" max="21" width="17" customWidth="1"/>
     <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="26" max="26" width="6.6640625" customWidth="1"/>
-    <col min="27" max="29" width="10.88671875" customWidth="1"/>
-    <col min="30" max="32" width="7.6640625" customWidth="1"/>
-    <col min="33" max="33" width="11.44140625" customWidth="1"/>
-    <col min="34" max="47" width="7.6640625" customWidth="1"/>
+    <col min="26" max="26" width="6.7109375" customWidth="1"/>
+    <col min="27" max="29" width="10.85546875" customWidth="1"/>
+    <col min="30" max="32" width="7.7109375" customWidth="1"/>
+    <col min="33" max="33" width="11.42578125" customWidth="1"/>
+    <col min="34" max="47" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>-1</v>
       </c>
@@ -4876,7 +4877,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>-2</v>
       </c>
@@ -4944,7 +4945,7 @@
       <c r="AR2" s="18"/>
       <c r="AT2" s="17"/>
     </row>
-    <row r="3" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>-3</v>
       </c>
@@ -5017,7 +5018,7 @@
       <c r="AR3" s="17"/>
       <c r="AU3" s="19"/>
     </row>
-    <row r="4" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>-4</v>
       </c>
@@ -5085,7 +5086,7 @@
       <c r="AN4" s="17"/>
       <c r="AP4" s="18"/>
     </row>
-    <row r="5" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>-5</v>
       </c>
@@ -5158,7 +5159,7 @@
       <c r="AS5" s="17"/>
       <c r="AU5" s="18"/>
     </row>
-    <row r="6" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>-6</v>
       </c>
@@ -5225,7 +5226,7 @@
       <c r="AP6" s="18"/>
       <c r="AR6" s="17"/>
     </row>
-    <row r="7" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>-7</v>
       </c>
@@ -5292,7 +5293,7 @@
       <c r="AP7" s="17"/>
       <c r="AR7" s="18"/>
     </row>
-    <row r="8" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>-8</v>
       </c>
@@ -5363,7 +5364,7 @@
       <c r="AT8" s="18"/>
       <c r="AU8" s="18"/>
     </row>
-    <row r="9" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>-9</v>
       </c>
@@ -5432,7 +5433,7 @@
       <c r="AR9" s="19"/>
       <c r="AT9" s="17"/>
     </row>
-    <row r="10" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>-10</v>
       </c>
@@ -5496,7 +5497,7 @@
       <c r="AR10" s="17"/>
       <c r="AU10" s="18"/>
     </row>
-    <row r="11" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>-11</v>
       </c>
@@ -5557,7 +5558,7 @@
       <c r="AR11" s="18"/>
       <c r="AU11" s="17"/>
     </row>
-    <row r="12" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>-12</v>
       </c>
@@ -5617,7 +5618,7 @@
       <c r="AQ12" s="19"/>
       <c r="AT12" s="18"/>
     </row>
-    <row r="13" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>-13</v>
       </c>
@@ -5683,7 +5684,7 @@
       <c r="AS13" s="17"/>
       <c r="AU13" s="18"/>
     </row>
-    <row r="14" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>-14</v>
       </c>
@@ -5740,7 +5741,7 @@
       <c r="AR14" s="18"/>
       <c r="AU14" s="17"/>
     </row>
-    <row r="15" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>-15</v>
       </c>
@@ -5795,7 +5796,7 @@
       <c r="AQ15" s="18"/>
       <c r="AS15" s="18"/>
     </row>
-    <row r="16" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>-16</v>
       </c>
@@ -5847,7 +5848,7 @@
       <c r="AR16" s="18"/>
       <c r="AT16" s="19"/>
     </row>
-    <row r="17" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>-17</v>
       </c>
@@ -5907,7 +5908,7 @@
       <c r="AQ17" s="18"/>
       <c r="AS17" s="18"/>
     </row>
-    <row r="18" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>-18</v>
       </c>
@@ -5973,7 +5974,7 @@
       <c r="AS18" s="17"/>
       <c r="AT18" s="18"/>
     </row>
-    <row r="19" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>-19</v>
       </c>
@@ -6037,7 +6038,7 @@
       <c r="AS19" s="18"/>
       <c r="AU19" s="17"/>
     </row>
-    <row r="20" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>-20</v>
       </c>
@@ -6098,7 +6099,7 @@
       <c r="AR20" s="17"/>
       <c r="AT20" s="18"/>
     </row>
-    <row r="21" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>-21</v>
       </c>
@@ -6151,7 +6152,7 @@
       <c r="AR21" s="18"/>
       <c r="AS21" s="18"/>
     </row>
-    <row r="22" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>-22</v>
       </c>
@@ -6200,7 +6201,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>-23</v>
       </c>
@@ -6248,7 +6249,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>-24</v>
       </c>
@@ -6296,7 +6297,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>-25</v>
       </c>
@@ -6344,7 +6345,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>-26</v>
       </c>
@@ -6389,7 +6390,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>-27</v>
       </c>
@@ -6434,7 +6435,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>-28</v>
       </c>
@@ -6479,7 +6480,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>-29</v>
       </c>
@@ -6551,7 +6552,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="30" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>-30</v>
       </c>
@@ -6618,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>-31</v>
       </c>
@@ -6685,7 +6686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>-32</v>
       </c>
@@ -6758,7 +6759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>-33</v>
       </c>
@@ -6840,7 +6841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>-34</v>
       </c>
@@ -6919,7 +6920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>-35</v>
       </c>
@@ -6998,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>-36</v>
       </c>
@@ -7077,7 +7078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>-37</v>
       </c>
@@ -7153,7 +7154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>-38</v>
       </c>
@@ -7229,7 +7230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>-39</v>
       </c>
@@ -7305,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>-40</v>
       </c>
@@ -7381,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>-41</v>
       </c>
@@ -7454,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>-42</v>
       </c>
@@ -7527,7 +7528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>-43</v>
       </c>
@@ -7603,7 +7604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>-44</v>
       </c>
@@ -7676,7 +7677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>-45</v>
       </c>
@@ -7746,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>-46</v>
       </c>
@@ -7813,7 +7814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>-47</v>
       </c>
@@ -7880,7 +7881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>-48</v>
       </c>
@@ -7947,7 +7948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>-49</v>
       </c>
@@ -8011,7 +8012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>-50</v>
       </c>
@@ -8078,7 +8079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>-51</v>
       </c>
@@ -8142,7 +8143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>-52</v>
       </c>
@@ -8206,7 +8207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>-53</v>
       </c>
@@ -8270,7 +8271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>-54</v>
       </c>
@@ -8358,7 +8359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>-55</v>
       </c>
@@ -8446,7 +8447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>-56</v>
       </c>
@@ -8534,7 +8535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>-57</v>
       </c>
@@ -8625,7 +8626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>-58</v>
       </c>
@@ -8713,7 +8714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>-59</v>
       </c>
@@ -8801,7 +8802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>-60</v>
       </c>
@@ -8892,7 +8893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>-61</v>
       </c>
@@ -8980,7 +8981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>-62</v>
       </c>
@@ -9068,7 +9069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>-63</v>
       </c>
@@ -9156,7 +9157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>-64</v>
       </c>
@@ -9244,7 +9245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>-65</v>
       </c>
@@ -9332,7 +9333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>-66</v>
       </c>
@@ -9420,7 +9421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>-67</v>
       </c>
@@ -9508,7 +9509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>-68</v>
       </c>
@@ -9596,7 +9597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>-69</v>
       </c>
@@ -9684,7 +9685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>-70</v>
       </c>
@@ -9772,7 +9773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>-71</v>
       </c>
@@ -9860,7 +9861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>-72</v>
       </c>
@@ -9948,7 +9949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>-73</v>
       </c>
@@ -10036,7 +10037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>-74</v>
       </c>
@@ -10124,7 +10125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>-75</v>
       </c>
@@ -10219,7 +10220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>-76</v>
       </c>
@@ -10283,7 +10284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>-77</v>
       </c>
@@ -10347,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>-78</v>
       </c>
@@ -10411,7 +10412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>-79</v>
       </c>
@@ -10475,7 +10476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>-80</v>
       </c>
@@ -10539,7 +10540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>-81</v>
       </c>
@@ -10603,7 +10604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>-82</v>
       </c>
@@ -10667,7 +10668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>-83</v>
       </c>
@@ -10731,7 +10732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>-84</v>
       </c>
@@ -10795,7 +10796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>-85</v>
       </c>
@@ -10862,7 +10863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>-86</v>
       </c>
@@ -10926,7 +10927,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="87" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>-87</v>
       </c>
@@ -10990,7 +10991,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="88" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>-88</v>
       </c>
@@ -11054,7 +11055,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="89" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>-89</v>
       </c>
@@ -11118,7 +11119,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="90" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>-90</v>
       </c>
@@ -11182,7 +11183,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="91" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>-91</v>
       </c>
@@ -11246,7 +11247,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="92" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>-92</v>
       </c>
@@ -11310,7 +11311,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="93" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>-93</v>
       </c>
@@ -11374,7 +11375,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="94" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>-94</v>
       </c>
@@ -11438,7 +11439,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="95" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>-95</v>
       </c>
@@ -11502,7 +11503,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="96" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>-96</v>
       </c>
@@ -11566,7 +11567,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="97" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>-97</v>
       </c>
@@ -11630,7 +11631,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="98" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>-98</v>
       </c>
@@ -11694,7 +11695,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="99" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>-99</v>
       </c>
@@ -11758,7 +11759,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="100" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>-100</v>
       </c>
@@ -11822,7 +11823,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="101" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>-101</v>
       </c>
@@ -11886,7 +11887,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="102" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>-102</v>
       </c>
@@ -11950,7 +11951,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="103" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>-103</v>
       </c>
@@ -12017,7 +12018,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="104" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>-104</v>
       </c>
@@ -12081,7 +12082,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="105" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>-105</v>
       </c>
@@ -12145,7 +12146,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="106" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>-106</v>
       </c>
@@ -12209,7 +12210,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="107" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>-107</v>
       </c>
@@ -12273,7 +12274,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="108" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>-108</v>
       </c>
@@ -12337,7 +12338,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="109" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>-109</v>
       </c>
@@ -12401,7 +12402,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="110" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>-110</v>
       </c>
@@ -12465,7 +12466,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="111" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>-111</v>
       </c>
@@ -12529,7 +12530,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="112" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>-112</v>
       </c>
@@ -12593,7 +12594,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="113" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>-113</v>
       </c>
@@ -12657,7 +12658,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="114" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>-114</v>
       </c>
@@ -12721,7 +12722,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="115" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>-115</v>
       </c>
@@ -12785,7 +12786,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="116" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>-116</v>
       </c>
@@ -12849,7 +12850,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="117" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>-117</v>
       </c>
@@ -12913,7 +12914,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="118" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>-118</v>
       </c>
@@ -12977,7 +12978,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="119" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>-119</v>
       </c>
@@ -13041,7 +13042,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="120" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>-120</v>
       </c>
@@ -13105,7 +13106,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="121" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>-121</v>
       </c>
@@ -13169,7 +13170,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="122" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>-122</v>
       </c>
@@ -13233,7 +13234,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="123" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>-123</v>
       </c>
@@ -13297,7 +13298,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="124" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>-124</v>
       </c>
@@ -13361,7 +13362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>-125</v>
       </c>
@@ -13425,7 +13426,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="126" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>-126</v>
       </c>
@@ -13489,7 +13490,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="127" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>-127</v>
       </c>
@@ -13553,7 +13554,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="128" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>-128</v>
       </c>
@@ -13617,7 +13618,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="129" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>-129</v>
       </c>
@@ -13681,7 +13682,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="130" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>-130</v>
       </c>
@@ -13745,7 +13746,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="131" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>-131</v>
       </c>
@@ -13809,7 +13810,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="132" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B132">
         <v>-132</v>
       </c>
@@ -13873,7 +13874,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="133" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B133">
         <v>-133</v>
       </c>
@@ -13937,7 +13938,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="134" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B134">
         <v>-134</v>
       </c>
@@ -14001,7 +14002,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="135" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B135">
         <v>-135</v>
       </c>
@@ -14065,7 +14066,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="136" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B136">
         <v>-136</v>
       </c>
@@ -14129,7 +14130,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="137" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B137">
         <v>-137</v>
       </c>
@@ -14193,7 +14194,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="138" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B138">
         <v>-138</v>
       </c>
@@ -14260,7 +14261,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="139" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B139">
         <v>-139</v>
       </c>
@@ -14324,7 +14325,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="140" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B140">
         <v>-140</v>
       </c>
@@ -14388,7 +14389,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="141" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B141">
         <v>-141</v>
       </c>
@@ -14459,7 +14460,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="142" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B142">
         <v>-142</v>
       </c>
@@ -14533,7 +14534,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="143" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B143">
         <v>-143</v>
       </c>
@@ -14604,7 +14605,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="144" spans="2:35" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B144">
         <v>-144</v>
       </c>
@@ -14687,7 +14688,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>1218</v>
       </c>
@@ -14763,7 +14764,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1</v>
       </c>
@@ -14864,7 +14865,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2</v>
       </c>
@@ -14962,7 +14963,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>3</v>
       </c>
@@ -15060,7 +15061,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>4</v>
       </c>
@@ -15158,7 +15159,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>5</v>
       </c>
@@ -15256,7 +15257,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>6</v>
       </c>
@@ -15351,7 +15352,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>7</v>
       </c>
@@ -15452,7 +15453,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>8</v>
       </c>
@@ -15550,7 +15551,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>9</v>
       </c>
@@ -15645,7 +15646,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>13</v>
       </c>
@@ -15743,7 +15744,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>14</v>
       </c>
@@ -15841,7 +15842,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>15</v>
       </c>
@@ -15939,7 +15940,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>10</v>
       </c>
@@ -16037,7 +16038,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>11</v>
       </c>
@@ -16135,7 +16136,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>12</v>
       </c>
@@ -16230,7 +16231,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>16</v>
       </c>
@@ -16328,7 +16329,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>17</v>
       </c>
@@ -16426,7 +16427,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>18</v>
       </c>
@@ -16524,7 +16525,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>41</v>
       </c>
@@ -16625,7 +16626,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>42</v>
       </c>
@@ -16723,7 +16724,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>43</v>
       </c>
@@ -16818,7 +16819,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>19</v>
       </c>
@@ -16914,7 +16915,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>20</v>
       </c>
@@ -17010,7 +17011,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="169" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>21</v>
       </c>
@@ -17105,7 +17106,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>22</v>
       </c>
@@ -17203,7 +17204,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>26</v>
       </c>
@@ -17299,7 +17300,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>27</v>
       </c>
@@ -17395,7 +17396,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>28</v>
       </c>
@@ -17485,7 +17486,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>29</v>
       </c>
@@ -17580,7 +17581,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>30</v>
       </c>
@@ -17675,7 +17676,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>31</v>
       </c>
@@ -17767,7 +17768,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>32</v>
       </c>
@@ -17860,7 +17861,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>33</v>
       </c>
@@ -17953,7 +17954,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>34</v>
       </c>
@@ -18043,7 +18044,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>122</v>
       </c>
@@ -18136,7 +18137,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="181" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>123</v>
       </c>
@@ -18229,7 +18230,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>124</v>
       </c>
@@ -18319,7 +18320,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>38</v>
       </c>
@@ -18411,7 +18412,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="184" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>39</v>
       </c>
@@ -18509,7 +18510,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>40</v>
       </c>
@@ -18604,7 +18605,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>35</v>
       </c>
@@ -18699,7 +18700,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>36</v>
       </c>
@@ -18794,7 +18795,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>37</v>
       </c>
@@ -18886,7 +18887,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>60</v>
       </c>
@@ -18979,7 +18980,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>61</v>
       </c>
@@ -19072,7 +19073,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="191" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>62</v>
       </c>
@@ -19162,7 +19163,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>129</v>
       </c>
@@ -19248,7 +19249,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>125</v>
       </c>
@@ -19337,7 +19338,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>126</v>
       </c>
@@ -19432,7 +19433,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="195" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>127</v>
       </c>
@@ -19524,7 +19525,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>128</v>
       </c>
@@ -19619,7 +19620,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>107</v>
       </c>
@@ -19714,7 +19715,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>108</v>
       </c>
@@ -19809,7 +19810,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>109</v>
       </c>
@@ -19901,7 +19902,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>130</v>
       </c>
@@ -19996,7 +19997,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="201" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>131</v>
       </c>
@@ -20088,7 +20089,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="202" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>180</v>
       </c>
@@ -20180,7 +20181,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>181</v>
       </c>
@@ -20269,7 +20270,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>84</v>
       </c>
@@ -20361,7 +20362,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>85</v>
       </c>
@@ -20450,7 +20451,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="206" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
@@ -20539,7 +20540,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>162</v>
       </c>
@@ -20631,7 +20632,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="208" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>163</v>
       </c>
@@ -20717,7 +20718,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="209" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>205</v>
       </c>
@@ -20804,7 +20805,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="210" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>206</v>
       </c>
@@ -20888,7 +20889,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="211" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>207</v>
       </c>
@@ -20977,7 +20978,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>208</v>
       </c>
@@ -21063,7 +21064,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="213" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>186</v>
       </c>
@@ -21152,7 +21153,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="214" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>187</v>
       </c>
@@ -21241,7 +21242,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="215" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>188</v>
       </c>
@@ -21327,7 +21328,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="216" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>81</v>
       </c>
@@ -21416,7 +21417,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="217" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>82</v>
       </c>
@@ -21502,7 +21503,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="218" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>94</v>
       </c>
@@ -21594,7 +21595,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="219" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>95</v>
       </c>
@@ -21683,7 +21684,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="220" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>49</v>
       </c>
@@ -21772,7 +21773,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="221" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>50</v>
       </c>
@@ -21861,7 +21862,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="222" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>51</v>
       </c>
@@ -21947,7 +21948,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="223" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>189</v>
       </c>
@@ -22039,7 +22040,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="224" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>190</v>
       </c>
@@ -22125,7 +22126,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="225" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>178</v>
       </c>
@@ -22214,7 +22215,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>179</v>
       </c>
@@ -22300,7 +22301,7 @@
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="227" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>132</v>
       </c>
@@ -22386,7 +22387,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>133</v>
       </c>
@@ -22475,7 +22476,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="229" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>134</v>
       </c>
@@ -22576,7 +22577,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>63</v>
       </c>
@@ -22674,7 +22675,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="231" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>64</v>
       </c>
@@ -22772,7 +22773,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>65</v>
       </c>
@@ -22867,7 +22868,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="233" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>66</v>
       </c>
@@ -22965,7 +22966,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>83</v>
       </c>
@@ -23060,7 +23061,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="235" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>137</v>
       </c>
@@ -23158,7 +23159,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>138</v>
       </c>
@@ -23253,7 +23254,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>52</v>
       </c>
@@ -23351,7 +23352,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>53</v>
       </c>
@@ -23446,7 +23447,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="239" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>54</v>
       </c>
@@ -23544,7 +23545,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="240" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>55</v>
       </c>
@@ -23642,7 +23643,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="241" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>56</v>
       </c>
@@ -23737,7 +23738,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="242" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>191</v>
       </c>
@@ -23829,7 +23830,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>209</v>
       </c>
@@ -23923,7 +23924,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="244" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>210</v>
       </c>
@@ -24016,7 +24017,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="245" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>211</v>
       </c>
@@ -24106,7 +24107,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="246" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>101</v>
       </c>
@@ -24201,7 +24202,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="247" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>102</v>
       </c>
@@ -24296,7 +24297,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="248" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>103</v>
       </c>
@@ -24388,7 +24389,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>96</v>
       </c>
@@ -24486,7 +24487,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>97</v>
       </c>
@@ -24581,7 +24582,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="251" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>92</v>
       </c>
@@ -24676,7 +24677,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>93</v>
       </c>
@@ -24768,7 +24769,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>110</v>
       </c>
@@ -24852,7 +24853,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="254" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>111</v>
       </c>
@@ -24942,7 +24943,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="255" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>112</v>
       </c>
@@ -25035,7 +25036,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="256" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>164</v>
       </c>
@@ -25130,7 +25131,7 @@
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="257" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>165</v>
       </c>
@@ -25225,7 +25226,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="258" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>166</v>
       </c>
@@ -25317,7 +25318,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="259" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>139</v>
       </c>
@@ -25412,7 +25413,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="260" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>140</v>
       </c>
@@ -25507,7 +25508,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="261" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>141</v>
       </c>
@@ -25599,7 +25600,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="262" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>151</v>
       </c>
@@ -25694,7 +25695,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="263" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>152</v>
       </c>
@@ -25789,7 +25790,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="264" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>153</v>
       </c>
@@ -25884,7 +25885,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="265" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>142</v>
       </c>
@@ -25980,7 +25981,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="266" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>143</v>
       </c>
@@ -26076,7 +26077,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="267" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>144</v>
       </c>
@@ -26169,7 +26170,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="268" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>145</v>
       </c>
@@ -26262,7 +26263,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="269" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>146</v>
       </c>
@@ -26355,7 +26356,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="270" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>147</v>
       </c>
@@ -26448,7 +26449,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="271" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>148</v>
       </c>
@@ -26544,7 +26545,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="272" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>149</v>
       </c>
@@ -26628,7 +26629,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="273" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>150</v>
       </c>
@@ -26709,7 +26710,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="274" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>78</v>
       </c>
@@ -26793,7 +26794,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="275" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>79</v>
       </c>
@@ -26874,7 +26875,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="276" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>80</v>
       </c>
@@ -26964,7 +26965,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="277" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>192</v>
       </c>
@@ -27057,7 +27058,7 @@
         <v>5.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="278" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>193</v>
       </c>
@@ -27147,7 +27148,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="279" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>154</v>
       </c>
@@ -27240,7 +27241,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="280" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>155</v>
       </c>
@@ -27330,7 +27331,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="281" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>156</v>
       </c>
@@ -27420,7 +27421,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="282" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>167</v>
       </c>
@@ -27513,7 +27514,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="283" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>168</v>
       </c>
@@ -27603,7 +27604,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="284" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>182</v>
       </c>
@@ -27695,7 +27696,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="285" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>183</v>
       </c>
@@ -27784,7 +27785,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="286" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>212</v>
       </c>
@@ -27858,7 +27859,7 @@
         <v>0.22</v>
       </c>
       <c r="AD286" s="37">
-        <f t="shared" ref="AD286:AD349" si="18">AC286*AB286</f>
+        <f t="shared" ref="AD286:AD325" si="18">AC286*AB286</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="AF286">
@@ -27874,7 +27875,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="287" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>213</v>
       </c>
@@ -27961,7 +27962,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="288" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>159</v>
       </c>
@@ -28051,7 +28052,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="289" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>160</v>
       </c>
@@ -28141,7 +28142,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="290" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>161</v>
       </c>
@@ -28228,7 +28229,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="291" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>174</v>
       </c>
@@ -28318,7 +28319,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="292" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>175</v>
       </c>
@@ -28405,7 +28406,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="293" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>176</v>
       </c>
@@ -28495,7 +28496,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="294" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>177</v>
       </c>
@@ -28582,7 +28583,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="295" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>217</v>
       </c>
@@ -28669,7 +28670,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="296" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>44</v>
       </c>
@@ -28764,7 +28765,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="297" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>45</v>
       </c>
@@ -28856,7 +28857,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="298" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>119</v>
       </c>
@@ -28951,7 +28952,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="299" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>120</v>
       </c>
@@ -29046,7 +29047,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="300" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>121</v>
       </c>
@@ -29138,7 +29139,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="301" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>194</v>
       </c>
@@ -29233,7 +29234,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="302" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>195</v>
       </c>
@@ -29325,7 +29326,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="303" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>196</v>
       </c>
@@ -29420,7 +29421,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="304" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>197</v>
       </c>
@@ -29512,7 +29513,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="305" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>169</v>
       </c>
@@ -29602,7 +29603,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="306" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>170</v>
       </c>
@@ -29692,7 +29693,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="307" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>171</v>
       </c>
@@ -29782,7 +29783,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="308" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>72</v>
       </c>
@@ -29872,7 +29873,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="309" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>73</v>
       </c>
@@ -29962,7 +29963,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="310" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>74</v>
       </c>
@@ -30049,7 +30050,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="311" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>75</v>
       </c>
@@ -30141,7 +30142,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="312" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>76</v>
       </c>
@@ -30233,7 +30234,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="313" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>77</v>
       </c>
@@ -30322,7 +30323,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="314" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>115</v>
       </c>
@@ -30414,7 +30415,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="315" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>116</v>
       </c>
@@ -30503,7 +30504,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="316" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>69</v>
       </c>
@@ -30595,7 +30596,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="317" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>70</v>
       </c>
@@ -30687,7 +30688,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="318" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>71</v>
       </c>
@@ -30776,7 +30777,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="319" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>57</v>
       </c>
@@ -30866,7 +30867,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="320" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>58</v>
       </c>
@@ -30956,7 +30957,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="321" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>59</v>
       </c>
@@ -31043,7 +31044,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="322" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>67</v>
       </c>
@@ -31133,7 +31134,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="323" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>68</v>
       </c>
@@ -31220,7 +31221,7 @@
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="324" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>117</v>
       </c>
@@ -31310,7 +31311,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="325" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>118</v>
       </c>
@@ -31397,7 +31398,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="326" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>214</v>
       </c>
@@ -31458,7 +31459,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="327" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>215</v>
       </c>
@@ -31522,7 +31523,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="328" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>216</v>
       </c>
@@ -31586,7 +31587,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="329" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>228</v>
       </c>
@@ -31645,7 +31646,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="330" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>229</v>
       </c>
@@ -31704,7 +31705,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="331" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>230</v>
       </c>
@@ -31763,7 +31764,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="332" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>231</v>
       </c>
@@ -31825,7 +31826,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="333" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>232</v>
       </c>
@@ -31887,7 +31888,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="334" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>233</v>
       </c>
@@ -31943,7 +31944,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="335" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>225</v>
       </c>
@@ -31998,7 +31999,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="336" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>226</v>
       </c>
@@ -32053,7 +32054,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="337" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>227</v>
       </c>
@@ -32105,7 +32106,7 @@
         <v>Galactasolder</v>
       </c>
     </row>
-    <row r="338" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>218</v>
       </c>
@@ -32160,7 +32161,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="339" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>219</v>
       </c>
@@ -32212,7 +32213,7 @@
         <v>Cosmocrash</v>
       </c>
     </row>
-    <row r="340" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>223</v>
       </c>
@@ -32267,7 +32268,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="341" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>224</v>
       </c>
@@ -32319,7 +32320,7 @@
         <v>Stellarock</v>
       </c>
     </row>
-    <row r="342" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A342" s="10">
         <v>-10</v>
       </c>
@@ -32374,7 +32375,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="343" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A343" s="10">
         <v>-11</v>
       </c>
@@ -32426,7 +32427,7 @@
         <v>Hast-E</v>
       </c>
     </row>
-    <row r="344" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A344" s="10">
         <v>-7</v>
       </c>
@@ -32481,7 +32482,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="345" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A345" s="10">
         <v>-8</v>
       </c>
@@ -32536,7 +32537,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="346" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A346" s="10">
         <v>-9</v>
       </c>
@@ -32588,7 +32589,7 @@
         <v>Soldrota-E</v>
       </c>
     </row>
-    <row r="347" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A347" s="10">
         <v>-14</v>
       </c>
@@ -32641,7 +32642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="348" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A348" s="10">
         <v>-15</v>
       </c>
@@ -32694,7 +32695,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="349" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A349" s="10">
         <v>-16</v>
       </c>
@@ -32744,7 +32745,7 @@
         <v>Blastflames-E</v>
       </c>
     </row>
-    <row r="350" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A350" s="10">
         <v>-1</v>
       </c>
@@ -32797,7 +32798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="351" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A351" s="10">
         <v>-2</v>
       </c>
@@ -32850,7 +32851,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="352" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A352" s="10">
         <v>-3</v>
       </c>
@@ -32900,7 +32901,7 @@
         <v>Blaster-E</v>
       </c>
     </row>
-    <row r="353" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A353" s="10">
         <v>-4</v>
       </c>
@@ -32953,7 +32954,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="354" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A354" s="10">
         <v>-5</v>
       </c>
@@ -33006,7 +33007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="355" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A355" s="10">
         <v>-6</v>
       </c>
@@ -33059,7 +33060,7 @@
         <v>Gyarados-E</v>
       </c>
     </row>
-    <row r="356" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A356" s="10">
         <v>-17</v>
       </c>
@@ -33111,7 +33112,7 @@
         <v>Shockfang</v>
       </c>
     </row>
-    <row r="357" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A357" s="10">
         <v>-18</v>
       </c>
@@ -33166,7 +33167,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="358" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A358" s="50">
         <v>-17</v>
       </c>
@@ -33218,7 +33219,7 @@
         <v>Nightrex</v>
       </c>
     </row>
-    <row r="359" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A359" s="50">
         <v>-18</v>
       </c>
@@ -33273,7 +33274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="360" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A360" s="50">
         <v>-15</v>
       </c>
@@ -33323,7 +33324,7 @@
         <v>Durfish-S</v>
       </c>
     </row>
-    <row r="361" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A361" s="50">
         <v>-16</v>
       </c>
@@ -33376,7 +33377,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="362" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A362" s="50">
         <v>-1</v>
       </c>
@@ -33425,7 +33426,7 @@
         <v>Wormite-S</v>
       </c>
     </row>
-    <row r="363" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A363" s="50">
         <v>-2</v>
       </c>
@@ -33477,7 +33478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="364" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A364" s="50">
         <v>-3</v>
       </c>
@@ -33529,7 +33530,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="365" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A365" s="50">
         <v>-12</v>
       </c>
@@ -33578,7 +33579,7 @@
         <v>Cluuz-S</v>
       </c>
     </row>
-    <row r="366" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A366" s="50">
         <v>-13</v>
       </c>
@@ -33630,7 +33631,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="367" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A367" s="50">
         <v>-14</v>
       </c>
@@ -33682,7 +33683,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="368" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A368" s="50">
         <v>-4</v>
       </c>
@@ -33737,7 +33738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="369" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A369" s="50">
         <v>-5</v>
       </c>
@@ -33792,7 +33793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="370" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A370" s="50">
         <v>-6</v>
       </c>
@@ -33844,7 +33845,7 @@
         <v>Pyrator-S</v>
       </c>
     </row>
-    <row r="371" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A371" s="50">
         <v>-7</v>
       </c>
@@ -33899,7 +33900,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="372" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A372" s="50">
         <v>-8</v>
       </c>
@@ -33951,7 +33952,7 @@
         <v>Arbok-S</v>
       </c>
     </row>
-    <row r="373" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>243</v>
       </c>
@@ -34001,7 +34002,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="374" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>240</v>
       </c>
@@ -34051,7 +34052,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="375" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>244</v>
       </c>
@@ -34101,7 +34102,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="376" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>242</v>
       </c>
@@ -34151,7 +34152,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="377" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>241</v>
       </c>
@@ -34201,7 +34202,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="378" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>245</v>
       </c>
@@ -34251,7 +34252,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="379" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>246</v>
       </c>
@@ -34301,7 +34302,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="380" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>247</v>
       </c>
@@ -34351,7 +34352,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="381" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>249</v>
       </c>
@@ -34401,7 +34402,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="382" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B382">
         <v>237</v>
       </c>
@@ -34444,7 +34445,7 @@
         <v>Kissyfishy-D</v>
       </c>
     </row>
-    <row r="383" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>89</v>
       </c>
@@ -34489,7 +34490,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="384" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>90</v>
       </c>
@@ -34534,7 +34535,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>91</v>
       </c>
@@ -34579,7 +34580,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>198</v>
       </c>
@@ -34615,7 +34616,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>199</v>
       </c>
@@ -34651,7 +34652,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>46</v>
       </c>
@@ -34687,7 +34688,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>47</v>
       </c>
@@ -34723,7 +34724,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>48</v>
       </c>
@@ -34759,7 +34760,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>220</v>
       </c>
@@ -34795,7 +34796,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>200</v>
       </c>
@@ -34831,7 +34832,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="393" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>201</v>
       </c>
@@ -34867,7 +34868,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>202</v>
       </c>
@@ -34903,7 +34904,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="395" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>203</v>
       </c>
@@ -34939,7 +34940,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="396" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A396" s="51">
         <v>-3</v>
       </c>
@@ -34975,7 +34976,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="397" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A397" s="51">
         <v>-4</v>
       </c>
@@ -35011,7 +35012,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="398" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A398" s="51">
         <v>-5</v>
       </c>
@@ -35047,7 +35048,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="399" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>86</v>
       </c>
@@ -35083,7 +35084,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="400" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>87</v>
       </c>
@@ -35119,7 +35120,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="401" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>88</v>
       </c>
@@ -35155,7 +35156,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="402" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>172</v>
       </c>
@@ -35191,7 +35192,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="403" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>173</v>
       </c>
@@ -35209,7 +35210,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="404" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A404" s="51">
         <v>-6</v>
       </c>
@@ -35245,7 +35246,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="405" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A405" s="51">
         <v>-7</v>
       </c>
@@ -35281,7 +35282,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="406" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>157</v>
       </c>
@@ -35317,7 +35318,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="407" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>158</v>
       </c>
@@ -35353,7 +35354,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="408" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>221</v>
       </c>
@@ -35368,7 +35369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>222</v>
       </c>
@@ -35383,7 +35384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>184</v>
       </c>
@@ -35425,7 +35426,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="411" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>185</v>
       </c>
@@ -35467,7 +35468,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="412" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A412" s="10">
         <v>-12</v>
       </c>
@@ -35479,10 +35480,31 @@
       </c>
       <c r="D412" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="413" spans="1:14" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+      <c r="E412" s="2">
+        <v>75</v>
+      </c>
+      <c r="F412" s="3">
+        <v>55</v>
+      </c>
+      <c r="G412" s="4">
+        <v>55</v>
+      </c>
+      <c r="H412" s="5">
+        <v>75</v>
+      </c>
+      <c r="I412" s="4">
+        <v>45</v>
+      </c>
+      <c r="J412" s="6">
+        <v>30</v>
+      </c>
+      <c r="K412">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="413" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A413" s="10">
         <v>-13</v>
       </c>
@@ -35494,10 +35516,31 @@
       </c>
       <c r="D413" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="414" spans="1:14" x14ac:dyDescent="0.3">
+        <v>485</v>
+      </c>
+      <c r="E413" s="2">
+        <v>95</v>
+      </c>
+      <c r="F413" s="3">
+        <v>85</v>
+      </c>
+      <c r="G413" s="4">
+        <v>70</v>
+      </c>
+      <c r="H413" s="5">
+        <v>130</v>
+      </c>
+      <c r="I413" s="4">
+        <v>65</v>
+      </c>
+      <c r="J413" s="6">
+        <v>40</v>
+      </c>
+      <c r="K413">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="414" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>23</v>
       </c>
@@ -35533,7 +35576,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="415" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A415" s="51">
         <v>-1</v>
       </c>
@@ -35569,7 +35612,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="416" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A416" s="51">
         <v>-2</v>
       </c>
@@ -35605,7 +35648,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="417" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>24</v>
       </c>
@@ -35641,7 +35684,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="418" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>25</v>
       </c>
@@ -35680,7 +35723,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="419" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A419" s="51">
         <v>-8</v>
       </c>
@@ -35716,7 +35759,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="420" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A420" s="51">
         <v>-9</v>
       </c>
@@ -35752,7 +35795,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="421" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>113</v>
       </c>
@@ -35764,13 +35807,31 @@
       </c>
       <c r="D421" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>300</v>
+      </c>
+      <c r="E421" s="2">
+        <v>57</v>
+      </c>
+      <c r="F421" s="3">
+        <v>14</v>
+      </c>
+      <c r="G421" s="4">
+        <v>76</v>
+      </c>
+      <c r="H421" s="5">
+        <v>44</v>
+      </c>
+      <c r="I421" s="4">
+        <v>86</v>
+      </c>
+      <c r="J421" s="6">
+        <v>23</v>
       </c>
       <c r="K421">
         <v>300</v>
       </c>
     </row>
-    <row r="422" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>114</v>
       </c>
@@ -35782,7 +35843,25 @@
       </c>
       <c r="D422" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>500</v>
+      </c>
+      <c r="E422" s="2">
+        <v>67</v>
+      </c>
+      <c r="F422" s="3">
+        <v>99</v>
+      </c>
+      <c r="G422" s="4">
+        <v>111</v>
+      </c>
+      <c r="H422" s="5">
+        <v>79</v>
+      </c>
+      <c r="I422" s="4">
+        <v>111</v>
+      </c>
+      <c r="J422" s="6">
+        <v>33</v>
       </c>
       <c r="K422">
         <v>500</v>
@@ -35791,7 +35870,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="423" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>98</v>
       </c>
@@ -35836,7 +35915,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="424" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>99</v>
       </c>
@@ -35881,7 +35960,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="425" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>100</v>
       </c>
@@ -35929,7 +36008,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="426" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A426" s="50">
         <v>-9</v>
       </c>
@@ -35974,7 +36053,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="427" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A427" s="50">
         <v>-10</v>
       </c>
@@ -36019,7 +36098,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="428" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A428" s="50">
         <v>-11</v>
       </c>
@@ -36067,7 +36146,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="429" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>234</v>
       </c>
@@ -36103,7 +36182,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="430" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>235</v>
       </c>
@@ -36121,7 +36200,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="431" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>236</v>
       </c>
@@ -36139,7 +36218,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="432" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>237</v>
       </c>
@@ -36157,7 +36236,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="433" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>238</v>
       </c>
@@ -36175,7 +36254,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="434" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>239</v>
       </c>
@@ -36193,7 +36272,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="435" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>248</v>
       </c>
@@ -36229,7 +36308,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="436" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B436">
         <v>291</v>
       </c>
@@ -36262,7 +36341,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="437" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>104</v>
       </c>
@@ -36307,7 +36386,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="438" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>105</v>
       </c>
@@ -36352,7 +36431,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="439" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>106</v>
       </c>
@@ -36397,7 +36476,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="440" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>135</v>
       </c>
@@ -36442,7 +36521,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="441" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>136</v>
       </c>
@@ -36487,7 +36566,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="620" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="620" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C620">
         <f>MAX(C385:C618)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Added chests and treasure items!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1681510D-1549-4565-8EF1-AC6F2297A7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EA058F-F5F0-4F05-A9D2-8E5ACADA6C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="1359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2882" uniqueCount="1359">
   <si>
     <t>Leafer</t>
   </si>
@@ -5098,10 +5098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
-  <dimension ref="A1:AU620"/>
+  <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE201" sqref="AE201"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5132,7 +5132,7 @@
     <col min="38" max="47" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>-1</v>
       </c>
@@ -5250,7 +5250,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>-2</v>
       </c>
@@ -5317,8 +5317,11 @@
       <c r="AO2" s="19"/>
       <c r="AR2" s="18"/>
       <c r="AT2" s="17"/>
-    </row>
-    <row r="3" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>-3</v>
       </c>
@@ -5390,8 +5393,11 @@
       <c r="AP3" s="18"/>
       <c r="AR3" s="17"/>
       <c r="AU3" s="19"/>
-    </row>
-    <row r="4" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>-4</v>
       </c>
@@ -5458,8 +5464,11 @@
       <c r="AJ4" s="17"/>
       <c r="AN4" s="17"/>
       <c r="AP4" s="18"/>
-    </row>
-    <row r="5" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>-5</v>
       </c>
@@ -5531,8 +5540,11 @@
       <c r="AR5" s="18"/>
       <c r="AS5" s="17"/>
       <c r="AU5" s="18"/>
-    </row>
-    <row r="6" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>-6</v>
       </c>
@@ -5598,8 +5610,11 @@
       <c r="AO6" s="18"/>
       <c r="AP6" s="18"/>
       <c r="AR6" s="17"/>
-    </row>
-    <row r="7" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>-7</v>
       </c>
@@ -5665,8 +5680,11 @@
       <c r="AK7" s="17"/>
       <c r="AP7" s="17"/>
       <c r="AR7" s="18"/>
-    </row>
-    <row r="8" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>-8</v>
       </c>
@@ -5736,8 +5754,11 @@
       <c r="AR8" s="17"/>
       <c r="AT8" s="18"/>
       <c r="AU8" s="18"/>
-    </row>
-    <row r="9" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>-9</v>
       </c>
@@ -5805,8 +5826,11 @@
       <c r="AO9" s="18"/>
       <c r="AR9" s="19"/>
       <c r="AT9" s="17"/>
-    </row>
-    <row r="10" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>-10</v>
       </c>
@@ -5869,8 +5893,11 @@
       <c r="AN10" s="17"/>
       <c r="AR10" s="17"/>
       <c r="AU10" s="18"/>
-    </row>
-    <row r="11" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>-11</v>
       </c>
@@ -5930,8 +5957,11 @@
       <c r="AN11" s="18"/>
       <c r="AR11" s="18"/>
       <c r="AU11" s="17"/>
-    </row>
-    <row r="12" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>-12</v>
       </c>
@@ -5990,8 +6020,11 @@
       <c r="AL12" s="18"/>
       <c r="AQ12" s="19"/>
       <c r="AT12" s="18"/>
-    </row>
-    <row r="13" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>-13</v>
       </c>
@@ -6056,8 +6089,11 @@
       <c r="AR13" s="18"/>
       <c r="AS13" s="17"/>
       <c r="AU13" s="18"/>
-    </row>
-    <row r="14" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>-14</v>
       </c>
@@ -6113,8 +6149,11 @@
       <c r="AM14" s="17"/>
       <c r="AR14" s="18"/>
       <c r="AU14" s="17"/>
-    </row>
-    <row r="15" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>-15</v>
       </c>
@@ -6168,8 +6207,11 @@
       <c r="AO15" s="17"/>
       <c r="AQ15" s="18"/>
       <c r="AS15" s="18"/>
-    </row>
-    <row r="16" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>-16</v>
       </c>
@@ -6220,8 +6262,11 @@
       <c r="AP16" s="17"/>
       <c r="AR16" s="18"/>
       <c r="AT16" s="19"/>
-    </row>
-    <row r="17" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>-17</v>
       </c>
@@ -6280,8 +6325,11 @@
       <c r="AO17" s="17"/>
       <c r="AQ17" s="18"/>
       <c r="AS17" s="18"/>
-    </row>
-    <row r="18" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>-18</v>
       </c>
@@ -6346,8 +6394,11 @@
       <c r="AR18" s="18"/>
       <c r="AS18" s="17"/>
       <c r="AT18" s="18"/>
-    </row>
-    <row r="19" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>-19</v>
       </c>
@@ -6410,8 +6461,11 @@
       <c r="AR19" s="18"/>
       <c r="AS19" s="18"/>
       <c r="AU19" s="17"/>
-    </row>
-    <row r="20" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>-20</v>
       </c>
@@ -6471,8 +6525,11 @@
       <c r="AP20" s="17"/>
       <c r="AR20" s="17"/>
       <c r="AT20" s="18"/>
-    </row>
-    <row r="21" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>-21</v>
       </c>
@@ -6524,8 +6581,11 @@
       <c r="AN21" s="18"/>
       <c r="AR21" s="18"/>
       <c r="AS21" s="18"/>
-    </row>
-    <row r="22" spans="2:47" x14ac:dyDescent="0.25">
+      <c r="AW21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>-22</v>
       </c>
@@ -6574,7 +6634,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>-23</v>
       </c>
@@ -6622,7 +6682,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>-24</v>
       </c>
@@ -6670,7 +6730,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>-25</v>
       </c>
@@ -6718,7 +6778,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>-26</v>
       </c>
@@ -6763,7 +6823,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>-27</v>
       </c>
@@ -6808,7 +6868,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>-28</v>
       </c>
@@ -6853,7 +6913,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>-29</v>
       </c>
@@ -6931,7 +6991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>-30</v>
       </c>
@@ -7004,7 +7064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>-31</v>
       </c>
@@ -7077,7 +7137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>-32</v>
       </c>
@@ -29306,7 +29366,7 @@
         <v>0.154</v>
       </c>
       <c r="AD286" s="37">
-        <f t="shared" ref="AD286:AD349" si="18">AC286*AB286</f>
+        <f t="shared" ref="AD286:AD325" si="18">AC286*AB286</f>
         <v>0.77</v>
       </c>
       <c r="AF286">

</xml_diff>

<commit_message>
AI Work and some Pokemon tweaks
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F8A8CF-82E5-40A4-B178-3C2E012C69BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8062CD0C-FC4F-41D8-9F73-1F76C987593A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="1368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="1369">
   <si>
     <t>Leafer</t>
   </si>
@@ -4140,6 +4140,9 @@
   </si>
   <si>
     <t>Gelb Cavern</t>
+  </si>
+  <si>
+    <t>Maze</t>
   </si>
 </sst>
 </file>
@@ -4459,7 +4462,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -4519,7 +4522,6 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -5128,8 +5130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N322" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U344" sqref="U344"/>
+    <sheetView tabSelected="1" topLeftCell="N319" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U341" sqref="U341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29394,7 +29396,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AD286" s="37">
-        <f t="shared" ref="AD286:AD349" si="18">AC286*AB286</f>
+        <f t="shared" ref="AD286:AD325" si="18">AC286*AB286</f>
         <v>0.3</v>
       </c>
       <c r="AF286">
@@ -33591,7 +33593,7 @@
       <c r="T336" t="s">
         <v>1360</v>
       </c>
-      <c r="U336" s="53" t="s">
+      <c r="U336" t="s">
         <v>1359</v>
       </c>
     </row>
@@ -33775,10 +33777,13 @@
         <v>3</v>
       </c>
       <c r="U339">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V339" t="s">
         <v>1219</v>
+      </c>
+      <c r="W339" t="s">
+        <v>1368</v>
       </c>
     </row>
     <row r="340" spans="1:24" x14ac:dyDescent="0.25">
@@ -34154,7 +34159,7 @@
       </c>
       <c r="U345">
         <f>SUM(U337:U344)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="346" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gym 5 split trainers and some Pokemon tweaks!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8062CD0C-FC4F-41D8-9F73-1F76C987593A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC239D10-FC61-4C32-BBAC-FF8D55ACEFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="1369">
   <si>
     <t>Leafer</t>
   </si>
@@ -5131,7 +5131,7 @@
   <dimension ref="A1:AW620"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N319" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U341" sqref="U341"/>
+      <selection activeCell="V337" sqref="V337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33597,7 +33597,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>227</v>
       </c>
@@ -33658,7 +33658,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="338" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>218</v>
       </c>
@@ -33722,7 +33722,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>219</v>
       </c>
@@ -33786,7 +33786,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="340" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>223</v>
       </c>
@@ -33844,7 +33844,7 @@
         <v>4</v>
       </c>
       <c r="U340">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V340" t="s">
         <v>825</v>
@@ -33855,8 +33855,11 @@
       <c r="X340" t="s">
         <v>1361</v>
       </c>
-    </row>
-    <row r="341" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y340" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>224</v>
       </c>
@@ -33920,7 +33923,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A342" s="10">
         <v>-10</v>
       </c>
@@ -33978,7 +33981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A343" s="10">
         <v>-11</v>
       </c>
@@ -34045,7 +34048,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A344" s="10">
         <v>-7</v>
       </c>
@@ -34103,7 +34106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A345" s="10">
         <v>-8</v>
       </c>
@@ -34159,10 +34162,10 @@
       </c>
       <c r="U345">
         <f>SUM(U337:U344)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A346" s="10">
         <v>-9</v>
       </c>
@@ -34214,7 +34217,7 @@
         <v>Soldrota-E</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A347" s="10">
         <v>-14</v>
       </c>
@@ -34267,7 +34270,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A348" s="10">
         <v>-15</v>
       </c>
@@ -34320,7 +34323,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A349" s="10">
         <v>-16</v>
       </c>
@@ -34370,7 +34373,7 @@
         <v>Blastflames-E</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A350" s="10">
         <v>-1</v>
       </c>
@@ -34423,7 +34426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A351" s="10">
         <v>-2</v>
       </c>
@@ -34476,7 +34479,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A352" s="10">
         <v>-3</v>
       </c>

</xml_diff>

<commit_message>
Balance changes, moveset and ability tweaks, and some 5 gym trainer work
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC239D10-FC61-4C32-BBAC-FF8D55ACEFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E7A2F6-9761-4375-BA11-02F7CF701082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">(Sheet1!$J$146:$J$429,Sheet1!$J$435:$J$441)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">(Sheet1!$J$146:$J$429,Sheet1!$J$435:$J$441)</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -5130,8 +5134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N319" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V337" sqref="V337"/>
+    <sheetView tabSelected="1" topLeftCell="W135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK153" sqref="AK153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Gym 6 trainers and scripting up to TN Base done!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E7A2F6-9761-4375-BA11-02F7CF701082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0B6F01-7DB8-4376-863E-EAE0CAEF3B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">(Sheet1!$J$146:$J$429,Sheet1!$J$435:$J$441)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">(Sheet1!$J$146:$J$429,Sheet1!$J$435:$J$441)</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4466,7 +4462,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -4526,6 +4522,7 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -5134,8 +5131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK153" sqref="AK153"/>
+    <sheetView tabSelected="1" topLeftCell="K322" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X341" sqref="X341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18325,7 +18322,7 @@
       <c r="B169">
         <v>24</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="10" t="s">
         <v>410</v>
       </c>
       <c r="D169" s="1">
@@ -18632,7 +18629,7 @@
       <c r="B172">
         <v>27</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D172" s="1">
@@ -18734,7 +18731,7 @@
       <c r="B173">
         <v>28</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="10" t="s">
         <v>412</v>
       </c>
       <c r="D173" s="1">
@@ -19920,7 +19917,7 @@
       <c r="B185">
         <v>40</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="10" t="s">
         <v>424</v>
       </c>
       <c r="D185" s="1">
@@ -21001,7 +20998,7 @@
       <c r="B196">
         <v>51</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="10" t="s">
         <v>427</v>
       </c>
       <c r="D196" s="1">
@@ -21304,7 +21301,7 @@
       <c r="B199">
         <v>54</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="10" t="s">
         <v>430</v>
       </c>
       <c r="D199" s="1">
@@ -21503,7 +21500,7 @@
       <c r="B201">
         <v>56</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="10" t="s">
         <v>432</v>
       </c>
       <c r="D201" s="1">
@@ -21699,7 +21696,7 @@
       <c r="B203">
         <v>58</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C203" s="10" t="s">
         <v>434</v>
       </c>
       <c r="D203" s="1">
@@ -22965,7 +22962,7 @@
       <c r="B217">
         <v>72</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="10" t="s">
         <v>448</v>
       </c>
       <c r="D217" s="1">
@@ -25191,7 +25188,7 @@
       <c r="B241">
         <v>96</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C241" s="10" t="s">
         <v>472</v>
       </c>
       <c r="D241" s="1">
@@ -25286,7 +25283,7 @@
       <c r="B242">
         <v>97</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="10" t="s">
         <v>473</v>
       </c>
       <c r="D242" s="1">
@@ -25565,7 +25562,7 @@
       <c r="B245">
         <v>100</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C245" s="53" t="s">
         <v>76</v>
       </c>
       <c r="D245" s="1">
@@ -25845,7 +25842,7 @@
       <c r="B248">
         <v>103</v>
       </c>
-      <c r="C248" t="s">
+      <c r="C248" s="10" t="s">
         <v>477</v>
       </c>
       <c r="D248" s="1">
@@ -26035,7 +26032,7 @@
       <c r="B250">
         <v>105</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C250" s="10" t="s">
         <v>479</v>
       </c>
       <c r="D250" s="1">
@@ -26401,7 +26398,7 @@
       <c r="B254">
         <v>109</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C254" s="53" t="s">
         <v>481</v>
       </c>
       <c r="D254" s="1">
@@ -26491,7 +26488,7 @@
       <c r="B255">
         <v>110</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C255" s="10" t="s">
         <v>482</v>
       </c>
       <c r="D255" s="1">
@@ -26774,7 +26771,7 @@
       <c r="B258">
         <v>113</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C258" s="10" t="s">
         <v>483</v>
       </c>
       <c r="D258" s="1">
@@ -27056,7 +27053,7 @@
       <c r="B261">
         <v>116</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C261" s="53" t="s">
         <v>486</v>
       </c>
       <c r="D261" s="1">
@@ -27338,7 +27335,7 @@
       <c r="B264">
         <v>119</v>
       </c>
-      <c r="C264" t="s">
+      <c r="C264" s="10" t="s">
         <v>489</v>
       </c>
       <c r="D264" s="1">
@@ -27904,7 +27901,7 @@
       <c r="B270">
         <v>125</v>
       </c>
-      <c r="C270" t="s">
+      <c r="C270" s="10" t="s">
         <v>491</v>
       </c>
       <c r="D270" s="1">
@@ -28879,7 +28876,7 @@
       <c r="B281">
         <v>136</v>
       </c>
-      <c r="C281" t="s">
+      <c r="C281" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D281" s="1">
@@ -29062,7 +29059,7 @@
       <c r="B283">
         <v>138</v>
       </c>
-      <c r="C283" t="s">
+      <c r="C283" s="10" t="s">
         <v>499</v>
       </c>
       <c r="D283" s="1">
@@ -29690,7 +29687,7 @@
       <c r="B290">
         <v>145</v>
       </c>
-      <c r="C290" t="s">
+      <c r="C290" s="10" t="s">
         <v>504</v>
       </c>
       <c r="D290" s="1">
@@ -29867,7 +29864,7 @@
       <c r="B292">
         <v>147</v>
       </c>
-      <c r="C292" t="s">
+      <c r="C292" s="10" t="s">
         <v>506</v>
       </c>
       <c r="D292" s="1">
@@ -30782,7 +30779,7 @@
       <c r="B302">
         <v>157</v>
       </c>
-      <c r="C302" t="s">
+      <c r="C302" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D302" s="1">
@@ -31241,7 +31238,7 @@
       <c r="B307">
         <v>162</v>
       </c>
-      <c r="C307" t="s">
+      <c r="C307" s="10" t="s">
         <v>803</v>
       </c>
       <c r="D307" s="1">
@@ -31511,7 +31508,7 @@
       <c r="B310">
         <v>165</v>
       </c>
-      <c r="C310" t="s">
+      <c r="C310" s="10" t="s">
         <v>518</v>
       </c>
       <c r="D310" s="1">
@@ -33071,7 +33068,7 @@
       <c r="B328">
         <v>183</v>
       </c>
-      <c r="C328" t="s">
+      <c r="C328" s="10" t="s">
         <v>94</v>
       </c>
       <c r="D328" s="1">

</xml_diff>

<commit_message>
Bug fixes and some new implementation changes
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0B6F01-7DB8-4376-863E-EAE0CAEF3B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E6EF59B-8671-4E85-8A41-ED1437F393E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2900" uniqueCount="1370">
   <si>
     <t>Leafer</t>
   </si>
@@ -4143,6 +4144,9 @@
   </si>
   <si>
     <t>Maze</t>
+  </si>
+  <si>
+    <t>Drillatron+</t>
   </si>
 </sst>
 </file>
@@ -4462,7 +4466,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -4505,7 +4509,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4522,7 +4525,6 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -5131,8 +5133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K322" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X341" sqref="X341"/>
+    <sheetView tabSelected="1" topLeftCell="K16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7328,10 +7330,10 @@
       <c r="AI33" s="36">
         <v>0</v>
       </c>
-      <c r="AK33" s="51" t="s">
+      <c r="AK33" s="50" t="s">
         <v>1239</v>
       </c>
-      <c r="AL33" s="51">
+      <c r="AL33" s="50">
         <v>1</v>
       </c>
     </row>
@@ -7370,7 +7372,7 @@
       <c r="N34" t="s">
         <v>19</v>
       </c>
-      <c r="O34" s="38" t="s">
+      <c r="O34" t="s">
         <v>1118</v>
       </c>
       <c r="P34" t="s">
@@ -7413,10 +7415,10 @@
       <c r="AI34" s="36">
         <v>0</v>
       </c>
-      <c r="AK34" s="51" t="s">
+      <c r="AK34" s="50" t="s">
         <v>1240</v>
       </c>
-      <c r="AL34" s="51">
+      <c r="AL34" s="50">
         <v>1</v>
       </c>
     </row>
@@ -7623,7 +7625,7 @@
         <v>435</v>
       </c>
       <c r="N37" t="s">
-        <v>70</v>
+        <v>1095</v>
       </c>
       <c r="O37" t="s">
         <v>1121</v>
@@ -7665,10 +7667,10 @@
       <c r="AI37" s="36">
         <v>0</v>
       </c>
-      <c r="AK37" s="51" t="s">
+      <c r="AK37" s="50" t="s">
         <v>1242</v>
       </c>
-      <c r="AL37" s="51">
+      <c r="AL37" s="50">
         <v>1</v>
       </c>
     </row>
@@ -7705,7 +7707,7 @@
         <v>400</v>
       </c>
       <c r="N38" t="s">
-        <v>520</v>
+        <v>1369</v>
       </c>
       <c r="O38" t="s">
         <v>1089</v>
@@ -7953,6 +7955,9 @@
       <c r="N41" t="s">
         <v>1094</v>
       </c>
+      <c r="O41" t="s">
+        <v>1166</v>
+      </c>
       <c r="P41" t="s">
         <v>1092</v>
       </c>
@@ -8033,7 +8038,7 @@
         <v>1083</v>
       </c>
       <c r="O42" t="s">
-        <v>1136</v>
+        <v>1168</v>
       </c>
       <c r="Q42" t="s">
         <v>1115</v>
@@ -8069,10 +8074,10 @@
       <c r="AI42" s="36">
         <v>0</v>
       </c>
-      <c r="AK42" s="51" t="s">
+      <c r="AK42" s="50" t="s">
         <v>1243</v>
       </c>
-      <c r="AL42" s="51">
+      <c r="AL42" s="50">
         <v>1</v>
       </c>
     </row>
@@ -8111,9 +8116,6 @@
       <c r="N43" t="s">
         <v>1084</v>
       </c>
-      <c r="O43" t="s">
-        <v>1137</v>
-      </c>
       <c r="P43" t="s">
         <v>1135</v>
       </c>
@@ -8194,7 +8196,7 @@
         <v>1085</v>
       </c>
       <c r="O44" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="Q44" t="s">
         <v>1097</v>
@@ -8269,8 +8271,11 @@
       <c r="K45">
         <v>505</v>
       </c>
+      <c r="N45" t="s">
+        <v>1232</v>
+      </c>
       <c r="O45" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="Q45" t="s">
         <v>1093</v>
@@ -8345,6 +8350,9 @@
       <c r="K46">
         <v>330</v>
       </c>
+      <c r="O46" t="s">
+        <v>1139</v>
+      </c>
       <c r="Q46" t="s">
         <v>1095</v>
       </c>
@@ -8418,6 +8426,9 @@
       <c r="K47">
         <v>492</v>
       </c>
+      <c r="O47" t="s">
+        <v>1138</v>
+      </c>
       <c r="Q47" t="s">
         <v>443</v>
       </c>
@@ -8738,10 +8749,10 @@
       <c r="AI51" s="36">
         <v>0</v>
       </c>
-      <c r="AK51" s="51" t="s">
+      <c r="AK51" s="50" t="s">
         <v>1250</v>
       </c>
-      <c r="AL51" s="51">
+      <c r="AL51" s="50">
         <v>2</v>
       </c>
     </row>
@@ -8808,10 +8819,10 @@
       <c r="AI52" s="36">
         <v>0</v>
       </c>
-      <c r="AK52" s="51" t="s">
+      <c r="AK52" s="50" t="s">
         <v>1251</v>
       </c>
-      <c r="AL52" s="51">
+      <c r="AL52" s="50">
         <v>2</v>
       </c>
     </row>
@@ -9730,10 +9741,10 @@
       <c r="AI62" s="36">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="AK62" s="51" t="s">
+      <c r="AK62" s="50" t="s">
         <v>1253</v>
       </c>
-      <c r="AL62" s="51">
+      <c r="AL62" s="50">
         <v>2</v>
       </c>
     </row>
@@ -10900,27 +10911,27 @@
       <c r="M75" t="s">
         <v>1081</v>
       </c>
-      <c r="N75" s="40">
+      <c r="N75" s="39">
         <f>SUBTOTAL(101,Table1[HP])</f>
         <v>71.09</v>
       </c>
-      <c r="O75" s="41">
+      <c r="O75" s="40">
         <f>SUBTOTAL(101,Table1[Atk])</f>
         <v>80.470000000000013</v>
       </c>
-      <c r="P75" s="42">
+      <c r="P75" s="41">
         <f>SUBTOTAL(101,Table1[Def])</f>
         <v>73.830000000000013</v>
       </c>
-      <c r="Q75" s="43">
+      <c r="Q75" s="42">
         <f>SUBTOTAL(101,Table1[SpA])</f>
         <v>73.559999999999988</v>
       </c>
-      <c r="R75" s="42">
+      <c r="R75" s="41">
         <f>SUBTOTAL(101,Table1[SpD])</f>
         <v>74.335000000000008</v>
       </c>
-      <c r="S75" s="44">
+      <c r="S75" s="43">
         <f>SUBTOTAL(101,Table1[Spe])</f>
         <v>72.03</v>
       </c>
@@ -11099,10 +11110,10 @@
       <c r="AI77" s="36">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="AK77" s="51" t="s">
+      <c r="AK77" s="50" t="s">
         <v>1263</v>
       </c>
-      <c r="AL77" s="51">
+      <c r="AL77" s="50">
         <v>1</v>
       </c>
     </row>
@@ -12222,10 +12233,10 @@
       <c r="AI93" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK93" s="51" t="s">
+      <c r="AK93" s="50" t="s">
         <v>1273</v>
       </c>
-      <c r="AL93" s="51">
+      <c r="AL93" s="50">
         <v>1</v>
       </c>
     </row>
@@ -12292,10 +12303,10 @@
       <c r="AI94" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK94" s="51" t="s">
+      <c r="AK94" s="50" t="s">
         <v>1274</v>
       </c>
-      <c r="AL94" s="51">
+      <c r="AL94" s="50">
         <v>1</v>
       </c>
     </row>
@@ -12572,10 +12583,10 @@
       <c r="AI98" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK98" s="51" t="s">
+      <c r="AK98" s="50" t="s">
         <v>1275</v>
       </c>
-      <c r="AL98" s="51">
+      <c r="AL98" s="50">
         <v>1</v>
       </c>
     </row>
@@ -13065,10 +13076,10 @@
       <c r="AI105" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK105" s="51" t="s">
+      <c r="AK105" s="50" t="s">
         <v>1280</v>
       </c>
-      <c r="AL105" s="51">
+      <c r="AL105" s="50">
         <v>1</v>
       </c>
     </row>
@@ -13415,10 +13426,10 @@
       <c r="AI110" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK110" s="51" t="s">
+      <c r="AK110" s="50" t="s">
         <v>1283</v>
       </c>
-      <c r="AL110" s="51">
+      <c r="AL110" s="50">
         <v>1</v>
       </c>
     </row>
@@ -13555,10 +13566,10 @@
       <c r="AI112" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK112" s="51" t="s">
+      <c r="AK112" s="50" t="s">
         <v>1285</v>
       </c>
-      <c r="AL112" s="51">
+      <c r="AL112" s="50">
         <v>2</v>
       </c>
     </row>
@@ -13625,10 +13636,10 @@
       <c r="AI113" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK113" s="51" t="s">
+      <c r="AK113" s="50" t="s">
         <v>1286</v>
       </c>
-      <c r="AL113" s="51">
+      <c r="AL113" s="50">
         <v>2</v>
       </c>
     </row>
@@ -13695,10 +13706,10 @@
       <c r="AI114" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK114" s="51" t="s">
+      <c r="AK114" s="50" t="s">
         <v>1287</v>
       </c>
-      <c r="AL114" s="51">
+      <c r="AL114" s="50">
         <v>1</v>
       </c>
     </row>
@@ -14465,10 +14476,10 @@
       <c r="AI125" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK125" s="51" t="s">
+      <c r="AK125" s="50" t="s">
         <v>1294</v>
       </c>
-      <c r="AL125" s="51">
+      <c r="AL125" s="50">
         <v>3</v>
       </c>
     </row>
@@ -15165,10 +15176,10 @@
       <c r="AI135" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK135" s="51" t="s">
+      <c r="AK135" s="50" t="s">
         <v>1298</v>
       </c>
-      <c r="AL135" s="51">
+      <c r="AL135" s="50">
         <v>1</v>
       </c>
     </row>
@@ -15448,10 +15459,10 @@
       <c r="AI139" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK139" s="51" t="s">
+      <c r="AK139" s="50" t="s">
         <v>1299</v>
       </c>
-      <c r="AL139" s="51">
+      <c r="AL139" s="50">
         <v>1</v>
       </c>
     </row>
@@ -15518,10 +15529,10 @@
       <c r="AI140" s="36">
         <v>1.8E-3</v>
       </c>
-      <c r="AK140" s="51" t="s">
+      <c r="AK140" s="50" t="s">
         <v>1300</v>
       </c>
-      <c r="AL140" s="51">
+      <c r="AL140" s="50">
         <v>1</v>
       </c>
     </row>
@@ -21584,10 +21595,10 @@
       <c r="AI201" s="36">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="AK201" s="51" t="s">
+      <c r="AK201" s="50" t="s">
         <v>1356</v>
       </c>
-      <c r="AL201" s="51">
+      <c r="AL201" s="50">
         <v>2</v>
       </c>
     </row>
@@ -21777,10 +21788,10 @@
       <c r="AI203" s="36">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="AK203" s="51" t="s">
+      <c r="AK203" s="50" t="s">
         <v>1357</v>
       </c>
-      <c r="AL203" s="51">
+      <c r="AL203" s="50">
         <v>2</v>
       </c>
     </row>
@@ -22065,10 +22076,10 @@
       <c r="AI206" s="36">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="AK206" s="51" t="s">
+      <c r="AK206" s="50" t="s">
         <v>1358</v>
       </c>
-      <c r="AL206" s="51">
+      <c r="AL206" s="50">
         <v>2</v>
       </c>
     </row>
@@ -25222,7 +25233,7 @@
       <c r="M241" t="s">
         <v>670</v>
       </c>
-      <c r="N241" s="39" t="s">
+      <c r="N241" s="38" t="s">
         <v>1148</v>
       </c>
       <c r="O241" s="32" t="s">
@@ -25562,7 +25573,7 @@
       <c r="B245">
         <v>100</v>
       </c>
-      <c r="C245" s="53" t="s">
+      <c r="C245" t="s">
         <v>76</v>
       </c>
       <c r="D245" s="1">
@@ -26398,7 +26409,7 @@
       <c r="B254">
         <v>109</v>
       </c>
-      <c r="C254" s="53" t="s">
+      <c r="C254" t="s">
         <v>481</v>
       </c>
       <c r="D254" s="1">
@@ -27053,7 +27064,7 @@
       <c r="B261">
         <v>116</v>
       </c>
-      <c r="C261" s="53" t="s">
+      <c r="C261" t="s">
         <v>486</v>
       </c>
       <c r="D261" s="1">
@@ -34797,7 +34808,7 @@
       </c>
     </row>
     <row r="358" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A358" s="50">
+      <c r="A358" s="49">
         <v>-17</v>
       </c>
       <c r="B358">
@@ -34849,7 +34860,7 @@
       </c>
     </row>
     <row r="359" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A359" s="50">
+      <c r="A359" s="49">
         <v>-18</v>
       </c>
       <c r="B359">
@@ -34904,7 +34915,7 @@
       </c>
     </row>
     <row r="360" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A360" s="50">
+      <c r="A360" s="49">
         <v>-15</v>
       </c>
       <c r="B360">
@@ -34954,7 +34965,7 @@
       </c>
     </row>
     <row r="361" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A361" s="50">
+      <c r="A361" s="49">
         <v>-16</v>
       </c>
       <c r="B361">
@@ -35007,7 +35018,7 @@
       </c>
     </row>
     <row r="362" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A362" s="50">
+      <c r="A362" s="49">
         <v>-1</v>
       </c>
       <c r="B362">
@@ -35056,7 +35067,7 @@
       </c>
     </row>
     <row r="363" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A363" s="50">
+      <c r="A363" s="49">
         <v>-2</v>
       </c>
       <c r="B363">
@@ -35108,7 +35119,7 @@
       </c>
     </row>
     <row r="364" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A364" s="50">
+      <c r="A364" s="49">
         <v>-3</v>
       </c>
       <c r="B364">
@@ -35160,7 +35171,7 @@
       </c>
     </row>
     <row r="365" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A365" s="50">
+      <c r="A365" s="49">
         <v>-12</v>
       </c>
       <c r="B365">
@@ -35209,7 +35220,7 @@
       </c>
     </row>
     <row r="366" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A366" s="50">
+      <c r="A366" s="49">
         <v>-13</v>
       </c>
       <c r="B366">
@@ -35261,7 +35272,7 @@
       </c>
     </row>
     <row r="367" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A367" s="50">
+      <c r="A367" s="49">
         <v>-14</v>
       </c>
       <c r="B367">
@@ -35313,7 +35324,7 @@
       </c>
     </row>
     <row r="368" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A368" s="50">
+      <c r="A368" s="49">
         <v>-4</v>
       </c>
       <c r="B368">
@@ -35368,7 +35379,7 @@
       </c>
     </row>
     <row r="369" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A369" s="50">
+      <c r="A369" s="49">
         <v>-5</v>
       </c>
       <c r="B369">
@@ -35423,7 +35434,7 @@
       </c>
     </row>
     <row r="370" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A370" s="50">
+      <c r="A370" s="49">
         <v>-6</v>
       </c>
       <c r="B370">
@@ -35475,7 +35486,7 @@
       </c>
     </row>
     <row r="371" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A371" s="50">
+      <c r="A371" s="49">
         <v>-7</v>
       </c>
       <c r="B371">
@@ -35530,7 +35541,7 @@
       </c>
     </row>
     <row r="372" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A372" s="50">
+      <c r="A372" s="49">
         <v>-8</v>
       </c>
       <c r="B372">
@@ -36511,22 +36522,22 @@
         <f t="shared" si="19"/>
         <v>430</v>
       </c>
-      <c r="E394" s="45">
+      <c r="E394" s="44">
         <v>55</v>
       </c>
-      <c r="F394" s="46">
+      <c r="F394" s="45">
         <v>95</v>
       </c>
-      <c r="G394" s="47">
+      <c r="G394" s="46">
         <v>55</v>
       </c>
-      <c r="H394" s="48">
+      <c r="H394" s="47">
         <v>35</v>
       </c>
-      <c r="I394" s="47">
+      <c r="I394" s="46">
         <v>75</v>
       </c>
-      <c r="J394" s="49">
+      <c r="J394" s="48">
         <v>115</v>
       </c>
       <c r="K394">
@@ -36570,7 +36581,7 @@
       </c>
     </row>
     <row r="396" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A396" s="51">
+      <c r="A396" s="50">
         <v>-3</v>
       </c>
       <c r="B396">
@@ -36606,7 +36617,7 @@
       </c>
     </row>
     <row r="397" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A397" s="51">
+      <c r="A397" s="50">
         <v>-4</v>
       </c>
       <c r="B397">
@@ -36642,7 +36653,7 @@
       </c>
     </row>
     <row r="398" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A398" s="51">
+      <c r="A398" s="50">
         <v>-5</v>
       </c>
       <c r="B398">
@@ -36858,7 +36869,7 @@
       </c>
     </row>
     <row r="404" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A404" s="51">
+      <c r="A404" s="50">
         <v>-6</v>
       </c>
       <c r="B404">
@@ -36894,7 +36905,7 @@
       </c>
     </row>
     <row r="405" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A405" s="51">
+      <c r="A405" s="50">
         <v>-7</v>
       </c>
       <c r="B405">
@@ -37224,7 +37235,7 @@
       </c>
     </row>
     <row r="415" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A415" s="51">
+      <c r="A415" s="50">
         <v>-1</v>
       </c>
       <c r="B415">
@@ -37260,7 +37271,7 @@
       </c>
     </row>
     <row r="416" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A416" s="51">
+      <c r="A416" s="50">
         <v>-2</v>
       </c>
       <c r="B416">
@@ -37371,7 +37382,7 @@
       </c>
     </row>
     <row r="419" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A419" s="51">
+      <c r="A419" s="50">
         <v>-8</v>
       </c>
       <c r="B419">
@@ -37407,7 +37418,7 @@
       </c>
     </row>
     <row r="420" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A420" s="51">
+      <c r="A420" s="50">
         <v>-9</v>
       </c>
       <c r="B420">
@@ -37656,7 +37667,7 @@
       </c>
     </row>
     <row r="426" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A426" s="50">
+      <c r="A426" s="49">
         <v>-9</v>
       </c>
       <c r="B426">
@@ -37701,7 +37712,7 @@
       </c>
     </row>
     <row r="427" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A427" s="50">
+      <c r="A427" s="49">
         <v>-10</v>
       </c>
       <c r="B427">
@@ -37746,7 +37757,7 @@
       </c>
     </row>
     <row r="428" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A428" s="50">
+      <c r="A428" s="49">
         <v>-11</v>
       </c>
       <c r="B428">
@@ -37998,7 +38009,7 @@
       <c r="C437" t="s">
         <v>1220</v>
       </c>
-      <c r="D437" s="52">
+      <c r="D437" s="51">
         <f t="shared" si="21"/>
         <v>190</v>
       </c>
@@ -38043,7 +38054,7 @@
       <c r="C438" t="s">
         <v>1221</v>
       </c>
-      <c r="D438" s="52">
+      <c r="D438" s="51">
         <f t="shared" si="21"/>
         <v>250</v>
       </c>
@@ -38088,7 +38099,7 @@
       <c r="C439" t="s">
         <v>1222</v>
       </c>
-      <c r="D439" s="52">
+      <c r="D439" s="51">
         <f t="shared" si="21"/>
         <v>420</v>
       </c>
@@ -38133,7 +38144,7 @@
       <c r="C440" t="s">
         <v>1225</v>
       </c>
-      <c r="D440" s="52">
+      <c r="D440" s="51">
         <f t="shared" si="21"/>
         <v>290</v>
       </c>
@@ -38178,7 +38189,7 @@
       <c r="C441" t="s">
         <v>1226</v>
       </c>
-      <c r="D441" s="52">
+      <c r="D441" s="51">
         <f t="shared" si="21"/>
         <v>485</v>
       </c>

</xml_diff>

<commit_message>
New sprite, set work, bug fixes and Rawwar done!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E6EF59B-8671-4E85-8A41-ED1437F393E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63141CF6-3A76-42A3-AF19-8E89DAE23750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2900" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2900" uniqueCount="1368">
   <si>
     <t>Leafer</t>
   </si>
@@ -3645,16 +3644,10 @@
     <t>Scovillain</t>
   </si>
   <si>
-    <t>Kerbernero</t>
-  </si>
-  <si>
     <t>Capsakid-S</t>
   </si>
   <si>
     <t>Scovillain-S</t>
-  </si>
-  <si>
-    <t>Kerbernero-S</t>
   </si>
   <si>
     <t>Spice War/Flash Fire/Moody</t>
@@ -4156,7 +4149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4238,6 +4231,15 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4466,7 +4468,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -4525,6 +4527,8 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -5133,8 +5137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" topLeftCell="A408" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7018,7 +7022,7 @@
         <v>1105</v>
       </c>
       <c r="AK29" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="AL29">
         <v>7</v>
@@ -7091,7 +7095,7 @@
         <v>0</v>
       </c>
       <c r="AK30" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="AL30">
         <v>3</v>
@@ -7164,7 +7168,7 @@
         <v>0</v>
       </c>
       <c r="AK31" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="AL31">
         <v>3</v>
@@ -7243,7 +7247,7 @@
         <v>0</v>
       </c>
       <c r="AK32" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="AL32">
         <v>4</v>
@@ -7331,7 +7335,7 @@
         <v>0</v>
       </c>
       <c r="AK33" s="50" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="AL33" s="50">
         <v>1</v>
@@ -7416,7 +7420,7 @@
         <v>0</v>
       </c>
       <c r="AK34" s="50" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="AL34" s="50">
         <v>1</v>
@@ -7586,7 +7590,7 @@
         <v>0</v>
       </c>
       <c r="AK36" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="AL36">
         <v>6</v>
@@ -7668,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="AK37" s="50" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="AL37" s="50">
         <v>1</v>
@@ -7707,7 +7711,7 @@
         <v>400</v>
       </c>
       <c r="N38" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="O38" t="s">
         <v>1089</v>
@@ -8075,7 +8079,7 @@
         <v>0</v>
       </c>
       <c r="AK42" s="50" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="AL42" s="50">
         <v>1</v>
@@ -8233,7 +8237,7 @@
         <v>0</v>
       </c>
       <c r="AK44" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="AL44">
         <v>3</v>
@@ -8272,7 +8276,7 @@
         <v>505</v>
       </c>
       <c r="N45" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="O45" t="s">
         <v>1137</v>
@@ -8312,7 +8316,7 @@
         <v>0</v>
       </c>
       <c r="AK45" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="AL45">
         <v>19</v>
@@ -8388,7 +8392,7 @@
         <v>0</v>
       </c>
       <c r="AK46" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="AL46">
         <v>3</v>
@@ -8455,7 +8459,7 @@
         <v>280</v>
       </c>
       <c r="AG47" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="AH47">
         <v>0</v>
@@ -8528,7 +8532,7 @@
         <v>283</v>
       </c>
       <c r="AG48" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="AH48">
         <v>0</v>
@@ -8537,7 +8541,7 @@
         <v>0</v>
       </c>
       <c r="AK48" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="AL48">
         <v>4</v>
@@ -8598,7 +8602,7 @@
         <v>286</v>
       </c>
       <c r="AG49" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="AH49">
         <v>0</v>
@@ -8607,7 +8611,7 @@
         <v>0</v>
       </c>
       <c r="AK49" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="AL49">
         <v>3</v>
@@ -8671,7 +8675,7 @@
         <v>287</v>
       </c>
       <c r="AG50" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="AH50">
         <v>0</v>
@@ -8680,7 +8684,7 @@
         <v>0</v>
       </c>
       <c r="AK50" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="AL50">
         <v>3</v>
@@ -8741,7 +8745,7 @@
         <v>288</v>
       </c>
       <c r="AG51" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="AH51">
         <v>0</v>
@@ -8750,7 +8754,7 @@
         <v>0</v>
       </c>
       <c r="AK51" s="50" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="AL51" s="50">
         <v>2</v>
@@ -8811,7 +8815,7 @@
         <v>289</v>
       </c>
       <c r="AG52" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="AH52">
         <v>0</v>
@@ -8820,7 +8824,7 @@
         <v>0</v>
       </c>
       <c r="AK52" s="50" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="AL52" s="50">
         <v>2</v>
@@ -9554,7 +9558,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK60" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="AL60">
         <v>4</v>
@@ -9742,7 +9746,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK62" s="50" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="AL62" s="50">
         <v>2</v>
@@ -9836,7 +9840,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK63" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="AL63">
         <v>1</v>
@@ -9930,7 +9934,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK64" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="AL64">
         <v>3</v>
@@ -10024,7 +10028,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK65" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="AL65">
         <v>8</v>
@@ -10212,7 +10216,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK67" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="AL67">
         <v>13</v>
@@ -10588,7 +10592,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK71" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="AL71">
         <v>1</v>
@@ -10682,7 +10686,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK72" s="10" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="AL72" s="10">
         <v>1</v>
@@ -10870,7 +10874,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK74" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="AL74">
         <v>4</v>
@@ -10971,7 +10975,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK75" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="AL75">
         <v>14</v>
@@ -11041,7 +11045,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK76" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="AL76">
         <v>4</v>
@@ -11111,7 +11115,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK77" s="50" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="AL77" s="50">
         <v>1</v>
@@ -11251,7 +11255,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK79" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="AL79">
         <v>9</v>
@@ -11321,7 +11325,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK80" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="AL80">
         <v>6</v>
@@ -11601,7 +11605,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK84" s="10" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="AL84" s="10">
         <v>1</v>
@@ -11674,7 +11678,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK85" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="AL85">
         <v>14</v>
@@ -11744,7 +11748,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK86" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="AL86">
         <v>2</v>
@@ -11875,7 +11879,7 @@
         <v>282</v>
       </c>
       <c r="AG88" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="AH88">
         <v>1</v>
@@ -11884,7 +11888,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK88" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="AL88">
         <v>2</v>
@@ -11945,7 +11949,7 @@
         <v>284</v>
       </c>
       <c r="AG89" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="AH89">
         <v>1</v>
@@ -11954,7 +11958,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK89" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="AL89">
         <v>2</v>
@@ -12015,7 +12019,7 @@
         <v>285</v>
       </c>
       <c r="AG90" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="AH90">
         <v>1</v>
@@ -12024,7 +12028,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK90" s="10" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="AL90" s="10">
         <v>1</v>
@@ -12085,7 +12089,7 @@
         <v>292</v>
       </c>
       <c r="AG91" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="AH91">
         <v>1</v>
@@ -12094,7 +12098,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AK91" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="AL91">
         <v>2</v>
@@ -12155,7 +12159,7 @@
         <v>293</v>
       </c>
       <c r="AG92" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="AH92">
         <v>1</v>
@@ -12234,7 +12238,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK93" s="50" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="AL93" s="50">
         <v>1</v>
@@ -12304,7 +12308,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK94" s="50" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="AL94" s="50">
         <v>1</v>
@@ -12584,7 +12588,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK98" s="50" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="AL98" s="50">
         <v>1</v>
@@ -12724,7 +12728,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK100" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="AL100">
         <v>14</v>
@@ -12794,7 +12798,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK101" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="AL101">
         <v>7</v>
@@ -12864,7 +12868,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK102" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="AL102">
         <v>5</v>
@@ -12937,7 +12941,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK103" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="AL103">
         <v>3</v>
@@ -13077,7 +13081,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK105" s="50" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="AL105" s="50">
         <v>1</v>
@@ -13147,7 +13151,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK106" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="AL106">
         <v>3</v>
@@ -13357,7 +13361,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK109" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="AL109">
         <v>2</v>
@@ -13427,7 +13431,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK110" s="50" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="AL110" s="50">
         <v>1</v>
@@ -13497,7 +13501,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK111" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="AL111">
         <v>7</v>
@@ -13567,7 +13571,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK112" s="50" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="AL112" s="50">
         <v>2</v>
@@ -13637,7 +13641,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK113" s="50" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="AL113" s="50">
         <v>2</v>
@@ -13707,7 +13711,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK114" s="50" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="AL114" s="50">
         <v>1</v>
@@ -13917,7 +13921,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK117" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="AL117">
         <v>5</v>
@@ -13987,7 +13991,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK118" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="AL118">
         <v>9</v>
@@ -14127,7 +14131,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK120" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="AL120">
         <v>3</v>
@@ -14197,7 +14201,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK121" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="AL121">
         <v>14</v>
@@ -14337,7 +14341,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK123" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="AL123">
         <v>3</v>
@@ -14407,7 +14411,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK124" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="AL124">
         <v>9</v>
@@ -14477,7 +14481,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK125" s="50" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="AL125" s="50">
         <v>3</v>
@@ -14617,7 +14621,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK127" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="AL127">
         <v>18</v>
@@ -14687,7 +14691,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK128" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="AL128">
         <v>9</v>
@@ -14897,7 +14901,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK131" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="AL131">
         <v>3</v>
@@ -15177,7 +15181,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK135" s="50" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="AL135" s="50">
         <v>1</v>
@@ -15460,7 +15464,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK139" s="50" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="AL139" s="50">
         <v>1</v>
@@ -15530,7 +15534,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK140" s="50" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="AL140" s="50">
         <v>1</v>
@@ -15607,7 +15611,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK141" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="AL141">
         <v>11</v>
@@ -15853,7 +15857,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK144" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="AL144">
         <v>1</v>
@@ -15861,7 +15865,7 @@
     </row>
     <row r="145" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="B145" t="s">
         <v>876</v>
@@ -15935,7 +15939,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK145" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="AL145">
         <v>4</v>
@@ -16008,7 +16012,7 @@
         <v>858</v>
       </c>
       <c r="W146" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="X146" t="s">
         <v>320</v>
@@ -16042,7 +16046,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK146" s="10" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="AL146" s="10">
         <v>1</v>
@@ -16146,7 +16150,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK147" s="10" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="AL147" s="10">
         <v>1</v>
@@ -16216,7 +16220,7 @@
         <v>858</v>
       </c>
       <c r="W148" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="X148" t="s">
         <v>322</v>
@@ -16250,7 +16254,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK148" s="10" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="AL148" s="10">
         <v>1</v>
@@ -16354,7 +16358,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK149" s="10" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="AL149" s="10">
         <v>1</v>
@@ -16458,7 +16462,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK150" s="10" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="AL150" s="10">
         <v>1</v>
@@ -16559,7 +16563,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK151" s="10" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="AL151" s="10">
         <v>1</v>
@@ -16666,7 +16670,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK152" s="10" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="AL152" s="10">
         <v>1</v>
@@ -16770,7 +16774,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK153" s="10" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="AL153" s="10">
         <v>1</v>
@@ -16871,7 +16875,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK154" s="10" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="AL154" s="10">
         <v>1</v>
@@ -16975,7 +16979,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK155" s="10" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="AL155" s="10">
         <v>1</v>
@@ -17079,7 +17083,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK156" s="10" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="AL156" s="10">
         <v>1</v>
@@ -17149,7 +17153,7 @@
         <v>859</v>
       </c>
       <c r="W157" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="X157" s="10" t="s">
         <v>330</v>
@@ -17183,7 +17187,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK157" s="10" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="AL157" s="10">
         <v>1</v>
@@ -17287,7 +17291,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK158" s="10" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="AL158" s="10">
         <v>1</v>
@@ -17391,7 +17395,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK159" s="10" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="AL159" s="10">
         <v>1</v>
@@ -17492,7 +17496,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK160" s="10" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="AL160" s="10">
         <v>1</v>
@@ -17596,7 +17600,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK161" s="10" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="AL161" s="10">
         <v>1</v>
@@ -17691,7 +17695,7 @@
         <v>281</v>
       </c>
       <c r="AG162" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="AH162">
         <v>2</v>
@@ -17700,7 +17704,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK162" s="10" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="AL162" s="10">
         <v>1</v>
@@ -17795,7 +17799,7 @@
         <v>296</v>
       </c>
       <c r="AG163" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="AH163">
         <v>2</v>
@@ -17804,7 +17808,7 @@
         <v>1.8E-3</v>
       </c>
       <c r="AK163" s="10" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="AL163" s="10">
         <v>1</v>
@@ -17877,7 +17881,7 @@
         <v>859</v>
       </c>
       <c r="W164" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="X164" t="s">
         <v>336</v>
@@ -17911,7 +17915,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK164" s="10" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="AL164" s="10">
         <v>1</v>
@@ -18015,7 +18019,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK165" s="10" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="AL165" s="10">
         <v>1</v>
@@ -18116,7 +18120,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK166" s="10" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="AL166" s="10">
         <v>1</v>
@@ -18218,7 +18222,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK167" s="10" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="AL167" s="10">
         <v>1</v>
@@ -18320,7 +18324,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK168" s="10" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="AL168" s="10">
         <v>1</v>
@@ -18421,7 +18425,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK169" s="10" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="AL169" s="10">
         <v>1</v>
@@ -18525,7 +18529,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK170" s="10" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="AL170" s="10">
         <v>1</v>
@@ -18627,7 +18631,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK171" s="10" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="AL171" s="10">
         <v>1</v>
@@ -18695,7 +18699,7 @@
         <v>835</v>
       </c>
       <c r="W172" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="X172" s="10" t="s">
         <v>194</v>
@@ -18729,7 +18733,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK172" s="10" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="AL172" s="10">
         <v>1</v>
@@ -18825,7 +18829,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK173" s="10" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="AL173" s="10">
         <v>1</v>
@@ -18926,7 +18930,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK174" s="10" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="AL174" s="10">
         <v>1</v>
@@ -19027,7 +19031,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK175" s="10" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="AL175" s="10">
         <v>1</v>
@@ -19125,7 +19129,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK176" s="10" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="AL176" s="10">
         <v>1</v>
@@ -19224,7 +19228,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK177" s="10" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="AL177" s="10">
         <v>1</v>
@@ -19323,7 +19327,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK178" s="10" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="AL178" s="10">
         <v>1</v>
@@ -19419,7 +19423,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK179" s="10" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="AL179" s="10">
         <v>1</v>
@@ -19518,7 +19522,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK180" s="10" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="AL180" s="10">
         <v>1</v>
@@ -19617,7 +19621,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK181" s="10" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="AL181" s="10">
         <v>1</v>
@@ -19713,7 +19717,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK182" s="10" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="AL182" s="10">
         <v>1</v>
@@ -19811,7 +19815,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK183" s="10" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="AL183" s="10">
         <v>1</v>
@@ -19915,7 +19919,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK184" s="10" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="AL184" s="10">
         <v>1</v>
@@ -20016,7 +20020,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK185" s="10" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="AL185" s="10">
         <v>1</v>
@@ -20117,7 +20121,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK186" s="10" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="AL186" s="10">
         <v>1</v>
@@ -20218,7 +20222,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK187" s="10" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="AL187" s="10">
         <v>1</v>
@@ -20316,7 +20320,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK188" s="10" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="AL188" s="10">
         <v>1</v>
@@ -20415,7 +20419,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK189" s="10" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="AL189" s="10">
         <v>1</v>
@@ -20514,7 +20518,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK190" s="10" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="AL190" s="10">
         <v>1</v>
@@ -20576,7 +20580,7 @@
         <v>47</v>
       </c>
       <c r="U191" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="X191" s="12" t="s">
         <v>198</v>
@@ -20610,7 +20614,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK191" s="10" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="AL191" s="10">
         <v>1</v>
@@ -20702,7 +20706,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK192" s="10" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="AL192" s="10">
         <v>1</v>
@@ -20797,7 +20801,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK193" s="10" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="AL193" s="10">
         <v>1</v>
@@ -20898,7 +20902,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK194" s="10" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="AL194" s="10">
         <v>1</v>
@@ -20996,7 +21000,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK195" s="10" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="AL195" s="10">
         <v>1</v>
@@ -21097,7 +21101,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK196" s="10" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="AL196" s="10">
         <v>1</v>
@@ -21397,7 +21401,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK199" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="AL199">
         <v>11</v>
@@ -21447,7 +21451,7 @@
       <c r="N200" s="20" t="s">
         <v>619</v>
       </c>
-      <c r="O200" s="17" t="s">
+      <c r="O200" s="52" t="s">
         <v>773</v>
       </c>
       <c r="P200">
@@ -21489,7 +21493,7 @@
         <v>294</v>
       </c>
       <c r="AG200" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="AH200">
         <v>3</v>
@@ -21587,7 +21591,7 @@
         <v>295</v>
       </c>
       <c r="AG201" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="AH201">
         <v>3</v>
@@ -21596,7 +21600,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="AK201" s="50" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="AL201" s="50">
         <v>2</v>
@@ -21789,7 +21793,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="AK203" s="50" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="AL203" s="50">
         <v>2</v>
@@ -21839,7 +21843,7 @@
       <c r="N204" s="20" t="s">
         <v>668</v>
       </c>
-      <c r="O204" s="32" t="s">
+      <c r="O204" s="53" t="s">
         <v>708</v>
       </c>
       <c r="P204">
@@ -22032,7 +22036,7 @@
       <c r="N206" s="20" t="s">
         <v>871</v>
       </c>
-      <c r="O206" s="17" t="s">
+      <c r="O206" s="52" t="s">
         <v>769</v>
       </c>
       <c r="P206">
@@ -22077,7 +22081,7 @@
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="AK206" s="50" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="AL206" s="50">
         <v>2</v>
@@ -24170,7 +24174,7 @@
       <c r="N230" s="20" t="s">
         <v>1172</v>
       </c>
-      <c r="O230" s="17" t="s">
+      <c r="O230" s="52" t="s">
         <v>759</v>
       </c>
       <c r="P230">
@@ -31487,7 +31491,7 @@
         <v>280</v>
       </c>
       <c r="AA309" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="AB309">
         <v>0</v>
@@ -31574,7 +31578,7 @@
         <v>281</v>
       </c>
       <c r="AA310" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="AB310">
         <v>7</v>
@@ -31666,7 +31670,7 @@
         <v>282</v>
       </c>
       <c r="AA311" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="AB311">
         <v>2</v>
@@ -31758,7 +31762,7 @@
         <v>283</v>
       </c>
       <c r="AA312" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="AB312">
         <v>0</v>
@@ -31847,7 +31851,7 @@
         <v>284</v>
       </c>
       <c r="AA313" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="AB313">
         <v>0</v>
@@ -31939,7 +31943,7 @@
         <v>285</v>
       </c>
       <c r="AA314" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="AB314">
         <v>0</v>
@@ -32028,7 +32032,7 @@
         <v>286</v>
       </c>
       <c r="AA315" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="AB315">
         <v>0</v>
@@ -32120,7 +32124,7 @@
         <v>287</v>
       </c>
       <c r="AA316" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="AB316">
         <v>0</v>
@@ -32212,7 +32216,7 @@
         <v>288</v>
       </c>
       <c r="AA317" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="AB317">
         <v>0</v>
@@ -32301,7 +32305,7 @@
         <v>289</v>
       </c>
       <c r="AA318" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="AB318">
         <v>0</v>
@@ -32568,7 +32572,7 @@
         <v>292</v>
       </c>
       <c r="AA321" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="AB321">
         <v>2</v>
@@ -32658,7 +32662,7 @@
         <v>293</v>
       </c>
       <c r="AA322" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="AB322">
         <v>1</v>
@@ -32745,7 +32749,7 @@
         <v>294</v>
       </c>
       <c r="AA323" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="AB323">
         <v>3</v>
@@ -32835,7 +32839,7 @@
         <v>295</v>
       </c>
       <c r="AA324" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="AB324">
         <v>3</v>
@@ -32922,7 +32926,7 @@
         <v>296</v>
       </c>
       <c r="AA325" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="AB325">
         <v>3</v>
@@ -33603,10 +33607,10 @@
         <v>60</v>
       </c>
       <c r="T336" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="U336" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="337" spans="1:25" x14ac:dyDescent="0.25">
@@ -33667,7 +33671,7 @@
         <v>1</v>
       </c>
       <c r="V337" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="338" spans="1:25" x14ac:dyDescent="0.25">
@@ -33731,7 +33735,7 @@
         <v>1</v>
       </c>
       <c r="V338" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="339" spans="1:25" x14ac:dyDescent="0.25">
@@ -33792,10 +33796,10 @@
         <v>2</v>
       </c>
       <c r="V339" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="W339" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="340" spans="1:25" x14ac:dyDescent="0.25">
@@ -33865,10 +33869,10 @@
         <v>815</v>
       </c>
       <c r="X340" t="s">
+        <v>1359</v>
+      </c>
+      <c r="Y340" t="s">
         <v>1361</v>
-      </c>
-      <c r="Y340" t="s">
-        <v>1363</v>
       </c>
     </row>
     <row r="341" spans="1:25" x14ac:dyDescent="0.25">
@@ -33932,7 +33936,7 @@
         <v>840</v>
       </c>
       <c r="W341" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="342" spans="1:25" x14ac:dyDescent="0.25">
@@ -34051,13 +34055,13 @@
         <v>3</v>
       </c>
       <c r="V343" t="s">
+        <v>1361</v>
+      </c>
+      <c r="W343" t="s">
         <v>1363</v>
       </c>
-      <c r="W343" t="s">
-        <v>1365</v>
-      </c>
       <c r="X343" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="344" spans="1:25" x14ac:dyDescent="0.25">
@@ -37078,10 +37082,10 @@
         <v>335</v>
       </c>
       <c r="L410" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="N410" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="411" spans="1:14" x14ac:dyDescent="0.25">
@@ -37120,10 +37124,10 @@
         <v>485</v>
       </c>
       <c r="L411" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="N411" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="412" spans="1:14" x14ac:dyDescent="0.25">
@@ -37570,7 +37574,7 @@
         <v>681</v>
       </c>
       <c r="N423" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="424" spans="1:15" x14ac:dyDescent="0.25">
@@ -37615,7 +37619,7 @@
         <v>681</v>
       </c>
       <c r="N424" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="425" spans="1:15" x14ac:dyDescent="0.25">
@@ -37626,7 +37630,7 @@
         <v>280</v>
       </c>
       <c r="C425" t="s">
-        <v>1202</v>
+        <v>1225</v>
       </c>
       <c r="D425" s="1">
         <f t="shared" si="21"/>
@@ -37660,10 +37664,10 @@
         <v>669</v>
       </c>
       <c r="N425" t="s">
+        <v>1204</v>
+      </c>
+      <c r="O425" t="s">
         <v>1206</v>
-      </c>
-      <c r="O425" t="s">
-        <v>1208</v>
       </c>
     </row>
     <row r="426" spans="1:15" x14ac:dyDescent="0.25">
@@ -37674,7 +37678,7 @@
         <v>281</v>
       </c>
       <c r="C426" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="D426" s="1">
         <f t="shared" si="21"/>
@@ -37708,7 +37712,7 @@
         <v>597</v>
       </c>
       <c r="N426" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="427" spans="1:15" x14ac:dyDescent="0.25">
@@ -37719,7 +37723,7 @@
         <v>282</v>
       </c>
       <c r="C427" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D427" s="1">
         <f t="shared" si="21"/>
@@ -37753,7 +37757,7 @@
         <v>597</v>
       </c>
       <c r="N427" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="428" spans="1:15" x14ac:dyDescent="0.25">
@@ -37764,7 +37768,7 @@
         <v>283</v>
       </c>
       <c r="C428" t="s">
-        <v>1205</v>
+        <v>1226</v>
       </c>
       <c r="D428" s="1">
         <f t="shared" si="21"/>
@@ -37798,10 +37802,10 @@
         <v>597</v>
       </c>
       <c r="N428" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="O428" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="429" spans="1:15" x14ac:dyDescent="0.25">
@@ -38007,7 +38011,7 @@
         <v>292</v>
       </c>
       <c r="C437" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="D437" s="51">
         <f t="shared" si="21"/>
@@ -38052,7 +38056,7 @@
         <v>293</v>
       </c>
       <c r="C438" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D438" s="51">
         <f t="shared" si="21"/>
@@ -38097,7 +38101,7 @@
         <v>294</v>
       </c>
       <c r="C439" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="D439" s="51">
         <f t="shared" si="21"/>
@@ -38142,7 +38146,7 @@
         <v>295</v>
       </c>
       <c r="C440" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="D440" s="51">
         <f t="shared" si="21"/>
@@ -38173,7 +38177,7 @@
         <v>661</v>
       </c>
       <c r="M440" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="N440" t="s">
         <v>1148</v>
@@ -38187,7 +38191,7 @@
         <v>296</v>
       </c>
       <c r="C441" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="D441" s="51">
         <f t="shared" si="21"/>
@@ -38218,7 +38222,7 @@
         <v>661</v>
       </c>
       <c r="M441" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="N441" t="s">
         <v>1148</v>

</xml_diff>

<commit_message>
Bug fixes trainers battle bet work
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaej\git\PokemonGame\PokemonGame\stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63141CF6-3A76-42A3-AF19-8E89DAE23750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF9A927-DC71-4E99-B987-6AB519543B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -5137,8 +5137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A408" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C426" sqref="C426"/>
+    <sheetView tabSelected="1" topLeftCell="A289" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5165,7 +5165,7 @@
     <col min="30" max="32" width="7.7109375" customWidth="1"/>
     <col min="33" max="33" width="11.42578125" customWidth="1"/>
     <col min="34" max="36" width="7.7109375" customWidth="1"/>
-    <col min="37" max="37" width="20" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8" customWidth="1"/>
     <col min="38" max="47" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
New Fred sprites/cutscene, put new TMs in overworld planned learnsets
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59754BF0-8FE4-49E7-AAEE-BBDC5A6EDF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81975B1E-021C-461A-B742-F26E4D8DEE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3106" uniqueCount="1558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3107" uniqueCount="1559">
   <si>
     <t>Leafer</t>
   </si>
@@ -4709,7 +4709,10 @@
     <t>Light Speed</t>
   </si>
   <si>
-    <t>Radio Burst/Defog</t>
+    <t>Defog</t>
+  </si>
+  <si>
+    <t>Radio Burst</t>
   </si>
 </sst>
 </file>
@@ -4823,7 +4826,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5024,6 +5027,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5046,7 +5061,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
@@ -5110,7 +5125,8 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -5735,8 +5751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E219" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P203" sqref="P203"/>
+    <sheetView tabSelected="1" topLeftCell="E183" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P244" sqref="P244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17106,11 +17122,11 @@
       <c r="N147" s="19" t="s">
         <v>659</v>
       </c>
-      <c r="O147" s="16" t="s">
+      <c r="O147" s="51" t="s">
         <v>730</v>
       </c>
-      <c r="P147">
-        <v>2</v>
+      <c r="P147" t="s">
+        <v>1558</v>
       </c>
       <c r="Q147" t="str">
         <f t="shared" si="11"/>
@@ -17323,7 +17339,7 @@
       <c r="O149" s="16" t="s">
         <v>731</v>
       </c>
-      <c r="P149">
+      <c r="P149" s="10">
         <v>4</v>
       </c>
       <c r="Q149" t="str">
@@ -17430,7 +17446,7 @@
       <c r="O150" s="16" t="s">
         <v>732</v>
       </c>
-      <c r="P150">
+      <c r="P150" s="10">
         <v>5</v>
       </c>
       <c r="Q150" t="str">
@@ -17537,7 +17553,7 @@
       <c r="O151" s="16" t="s">
         <v>740</v>
       </c>
-      <c r="P151">
+      <c r="P151" s="10">
         <v>6</v>
       </c>
       <c r="Q151" t="str">
@@ -17641,7 +17657,7 @@
       <c r="O152" s="16" t="s">
         <v>746</v>
       </c>
-      <c r="P152">
+      <c r="P152" s="10">
         <v>7</v>
       </c>
       <c r="Q152" t="str">
@@ -17751,7 +17767,7 @@
       <c r="O153" s="16" t="s">
         <v>733</v>
       </c>
-      <c r="P153">
+      <c r="P153" s="10">
         <v>8</v>
       </c>
       <c r="Q153" t="str">
@@ -17858,7 +17874,7 @@
       <c r="O154" s="16" t="s">
         <v>734</v>
       </c>
-      <c r="P154">
+      <c r="P154" s="10">
         <v>9</v>
       </c>
       <c r="Q154" t="str">
@@ -18176,7 +18192,7 @@
       <c r="O157" s="10" t="s">
         <v>685</v>
       </c>
-      <c r="P157">
+      <c r="P157" s="10">
         <v>12</v>
       </c>
       <c r="Q157" t="str">
@@ -18283,7 +18299,7 @@
       <c r="O158" s="10" t="s">
         <v>686</v>
       </c>
-      <c r="P158">
+      <c r="P158" s="10">
         <v>13</v>
       </c>
       <c r="Q158" t="str">
@@ -18390,7 +18406,7 @@
       <c r="O159" s="16" t="s">
         <v>736</v>
       </c>
-      <c r="P159">
+      <c r="P159" s="10">
         <v>14</v>
       </c>
       <c r="Q159" t="str">
@@ -18497,7 +18513,7 @@
       <c r="O160" s="10" t="s">
         <v>687</v>
       </c>
-      <c r="P160">
+      <c r="P160" s="10">
         <v>15</v>
       </c>
       <c r="Q160" t="str">
@@ -18601,7 +18617,7 @@
       <c r="O161" s="10" t="s">
         <v>688</v>
       </c>
-      <c r="P161">
+      <c r="P161" s="10">
         <v>16</v>
       </c>
       <c r="Q161" t="str">
@@ -18708,7 +18724,7 @@
       <c r="O162" s="16" t="s">
         <v>725</v>
       </c>
-      <c r="P162">
+      <c r="P162" s="10">
         <v>17</v>
       </c>
       <c r="Q162" t="str">
@@ -18922,7 +18938,7 @@
       <c r="O164" s="16" t="s">
         <v>783</v>
       </c>
-      <c r="P164">
+      <c r="P164" s="10">
         <v>19</v>
       </c>
       <c r="Q164" t="str">
@@ -19032,7 +19048,7 @@
       <c r="O165" s="16" t="s">
         <v>739</v>
       </c>
-      <c r="P165">
+      <c r="P165" s="10">
         <v>20</v>
       </c>
       <c r="Q165" t="str">
@@ -19346,7 +19362,7 @@
       <c r="O168" s="10" t="s">
         <v>689</v>
       </c>
-      <c r="P168">
+      <c r="P168" s="10">
         <v>23</v>
       </c>
       <c r="Q168" t="str">
@@ -19453,7 +19469,7 @@
       <c r="O169" s="10" t="s">
         <v>690</v>
       </c>
-      <c r="P169">
+      <c r="P169" s="10">
         <v>24</v>
       </c>
       <c r="Q169" t="str">
@@ -19557,7 +19573,7 @@
       <c r="O170" s="16" t="s">
         <v>738</v>
       </c>
-      <c r="P170">
+      <c r="P170" s="10">
         <v>25</v>
       </c>
       <c r="Q170" t="str">
@@ -19662,7 +19678,7 @@
       <c r="O171" s="16" t="s">
         <v>691</v>
       </c>
-      <c r="P171">
+      <c r="P171" s="10">
         <v>26</v>
       </c>
       <c r="Q171" t="str">
@@ -19767,7 +19783,7 @@
       <c r="O172" s="16" t="s">
         <v>750</v>
       </c>
-      <c r="P172">
+      <c r="P172" s="57">
         <v>27</v>
       </c>
       <c r="Q172" t="str">
@@ -19872,7 +19888,7 @@
       <c r="O173" s="16" t="s">
         <v>763</v>
       </c>
-      <c r="P173">
+      <c r="P173" s="10">
         <v>28</v>
       </c>
       <c r="Q173" t="str">
@@ -19973,7 +19989,7 @@
       <c r="O174" s="16" t="s">
         <v>764</v>
       </c>
-      <c r="P174">
+      <c r="P174" s="10">
         <v>29</v>
       </c>
       <c r="Q174" t="str">
@@ -20077,7 +20093,7 @@
       <c r="O175" s="16" t="s">
         <v>707</v>
       </c>
-      <c r="P175">
+      <c r="P175" s="10">
         <v>30</v>
       </c>
       <c r="Q175" t="str">
@@ -20181,7 +20197,7 @@
       <c r="O176" s="16" t="s">
         <v>747</v>
       </c>
-      <c r="P176">
+      <c r="P176" s="10">
         <v>31</v>
       </c>
       <c r="Q176" t="str">
@@ -20280,7 +20296,7 @@
       <c r="O177" s="16" t="s">
         <v>765</v>
       </c>
-      <c r="P177">
+      <c r="P177" s="17">
         <v>32</v>
       </c>
       <c r="Q177" t="str">
@@ -20382,7 +20398,7 @@
       <c r="O178" s="16" t="s">
         <v>770</v>
       </c>
-      <c r="P178">
+      <c r="P178" s="17">
         <v>33</v>
       </c>
       <c r="Q178" t="str">
@@ -20481,10 +20497,10 @@
         <v>608</v>
       </c>
       <c r="N179" s="19"/>
-      <c r="O179" s="57" t="s">
+      <c r="O179" s="16" t="s">
         <v>774</v>
       </c>
-      <c r="P179">
+      <c r="P179" s="17">
         <v>34</v>
       </c>
       <c r="Q179" t="str">
@@ -20583,7 +20599,7 @@
       <c r="O180" s="16" t="s">
         <v>742</v>
       </c>
-      <c r="P180">
+      <c r="P180" s="10">
         <v>35</v>
       </c>
       <c r="Q180" t="str">
@@ -20685,7 +20701,7 @@
       <c r="O181" s="16" t="s">
         <v>743</v>
       </c>
-      <c r="P181">
+      <c r="P181" s="10">
         <v>36</v>
       </c>
       <c r="Q181" t="str">
@@ -20787,7 +20803,7 @@
       <c r="O182" s="16" t="s">
         <v>744</v>
       </c>
-      <c r="P182">
+      <c r="P182" s="10">
         <v>37</v>
       </c>
       <c r="Q182" t="str">
@@ -21096,7 +21112,7 @@
       <c r="O185" s="16" t="s">
         <v>745</v>
       </c>
-      <c r="P185">
+      <c r="P185" s="10">
         <v>40</v>
       </c>
       <c r="Q185" t="str">
@@ -21200,7 +21216,7 @@
       <c r="O186" s="10" t="s">
         <v>703</v>
       </c>
-      <c r="P186">
+      <c r="P186" s="10">
         <v>41</v>
       </c>
       <c r="Q186" t="str">
@@ -21304,7 +21320,7 @@
       <c r="O187" s="10" t="s">
         <v>704</v>
       </c>
-      <c r="P187">
+      <c r="P187" s="10">
         <v>42</v>
       </c>
       <c r="Q187" t="str">
@@ -21609,7 +21625,7 @@
       <c r="O190" s="10" t="s">
         <v>728</v>
       </c>
-      <c r="P190">
+      <c r="P190" s="10">
         <v>45</v>
       </c>
       <c r="Q190" t="str">
@@ -21812,7 +21828,7 @@
       <c r="O192" s="16" t="s">
         <v>776</v>
       </c>
-      <c r="P192">
+      <c r="P192" s="10">
         <v>47</v>
       </c>
       <c r="Q192" t="str">
@@ -21907,7 +21923,7 @@
       <c r="O193" s="16" t="s">
         <v>784</v>
       </c>
-      <c r="P193">
+      <c r="P193" s="10">
         <v>48</v>
       </c>
       <c r="Q193" t="str">
@@ -22005,7 +22021,7 @@
       <c r="O194" s="10" t="s">
         <v>683</v>
       </c>
-      <c r="P194">
+      <c r="P194" s="10">
         <v>49</v>
       </c>
       <c r="Q194" t="str">
@@ -22109,7 +22125,7 @@
       <c r="O195" s="10" t="s">
         <v>692</v>
       </c>
-      <c r="P195">
+      <c r="P195" s="10">
         <v>50</v>
       </c>
       <c r="Q195" t="str">
@@ -22210,7 +22226,7 @@
       <c r="O196" s="10" t="s">
         <v>684</v>
       </c>
-      <c r="P196">
+      <c r="P196" s="10">
         <v>51</v>
       </c>
       <c r="Q196" t="str">
@@ -22522,7 +22538,7 @@
       <c r="O199" s="10" t="s">
         <v>693</v>
       </c>
-      <c r="P199">
+      <c r="P199" s="10">
         <v>54</v>
       </c>
       <c r="Q199" t="str">
@@ -22929,7 +22945,7 @@
       <c r="O203" s="16" t="s">
         <v>749</v>
       </c>
-      <c r="P203">
+      <c r="P203" s="17">
         <v>58</v>
       </c>
       <c r="Q203" t="str">
@@ -23324,7 +23340,7 @@
       <c r="O207" s="16" t="s">
         <v>854</v>
       </c>
-      <c r="P207">
+      <c r="P207" s="17">
         <v>62</v>
       </c>
       <c r="Q207" t="str">
@@ -23614,7 +23630,7 @@
       <c r="O210" s="16" t="s">
         <v>751</v>
       </c>
-      <c r="P210">
+      <c r="P210" s="17">
         <v>65</v>
       </c>
       <c r="Q210" t="str">
@@ -24000,7 +24016,7 @@
       <c r="O214" s="16" t="s">
         <v>752</v>
       </c>
-      <c r="P214">
+      <c r="P214" s="10">
         <v>69</v>
       </c>
       <c r="Q214" t="str">
@@ -24193,7 +24209,7 @@
       <c r="O216" s="16" t="s">
         <v>754</v>
       </c>
-      <c r="P216">
+      <c r="P216" s="10">
         <v>71</v>
       </c>
       <c r="Q216" t="str">
@@ -24291,7 +24307,7 @@
       <c r="O217" s="16" t="s">
         <v>766</v>
       </c>
-      <c r="P217">
+      <c r="P217" s="10">
         <v>72</v>
       </c>
       <c r="Q217" t="str">
@@ -24386,7 +24402,7 @@
       <c r="O218" s="16" t="s">
         <v>755</v>
       </c>
-      <c r="P218">
+      <c r="P218" s="10">
         <v>73</v>
       </c>
       <c r="Q218" t="str">
@@ -24487,7 +24503,7 @@
       <c r="O219" s="10" t="s">
         <v>695</v>
       </c>
-      <c r="P219">
+      <c r="P219" s="10">
         <v>74</v>
       </c>
       <c r="Q219" t="str">
@@ -24585,7 +24601,7 @@
       <c r="O220" s="10" t="s">
         <v>696</v>
       </c>
-      <c r="P220">
+      <c r="P220" s="10">
         <v>75</v>
       </c>
       <c r="Q220" t="str">
@@ -24683,7 +24699,7 @@
       <c r="O221" s="10" t="s">
         <v>855</v>
       </c>
-      <c r="P221">
+      <c r="P221" s="10">
         <v>76</v>
       </c>
       <c r="Q221" t="str">
@@ -24781,7 +24797,7 @@
       <c r="O222" s="10" t="s">
         <v>697</v>
       </c>
-      <c r="P222">
+      <c r="P222" s="10">
         <v>77</v>
       </c>
       <c r="Q222" t="str">
@@ -24876,7 +24892,7 @@
       <c r="O223" s="16" t="s">
         <v>756</v>
       </c>
-      <c r="P223">
+      <c r="P223" s="10">
         <v>78</v>
       </c>
       <c r="Q223" t="str">
@@ -24977,7 +24993,7 @@
       <c r="O224" s="10" t="s">
         <v>698</v>
       </c>
-      <c r="P224">
+      <c r="P224" s="10">
         <v>79</v>
       </c>
       <c r="Q224" t="str">
@@ -25072,7 +25088,7 @@
       <c r="O225" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="P225">
+      <c r="P225" s="10">
         <v>80</v>
       </c>
       <c r="Q225" t="str">
@@ -25170,7 +25186,7 @@
       <c r="O226" s="10" t="s">
         <v>700</v>
       </c>
-      <c r="P226">
+      <c r="P226" s="10">
         <v>81</v>
       </c>
       <c r="Q226" t="str">
@@ -25265,7 +25281,7 @@
       <c r="O227" s="10" t="s">
         <v>701</v>
       </c>
-      <c r="P227">
+      <c r="P227" s="10">
         <v>82</v>
       </c>
       <c r="Q227" t="str">
@@ -25360,7 +25376,7 @@
       <c r="O228" s="16" t="s">
         <v>757</v>
       </c>
-      <c r="P228">
+      <c r="P228" s="10">
         <v>83</v>
       </c>
       <c r="Q228" t="str">
@@ -25458,7 +25474,7 @@
       <c r="O229" s="16" t="s">
         <v>758</v>
       </c>
-      <c r="P229">
+      <c r="P229" s="17">
         <v>84</v>
       </c>
       <c r="Q229" t="str">
@@ -25675,7 +25691,7 @@
       <c r="O231" s="16" t="s">
         <v>760</v>
       </c>
-      <c r="P231">
+      <c r="P231" s="10">
         <v>86</v>
       </c>
       <c r="Q231" t="str">
@@ -25782,7 +25798,7 @@
       <c r="O232" s="16" t="s">
         <v>761</v>
       </c>
-      <c r="P232">
+      <c r="P232" s="17">
         <v>87</v>
       </c>
       <c r="Q232" t="str">
@@ -25886,7 +25902,7 @@
       <c r="O233" t="s">
         <v>775</v>
       </c>
-      <c r="P233">
+      <c r="P233" s="17">
         <v>88</v>
       </c>
       <c r="Q233" t="str">
@@ -25993,7 +26009,7 @@
       <c r="O234" s="16" t="s">
         <v>771</v>
       </c>
-      <c r="P234">
+      <c r="P234" s="10">
         <v>89</v>
       </c>
       <c r="Q234" t="str">
@@ -26097,7 +26113,7 @@
       <c r="O235" s="16" t="s">
         <v>762</v>
       </c>
-      <c r="P235">
+      <c r="P235" s="58">
         <v>90</v>
       </c>
       <c r="Q235" t="str">
@@ -26204,7 +26220,7 @@
       <c r="O236" s="10" t="s">
         <v>702</v>
       </c>
-      <c r="P236">
+      <c r="P236" s="58">
         <v>91</v>
       </c>
       <c r="Q236" t="str">
@@ -26415,7 +26431,7 @@
       <c r="O238" s="16" t="s">
         <v>767</v>
       </c>
-      <c r="P238">
+      <c r="P238" s="10">
         <v>93</v>
       </c>
       <c r="Q238" t="str">
@@ -26626,7 +26642,7 @@
       <c r="O240" s="10" t="s">
         <v>694</v>
       </c>
-      <c r="P240">
+      <c r="P240" s="10">
         <v>95</v>
       </c>
       <c r="Q240" t="str">
@@ -26934,7 +26950,7 @@
       <c r="O243" s="21" t="s">
         <v>709</v>
       </c>
-      <c r="P243">
+      <c r="P243" s="10">
         <v>98</v>
       </c>
       <c r="Q243" t="str">
@@ -27036,7 +27052,7 @@
       <c r="O244" s="21" t="s">
         <v>800</v>
       </c>
-      <c r="P244">
+      <c r="P244" s="10">
         <v>99</v>
       </c>
       <c r="Q244" t="str">

</xml_diff>

<commit_message>
Bug fixes, revamp Grust, item/trainer/map updates 5+ gym split
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81975B1E-021C-461A-B742-F26E4D8DEE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA10AF-C8B4-40EA-9C46-5769E8A81B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3107" uniqueCount="1559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="1560">
   <si>
     <t>Leafer</t>
   </si>
@@ -4713,6 +4713,9 @@
   </si>
   <si>
     <t>Radio Burst</t>
+  </si>
+  <si>
+    <t>Shadow -1</t>
   </si>
 </sst>
 </file>
@@ -5751,8 +5754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E183" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P244" sqref="P244"/>
+    <sheetView tabSelected="1" topLeftCell="O328" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X342" sqref="X342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36336,13 +36339,16 @@
         <v>5</v>
       </c>
       <c r="U341">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V341" t="s">
         <v>840</v>
       </c>
       <c r="W341" t="s">
         <v>1365</v>
+      </c>
+      <c r="X341" t="s">
+        <v>1559</v>
       </c>
       <c r="AK341">
         <v>266</v>
@@ -36411,6 +36417,9 @@
       <c r="T342">
         <v>6</v>
       </c>
+      <c r="U342">
+        <v>2</v>
+      </c>
       <c r="AK342">
         <v>267</v>
       </c>
@@ -36554,6 +36563,9 @@
       <c r="T344">
         <v>8</v>
       </c>
+      <c r="U344">
+        <v>4</v>
+      </c>
       <c r="AK344">
         <v>8</v>
       </c>
@@ -36620,7 +36632,7 @@
       </c>
       <c r="U345">
         <f>SUM(U337:U344)</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="AK345">
         <v>11</v>

</xml_diff>

<commit_message>
Ability/moveset for Genieova, trainer fixes, bug fixes
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BA10AF-C8B4-40EA-9C46-5769E8A81B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853044FD-1DCF-4C76-B657-5E009C681340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5754,8 +5754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O328" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X342" sqref="X342"/>
+    <sheetView tabSelected="1" topLeftCell="A400" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D409" sqref="D409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39797,7 +39797,28 @@
       </c>
       <c r="D408" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>410</v>
+      </c>
+      <c r="E408" s="2">
+        <v>60</v>
+      </c>
+      <c r="F408" s="3">
+        <v>55</v>
+      </c>
+      <c r="G408" s="4">
+        <v>70</v>
+      </c>
+      <c r="H408" s="5">
+        <v>90</v>
+      </c>
+      <c r="I408" s="4">
+        <v>70</v>
+      </c>
+      <c r="J408" s="6">
+        <v>65</v>
+      </c>
+      <c r="K408">
+        <v>410</v>
       </c>
     </row>
     <row r="409" spans="1:14" x14ac:dyDescent="0.25">
@@ -39812,7 +39833,28 @@
       </c>
       <c r="D409" s="1">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>570</v>
+      </c>
+      <c r="E409" s="2">
+        <v>90</v>
+      </c>
+      <c r="F409" s="3">
+        <v>70</v>
+      </c>
+      <c r="G409" s="4">
+        <v>105</v>
+      </c>
+      <c r="H409" s="5">
+        <v>120</v>
+      </c>
+      <c r="I409" s="4">
+        <v>95</v>
+      </c>
+      <c r="J409" s="6">
+        <v>90</v>
+      </c>
+      <c r="K409">
+        <v>570</v>
       </c>
     </row>
     <row r="410" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Encounters for 7th gym, updated a batch of old names!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C81FFD01-2BBD-446A-BC38-C48614CD9E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9C816C-C3C9-4667-B824-660A92BBC07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5835,7 +5834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R220" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA100" sqref="AA100"/>
     </sheetView>
   </sheetViews>
@@ -31446,7 +31445,7 @@
         <v>0.13</v>
       </c>
       <c r="AD286" s="36">
-        <f t="shared" ref="AD286:AD349" si="18">AC286*AB286</f>
+        <f t="shared" ref="AD286:AD325" si="18">AC286*AB286</f>
         <v>0.78</v>
       </c>
       <c r="AF286">

</xml_diff>

<commit_message>
8th gym work (AT dialogue, Eclipse base dialogue + trainers done!)
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503EE19F-121F-446F-82F0-731E032AF51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95CB807-0BAB-405E-A2E8-4A2A6DCB0C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3182" uniqueCount="1587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3182" uniqueCount="1643">
   <si>
     <t>Leafer</t>
   </si>
@@ -4797,6 +4797,174 @@
   </si>
   <si>
     <t>6. Dust Sorcerer</t>
+  </si>
+  <si>
+    <t>Chivick</t>
+  </si>
+  <si>
+    <t>Humbrill</t>
+  </si>
+  <si>
+    <t>Huminescence</t>
+  </si>
+  <si>
+    <t>Scigeon</t>
+  </si>
+  <si>
+    <t>Thieven</t>
+  </si>
+  <si>
+    <t>Armoraven</t>
+  </si>
+  <si>
+    <t>Grunswine</t>
+  </si>
+  <si>
+    <t>Hoghoncho</t>
+  </si>
+  <si>
+    <t>Teddull</t>
+  </si>
+  <si>
+    <t>Teddician</t>
+  </si>
+  <si>
+    <t>Teddinaut</t>
+  </si>
+  <si>
+    <t>Minipede</t>
+  </si>
+  <si>
+    <t>Centinel</t>
+  </si>
+  <si>
+    <t>Milimace</t>
+  </si>
+  <si>
+    <t>Milipleura</t>
+  </si>
+  <si>
+    <t>Kappalm</t>
+  </si>
+  <si>
+    <t>Serpenge</t>
+  </si>
+  <si>
+    <t>Scarabit</t>
+  </si>
+  <si>
+    <t>Spartipede</t>
+  </si>
+  <si>
+    <t>Gladipede</t>
+  </si>
+  <si>
+    <t>Willolagos</t>
+  </si>
+  <si>
+    <t>Sedinister</t>
+  </si>
+  <si>
+    <t>Metaslate</t>
+  </si>
+  <si>
+    <t>Sedisoftra</t>
+  </si>
+  <si>
+    <t>Prismodon</t>
+  </si>
+  <si>
+    <t>Asmethiss</t>
+  </si>
+  <si>
+    <t>Aspomancer</t>
+  </si>
+  <si>
+    <t>Kobraturgy</t>
+  </si>
+  <si>
+    <t>Sabore</t>
+  </si>
+  <si>
+    <t>Saberock</t>
+  </si>
+  <si>
+    <t>Rexisilt</t>
+  </si>
+  <si>
+    <t>Pterator</t>
+  </si>
+  <si>
+    <t>Snowlet</t>
+  </si>
+  <si>
+    <t>Nixnerva</t>
+  </si>
+  <si>
+    <t>Cervora</t>
+  </si>
+  <si>
+    <t>Grislush</t>
+  </si>
+  <si>
+    <t>Thalarctic</t>
+  </si>
+  <si>
+    <t>Ceramber</t>
+  </si>
+  <si>
+    <t>Topazatops</t>
+  </si>
+  <si>
+    <t>Lunymph</t>
+  </si>
+  <si>
+    <t>Fearomoth</t>
+  </si>
+  <si>
+    <t>Whotter</t>
+  </si>
+  <si>
+    <t>Lutrineer</t>
+  </si>
+  <si>
+    <t>Mosscelot</t>
+  </si>
+  <si>
+    <t>Osceloma</t>
+  </si>
+  <si>
+    <t>Benglow</t>
+  </si>
+  <si>
+    <t>Sember</t>
+  </si>
+  <si>
+    <t>Kaboon</t>
+  </si>
+  <si>
+    <t>Detonape</t>
+  </si>
+  <si>
+    <t>Sedinister-E</t>
+  </si>
+  <si>
+    <t>Metaslate-E</t>
+  </si>
+  <si>
+    <t>Sedisoftra-E</t>
+  </si>
+  <si>
+    <t>Prismodon-E</t>
+  </si>
+  <si>
+    <t>Sember-S</t>
+  </si>
+  <si>
+    <t>Kaboon-S</t>
+  </si>
+  <si>
+    <t>Detonape-S</t>
   </si>
 </sst>
 </file>
@@ -5834,8 +6002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I434" sqref="I434"/>
+    <sheetView tabSelected="1" topLeftCell="R34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI34" sqref="AI34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8124,10 +8292,10 @@
         <v>0</v>
       </c>
       <c r="AF34">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AG34" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="AH34">
         <v>0</v>
@@ -8212,10 +8380,10 @@
         <v>0</v>
       </c>
       <c r="AF35">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AG35" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="AH35">
         <v>0</v>
@@ -8300,10 +8468,10 @@
         <v>0</v>
       </c>
       <c r="AF36">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="AG36" t="s">
-        <v>570</v>
+        <v>1146</v>
       </c>
       <c r="AH36">
         <v>0</v>
@@ -8385,10 +8553,10 @@
         <v>0</v>
       </c>
       <c r="AF37">
-        <v>236</v>
+        <v>270</v>
       </c>
       <c r="AG37" t="s">
-        <v>571</v>
+        <v>1164</v>
       </c>
       <c r="AH37">
         <v>0</v>
@@ -8470,10 +8638,10 @@
         <v>0</v>
       </c>
       <c r="AF38">
-        <v>237</v>
+        <v>289</v>
       </c>
       <c r="AG38" t="s">
-        <v>576</v>
+        <v>1213</v>
       </c>
       <c r="AH38">
         <v>0</v>
@@ -8555,10 +8723,10 @@
         <v>0</v>
       </c>
       <c r="AF39">
-        <v>259</v>
+        <v>290</v>
       </c>
       <c r="AG39" t="s">
-        <v>1146</v>
+        <v>1179</v>
       </c>
       <c r="AH39">
         <v>0</v>
@@ -8637,10 +8805,10 @@
         <v>0</v>
       </c>
       <c r="AF40">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="AG40" t="s">
-        <v>1162</v>
+        <v>1180</v>
       </c>
       <c r="AH40">
         <v>0</v>
@@ -8716,16 +8884,16 @@
         <v>0</v>
       </c>
       <c r="AF41">
-        <v>270</v>
+        <v>117</v>
       </c>
       <c r="AG41" t="s">
-        <v>1164</v>
+        <v>487</v>
       </c>
       <c r="AH41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI41" s="35">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="AK41">
         <v>11</v>
@@ -8792,16 +8960,16 @@
         <v>0</v>
       </c>
       <c r="AF42">
-        <v>290</v>
+        <v>118</v>
       </c>
       <c r="AG42" t="s">
-        <v>1179</v>
+        <v>488</v>
       </c>
       <c r="AH42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI42" s="35">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="AK42">
         <v>12</v>
@@ -8871,16 +9039,16 @@
         <v>0</v>
       </c>
       <c r="AF43">
-        <v>291</v>
+        <v>156</v>
       </c>
       <c r="AG43" t="s">
-        <v>1180</v>
+        <v>37</v>
       </c>
       <c r="AH43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI43" s="35">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="AK43">
         <v>13</v>
@@ -8944,10 +9112,10 @@
         <v>0</v>
       </c>
       <c r="AF44">
-        <v>117</v>
+        <v>181</v>
       </c>
       <c r="AG44" t="s">
-        <v>487</v>
+        <v>92</v>
       </c>
       <c r="AH44">
         <v>1</v>
@@ -9020,10 +9188,10 @@
         <v>0</v>
       </c>
       <c r="AF45">
-        <v>118</v>
+        <v>184</v>
       </c>
       <c r="AG45" t="s">
-        <v>488</v>
+        <v>101</v>
       </c>
       <c r="AH45">
         <v>1</v>
@@ -9096,10 +9264,10 @@
         <v>0</v>
       </c>
       <c r="AF46">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="AG46" t="s">
-        <v>37</v>
+        <v>534</v>
       </c>
       <c r="AH46">
         <v>1</v>
@@ -9172,10 +9340,10 @@
         <v>0</v>
       </c>
       <c r="AF47">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="AG47" t="s">
-        <v>519</v>
+        <v>536</v>
       </c>
       <c r="AH47">
         <v>1</v>
@@ -9245,10 +9413,10 @@
         <v>0</v>
       </c>
       <c r="AF48">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="AG48" t="s">
-        <v>92</v>
+        <v>537</v>
       </c>
       <c r="AH48">
         <v>1</v>
@@ -9318,10 +9486,10 @@
         <v>0</v>
       </c>
       <c r="AF49">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="AG49" t="s">
-        <v>101</v>
+        <v>539</v>
       </c>
       <c r="AH49">
         <v>1</v>
@@ -9394,10 +9562,10 @@
         <v>0</v>
       </c>
       <c r="AF50">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="AG50" t="s">
-        <v>534</v>
+        <v>1636</v>
       </c>
       <c r="AH50">
         <v>1</v>
@@ -9467,10 +9635,10 @@
         <v>0</v>
       </c>
       <c r="AF51">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="AG51" t="s">
-        <v>536</v>
+        <v>1637</v>
       </c>
       <c r="AH51">
         <v>1</v>
@@ -9540,10 +9708,10 @@
         <v>0</v>
       </c>
       <c r="AF52">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="AG52" t="s">
-        <v>537</v>
+        <v>569</v>
       </c>
       <c r="AH52">
         <v>1</v>
@@ -9613,10 +9781,10 @@
         <v>0</v>
       </c>
       <c r="AF53">
-        <v>202</v>
+        <v>235</v>
       </c>
       <c r="AG53" t="s">
-        <v>539</v>
+        <v>570</v>
       </c>
       <c r="AH53">
         <v>1</v>
@@ -9710,10 +9878,10 @@
         <v>0</v>
       </c>
       <c r="AF54">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="AG54" t="s">
-        <v>542</v>
+        <v>1130</v>
       </c>
       <c r="AH54">
         <v>1</v>
@@ -9807,10 +9975,10 @@
         <v>0</v>
       </c>
       <c r="AF55">
-        <v>206</v>
+        <v>251</v>
       </c>
       <c r="AG55" t="s">
-        <v>543</v>
+        <v>1138</v>
       </c>
       <c r="AH55">
         <v>1</v>
@@ -9904,10 +10072,10 @@
         <v>0</v>
       </c>
       <c r="AF56">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="AG56" t="s">
-        <v>1130</v>
+        <v>1150</v>
       </c>
       <c r="AH56">
         <v>1</v>
@@ -10004,10 +10172,10 @@
         <v>0</v>
       </c>
       <c r="AF57">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="AG57" t="s">
-        <v>1138</v>
+        <v>1162</v>
       </c>
       <c r="AH57">
         <v>1</v>
@@ -10101,10 +10269,10 @@
         <v>0</v>
       </c>
       <c r="AF58">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="AG58" t="s">
-        <v>1150</v>
+        <v>1163</v>
       </c>
       <c r="AH58">
         <v>1</v>
@@ -10198,10 +10366,10 @@
         <v>0</v>
       </c>
       <c r="AF59">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AG59" t="s">
-        <v>1163</v>
+        <v>1168</v>
       </c>
       <c r="AH59">
         <v>1</v>
@@ -10298,10 +10466,10 @@
         <v>0</v>
       </c>
       <c r="AF60">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="AG60" t="s">
-        <v>1166</v>
+        <v>1184</v>
       </c>
       <c r="AH60">
         <v>1</v>
@@ -10395,10 +10563,10 @@
         <v>0</v>
       </c>
       <c r="AF61">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="AG61" t="s">
-        <v>1168</v>
+        <v>1208</v>
       </c>
       <c r="AH61">
         <v>1</v>
@@ -10492,10 +10660,10 @@
         <v>0</v>
       </c>
       <c r="AF62">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="AG62" t="s">
-        <v>1184</v>
+        <v>1209</v>
       </c>
       <c r="AH62">
         <v>1</v>
@@ -10589,10 +10757,10 @@
         <v>0</v>
       </c>
       <c r="AF63">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AG63" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
       <c r="AH63">
         <v>1</v>
@@ -10686,10 +10854,10 @@
         <v>0</v>
       </c>
       <c r="AF64">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AG64" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="AH64">
         <v>1</v>
@@ -10783,10 +10951,10 @@
         <v>0</v>
       </c>
       <c r="AF65">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AG65" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
       <c r="AH65">
         <v>1</v>
@@ -10880,10 +11048,10 @@
         <v>0</v>
       </c>
       <c r="AF66">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="AG66" t="s">
-        <v>1211</v>
+        <v>1199</v>
       </c>
       <c r="AH66">
         <v>1</v>
@@ -10977,10 +11145,10 @@
         <v>0</v>
       </c>
       <c r="AF67">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="AG67" t="s">
-        <v>1212</v>
+        <v>1200</v>
       </c>
       <c r="AH67">
         <v>1</v>
@@ -11074,16 +11242,16 @@
         <v>0</v>
       </c>
       <c r="AF68">
-        <v>289</v>
+        <v>4</v>
       </c>
       <c r="AG68" t="s">
-        <v>1213</v>
+        <v>392</v>
       </c>
       <c r="AH68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI68" s="35">
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AK68">
         <v>38</v>
@@ -11171,16 +11339,16 @@
         <v>0</v>
       </c>
       <c r="AF69">
-        <v>292</v>
+        <v>7</v>
       </c>
       <c r="AG69" t="s">
-        <v>1199</v>
+        <v>395</v>
       </c>
       <c r="AH69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI69" s="35">
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AK69">
         <v>39</v>
@@ -11268,16 +11436,16 @@
         <v>0</v>
       </c>
       <c r="AF70">
-        <v>293</v>
+        <v>23</v>
       </c>
       <c r="AG70" t="s">
-        <v>1200</v>
+        <v>1599</v>
       </c>
       <c r="AH70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI70" s="35">
-        <v>8.0000000000000004E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AK70">
         <v>40</v>
@@ -11365,10 +11533,10 @@
         <v>0</v>
       </c>
       <c r="AF71">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="AG71" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="AH71">
         <v>2</v>
@@ -11462,10 +11630,10 @@
         <v>0</v>
       </c>
       <c r="AF72">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AG72" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="AH72">
         <v>2</v>
@@ -11559,10 +11727,10 @@
         <v>0</v>
       </c>
       <c r="AF73">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AG73" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="AH73">
         <v>2</v>
@@ -11656,10 +11824,10 @@
         <v>0</v>
       </c>
       <c r="AF74">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AG74" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="AH74">
         <v>2</v>
@@ -11760,10 +11928,10 @@
         <v>0</v>
       </c>
       <c r="AF75">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AG75" t="s">
-        <v>422</v>
+        <v>1604</v>
       </c>
       <c r="AH75">
         <v>2</v>
@@ -11833,10 +12001,10 @@
         <v>0</v>
       </c>
       <c r="AF76">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AG76" t="s">
-        <v>47</v>
+        <v>577</v>
       </c>
       <c r="AH76">
         <v>2</v>
@@ -11906,10 +12074,10 @@
         <v>0</v>
       </c>
       <c r="AF77">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AG77" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="AH77">
         <v>2</v>
@@ -11979,10 +12147,10 @@
         <v>0</v>
       </c>
       <c r="AF78">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AG78" t="s">
-        <v>578</v>
+        <v>1608</v>
       </c>
       <c r="AH78">
         <v>2</v>
@@ -12052,10 +12220,10 @@
         <v>0</v>
       </c>
       <c r="AF79">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AG79" t="s">
-        <v>17</v>
+        <v>1609</v>
       </c>
       <c r="AH79">
         <v>2</v>
@@ -12125,10 +12293,10 @@
         <v>0</v>
       </c>
       <c r="AF80">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AG80" t="s">
-        <v>18</v>
+        <v>1613</v>
       </c>
       <c r="AH80">
         <v>2</v>
@@ -12201,7 +12369,7 @@
         <v>55</v>
       </c>
       <c r="AG81" t="s">
-        <v>431</v>
+        <v>1615</v>
       </c>
       <c r="AH81">
         <v>2</v>
@@ -12274,7 +12442,7 @@
         <v>59</v>
       </c>
       <c r="AG82" t="s">
-        <v>435</v>
+        <v>1619</v>
       </c>
       <c r="AH82">
         <v>2</v>
@@ -12569,7 +12737,7 @@
         <v>73</v>
       </c>
       <c r="AG86" t="s">
-        <v>449</v>
+        <v>1626</v>
       </c>
       <c r="AH86">
         <v>2</v>
@@ -12861,7 +13029,7 @@
         <v>94</v>
       </c>
       <c r="AG90" t="s">
-        <v>470</v>
+        <v>1633</v>
       </c>
       <c r="AH90">
         <v>2</v>
@@ -12934,7 +13102,7 @@
         <v>95</v>
       </c>
       <c r="AG91" t="s">
-        <v>471</v>
+        <v>1634</v>
       </c>
       <c r="AH91">
         <v>2</v>
@@ -14175,10 +14343,10 @@
         <v>0</v>
       </c>
       <c r="AF108">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AG108" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AH108">
         <v>2</v>
@@ -14248,10 +14416,10 @@
         <v>0</v>
       </c>
       <c r="AF109">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AG109" t="s">
-        <v>572</v>
+        <v>521</v>
       </c>
       <c r="AH109">
         <v>2</v>
@@ -14321,10 +14489,10 @@
         <v>0</v>
       </c>
       <c r="AF110">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AG110" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="AH110">
         <v>2</v>
@@ -14394,10 +14562,10 @@
         <v>0</v>
       </c>
       <c r="AF111">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AG111" t="s">
-        <v>93</v>
+        <v>573</v>
       </c>
       <c r="AH111">
         <v>2</v>
@@ -14467,10 +14635,10 @@
         <v>0</v>
       </c>
       <c r="AF112">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="AG112" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AH112">
         <v>2</v>
@@ -14540,10 +14708,10 @@
         <v>0</v>
       </c>
       <c r="AF113">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AG113" t="s">
-        <v>528</v>
+        <v>95</v>
       </c>
       <c r="AH113">
         <v>2</v>
@@ -14613,10 +14781,10 @@
         <v>0</v>
       </c>
       <c r="AF114">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AG114" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="AH114">
         <v>2</v>
@@ -14686,10 +14854,10 @@
         <v>0</v>
       </c>
       <c r="AF115">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="AG115" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="AH115">
         <v>2</v>
@@ -14759,10 +14927,10 @@
         <v>0</v>
       </c>
       <c r="AF116">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="AG116" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="AH116">
         <v>2</v>
@@ -14832,10 +15000,10 @@
         <v>0</v>
       </c>
       <c r="AF117">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="AG117" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="AH117">
         <v>2</v>
@@ -14905,10 +15073,10 @@
         <v>0</v>
       </c>
       <c r="AF118">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AG118" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AH118">
         <v>2</v>
@@ -14978,10 +15146,10 @@
         <v>0.2</v>
       </c>
       <c r="AF119">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="AG119" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="AH119">
         <v>2</v>
@@ -15054,10 +15222,10 @@
         <v>0.12</v>
       </c>
       <c r="AF120">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AG120" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="AH120">
         <v>2</v>
@@ -15130,10 +15298,10 @@
         <v>0.09</v>
       </c>
       <c r="AF121">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AG121" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="AH121">
         <v>2</v>
@@ -15203,10 +15371,10 @@
         <v>0.05</v>
       </c>
       <c r="AF122">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AG122" t="s">
-        <v>560</v>
+        <v>1640</v>
       </c>
       <c r="AH122">
         <v>2</v>
@@ -15276,10 +15444,10 @@
         <v>0.12</v>
       </c>
       <c r="AF123">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AG123" t="s">
-        <v>86</v>
+        <v>1641</v>
       </c>
       <c r="AH123">
         <v>2</v>
@@ -15349,10 +15517,10 @@
         <v>0.11</v>
       </c>
       <c r="AF124">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="AG124" t="s">
-        <v>567</v>
+        <v>86</v>
       </c>
       <c r="AH124">
         <v>2</v>
@@ -15422,10 +15590,10 @@
         <v>0.17</v>
       </c>
       <c r="AF125">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="AG125" t="s">
-        <v>804</v>
+        <v>567</v>
       </c>
       <c r="AH125">
         <v>2</v>
@@ -15495,10 +15663,10 @@
         <v>0.02</v>
       </c>
       <c r="AF126">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="AG126" t="s">
-        <v>1137</v>
+        <v>568</v>
       </c>
       <c r="AH126">
         <v>2</v>
@@ -15568,10 +15736,10 @@
         <v>0.01</v>
       </c>
       <c r="AF127">
-        <v>267</v>
+        <v>238</v>
       </c>
       <c r="AG127" t="s">
-        <v>1160</v>
+        <v>804</v>
       </c>
       <c r="AH127">
         <v>2</v>
@@ -15641,10 +15809,10 @@
         <v>0.02</v>
       </c>
       <c r="AF128">
-        <v>276</v>
+        <v>249</v>
       </c>
       <c r="AG128" t="s">
-        <v>1170</v>
+        <v>1137</v>
       </c>
       <c r="AH128">
         <v>2</v>
@@ -15714,10 +15882,10 @@
         <v>0.11</v>
       </c>
       <c r="AF129">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="AG129" t="s">
-        <v>1181</v>
+        <v>1160</v>
       </c>
       <c r="AH129">
         <v>2</v>
@@ -15787,10 +15955,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AF130">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="AG130" t="s">
-        <v>1183</v>
+        <v>1166</v>
       </c>
       <c r="AH130">
         <v>2</v>
@@ -15860,16 +16028,16 @@
         <v>0.15</v>
       </c>
       <c r="AF131">
-        <v>11</v>
+        <v>276</v>
       </c>
       <c r="AG131" t="s">
-        <v>399</v>
+        <v>1170</v>
       </c>
       <c r="AH131">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI131" s="35">
-        <v>2.3999999999999998E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AK131">
         <v>101</v>
@@ -15933,16 +16101,16 @@
         <v>0.3</v>
       </c>
       <c r="AF132">
-        <v>26</v>
+        <v>278</v>
       </c>
       <c r="AG132" t="s">
-        <v>11</v>
+        <v>1181</v>
       </c>
       <c r="AH132">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI132" s="35">
-        <v>2.3999999999999998E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AK132">
         <v>102</v>
@@ -16009,16 +16177,16 @@
         <v>0.17</v>
       </c>
       <c r="AF133">
-        <v>30</v>
+        <v>281</v>
       </c>
       <c r="AG133" t="s">
-        <v>414</v>
+        <v>1183</v>
       </c>
       <c r="AH133">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI133" s="35">
-        <v>2.3999999999999998E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="AK133">
         <v>103</v>
@@ -16082,10 +16250,10 @@
         <v>0.05</v>
       </c>
       <c r="AF134">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="AG134" t="s">
-        <v>416</v>
+        <v>390</v>
       </c>
       <c r="AH134">
         <v>3</v>
@@ -16155,10 +16323,10 @@
         <v>0.01</v>
       </c>
       <c r="AF135">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="AG135" t="s">
-        <v>420</v>
+        <v>393</v>
       </c>
       <c r="AH135">
         <v>3</v>
@@ -16228,10 +16396,10 @@
         <v>0.04</v>
       </c>
       <c r="AF136">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="AG136" t="s">
-        <v>428</v>
+        <v>396</v>
       </c>
       <c r="AH136">
         <v>3</v>
@@ -16301,10 +16469,10 @@
         <v>0.09</v>
       </c>
       <c r="AF137">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="AG137" t="s">
-        <v>429</v>
+        <v>1588</v>
       </c>
       <c r="AH137">
         <v>3</v>
@@ -16377,10 +16545,10 @@
         <v>0.1</v>
       </c>
       <c r="AF138">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="AG138" t="s">
-        <v>433</v>
+        <v>11</v>
       </c>
       <c r="AH138">
         <v>3</v>
@@ -16453,10 +16621,10 @@
         <v>0.09</v>
       </c>
       <c r="AF139">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="AG139" t="s">
-        <v>442</v>
+        <v>414</v>
       </c>
       <c r="AH139">
         <v>3</v>
@@ -16529,10 +16697,10 @@
         <v>0.02</v>
       </c>
       <c r="AF140">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="AG140" t="s">
-        <v>446</v>
+        <v>416</v>
       </c>
       <c r="AH140">
         <v>3</v>
@@ -16609,10 +16777,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="AF141">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="AG141" t="s">
-        <v>456</v>
+        <v>420</v>
       </c>
       <c r="AH141">
         <v>3</v>
@@ -16692,10 +16860,10 @@
         <v>0.18</v>
       </c>
       <c r="AF142">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="AG142" t="s">
-        <v>457</v>
+        <v>1612</v>
       </c>
       <c r="AH142">
         <v>3</v>
@@ -16772,10 +16940,10 @@
         <v>0.22</v>
       </c>
       <c r="AF143">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="AG143" t="s">
-        <v>458</v>
+        <v>1617</v>
       </c>
       <c r="AH143">
         <v>3</v>
@@ -16864,10 +17032,10 @@
         <v>0.12</v>
       </c>
       <c r="AF144">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="AG144" t="s">
-        <v>461</v>
+        <v>1624</v>
       </c>
       <c r="AH144">
         <v>3</v>
@@ -16949,10 +17117,10 @@
         <v>0.09</v>
       </c>
       <c r="AF145">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="AG145" t="s">
-        <v>476</v>
+        <v>446</v>
       </c>
       <c r="AH145">
         <v>3</v>
@@ -17059,10 +17227,10 @@
         <v>0.1</v>
       </c>
       <c r="AF146">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="AG146" t="s">
-        <v>478</v>
+        <v>1630</v>
       </c>
       <c r="AH146">
         <v>3</v>
@@ -17166,10 +17334,10 @@
         <v>0.02</v>
       </c>
       <c r="AF147">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="AG147" t="s">
-        <v>43</v>
+        <v>1631</v>
       </c>
       <c r="AH147">
         <v>3</v>
@@ -17273,10 +17441,10 @@
         <v>0.19</v>
       </c>
       <c r="AF148">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="AG148" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="AH148">
         <v>3</v>
@@ -17380,10 +17548,10 @@
         <v>0.04</v>
       </c>
       <c r="AF149">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="AG149" t="s">
-        <v>583</v>
+        <v>461</v>
       </c>
       <c r="AH149">
         <v>3</v>
@@ -17487,10 +17655,10 @@
         <v>0.05</v>
       </c>
       <c r="AF150">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="AG150" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
       <c r="AH150">
         <v>3</v>
@@ -17591,10 +17759,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AF151">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="AG151" t="s">
-        <v>62</v>
+        <v>478</v>
       </c>
       <c r="AH151">
         <v>3</v>
@@ -17701,10 +17869,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AF152">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="AG152" t="s">
-        <v>507</v>
+        <v>43</v>
       </c>
       <c r="AH152">
         <v>3</v>
@@ -17808,10 +17976,10 @@
         <v>0.25</v>
       </c>
       <c r="AF153">
-        <v>172</v>
+        <v>115</v>
       </c>
       <c r="AG153" t="s">
-        <v>522</v>
+        <v>485</v>
       </c>
       <c r="AH153">
         <v>3</v>
@@ -17912,10 +18080,10 @@
         <v>0.04</v>
       </c>
       <c r="AF154">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="AG154" t="s">
-        <v>524</v>
+        <v>583</v>
       </c>
       <c r="AH154">
         <v>3</v>
@@ -18019,10 +18187,10 @@
         <v>0.04</v>
       </c>
       <c r="AF155">
-        <v>186</v>
+        <v>132</v>
       </c>
       <c r="AG155" t="s">
-        <v>103</v>
+        <v>495</v>
       </c>
       <c r="AH155">
         <v>3</v>
@@ -18126,10 +18294,10 @@
         <v>0.01</v>
       </c>
       <c r="AF156">
-        <v>188</v>
+        <v>135</v>
       </c>
       <c r="AG156" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="AH156">
         <v>3</v>
@@ -18233,10 +18401,10 @@
         <v>0.01</v>
       </c>
       <c r="AF157">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="AG157" t="s">
-        <v>529</v>
+        <v>507</v>
       </c>
       <c r="AH157">
         <v>3</v>
@@ -18343,10 +18511,10 @@
         <v>0.12</v>
       </c>
       <c r="AF158">
-        <v>212</v>
+        <v>172</v>
       </c>
       <c r="AG158" t="s">
-        <v>549</v>
+        <v>522</v>
       </c>
       <c r="AH158">
         <v>3</v>
@@ -18450,10 +18618,10 @@
         <v>0.04</v>
       </c>
       <c r="AF159">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="AG159" t="s">
-        <v>552</v>
+        <v>524</v>
       </c>
       <c r="AH159">
         <v>3</v>
@@ -18554,10 +18722,10 @@
         <v>0.13</v>
       </c>
       <c r="AF160">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="AG160" t="s">
-        <v>555</v>
+        <v>96</v>
       </c>
       <c r="AH160">
         <v>3</v>
@@ -18661,10 +18829,10 @@
         <v>0.12</v>
       </c>
       <c r="AF161">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="AG161" t="s">
-        <v>562</v>
+        <v>529</v>
       </c>
       <c r="AH161">
         <v>3</v>
@@ -18768,10 +18936,10 @@
         <v>0.22</v>
       </c>
       <c r="AF162">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="AG162" t="s">
-        <v>1126</v>
+        <v>549</v>
       </c>
       <c r="AH162">
         <v>3</v>
@@ -18875,10 +19043,10 @@
         <v>0.22</v>
       </c>
       <c r="AF163">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="AG163" t="s">
-        <v>1131</v>
+        <v>552</v>
       </c>
       <c r="AH163">
         <v>3</v>
@@ -18985,10 +19153,10 @@
         <v>0.2</v>
       </c>
       <c r="AF164">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="AG164" t="s">
-        <v>1134</v>
+        <v>555</v>
       </c>
       <c r="AH164">
         <v>3</v>
@@ -19092,10 +19260,10 @@
         <v>0.3</v>
       </c>
       <c r="AF165">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="AG165" t="s">
-        <v>1139</v>
+        <v>562</v>
       </c>
       <c r="AH165">
         <v>3</v>
@@ -19199,10 +19367,10 @@
         <v>0.31</v>
       </c>
       <c r="AF166">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="AG166" t="s">
-        <v>1141</v>
+        <v>1126</v>
       </c>
       <c r="AH166">
         <v>3</v>
@@ -19307,10 +19475,10 @@
         <v>0.8</v>
       </c>
       <c r="AF167">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="AG167" t="s">
-        <v>1159</v>
+        <v>1131</v>
       </c>
       <c r="AH167">
         <v>3</v>
@@ -19412,10 +19580,10 @@
         <v>0.2</v>
       </c>
       <c r="AF168">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="AG168" t="s">
-        <v>1161</v>
+        <v>1134</v>
       </c>
       <c r="AH168">
         <v>3</v>
@@ -19516,10 +19684,10 @@
         <v>0.09</v>
       </c>
       <c r="AF169">
-        <v>280</v>
+        <v>252</v>
       </c>
       <c r="AG169" t="s">
-        <v>1206</v>
+        <v>1139</v>
       </c>
       <c r="AH169">
         <v>3</v>
@@ -19623,10 +19791,10 @@
         <v>0.22</v>
       </c>
       <c r="AF170">
-        <v>295</v>
+        <v>254</v>
       </c>
       <c r="AG170" t="s">
-        <v>1204</v>
+        <v>1141</v>
       </c>
       <c r="AH170">
         <v>3</v>
@@ -19731,16 +19899,16 @@
         <v>0.16</v>
       </c>
       <c r="AF171">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="AG171" t="s">
-        <v>389</v>
+        <v>1159</v>
       </c>
       <c r="AH171">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AI171" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="AK171">
         <v>141</v>
@@ -19836,16 +20004,16 @@
         <v>0.75</v>
       </c>
       <c r="AF172">
-        <v>4</v>
+        <v>268</v>
       </c>
       <c r="AG172" t="s">
-        <v>392</v>
+        <v>1161</v>
       </c>
       <c r="AH172">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AI172" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="AK172">
         <v>142</v>
@@ -19935,16 +20103,16 @@
         <v>0.25</v>
       </c>
       <c r="AF173">
-        <v>7</v>
+        <v>280</v>
       </c>
       <c r="AG173" t="s">
-        <v>395</v>
+        <v>1206</v>
       </c>
       <c r="AH173">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AI173" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="AK173">
         <v>143</v>
@@ -20039,16 +20207,16 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AF174">
-        <v>14</v>
+        <v>295</v>
       </c>
       <c r="AG174" t="s">
-        <v>402</v>
+        <v>1204</v>
       </c>
       <c r="AH174">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AI174" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="AK174">
         <v>144</v>
@@ -20143,10 +20311,10 @@
         <v>0.19</v>
       </c>
       <c r="AF175">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AG175" t="s">
-        <v>404</v>
+        <v>1591</v>
       </c>
       <c r="AH175">
         <v>4</v>
@@ -20244,10 +20412,10 @@
         <v>0.25</v>
       </c>
       <c r="AF176">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AG176" t="s">
-        <v>406</v>
+        <v>1594</v>
       </c>
       <c r="AH176">
         <v>4</v>
@@ -20349,10 +20517,10 @@
         <v>0.24</v>
       </c>
       <c r="AF177">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="AG177" t="s">
-        <v>423</v>
+        <v>1596</v>
       </c>
       <c r="AH177">
         <v>4</v>
@@ -20451,10 +20619,10 @@
         <v>0.11</v>
       </c>
       <c r="AF178">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AG178" t="s">
-        <v>49</v>
+        <v>423</v>
       </c>
       <c r="AH178">
         <v>4</v>
@@ -20550,10 +20718,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AF179">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="AG179" t="s">
-        <v>440</v>
+        <v>1606</v>
       </c>
       <c r="AH179">
         <v>4</v>
@@ -20652,10 +20820,10 @@
         <v>0.25</v>
       </c>
       <c r="AF180">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AG180" t="s">
-        <v>445</v>
+        <v>1622</v>
       </c>
       <c r="AH180">
         <v>4</v>
@@ -20754,10 +20922,10 @@
         <v>0.19</v>
       </c>
       <c r="AF181">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="AG181" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="AH181">
         <v>4</v>
@@ -20853,10 +21021,10 @@
         <v>0.15</v>
       </c>
       <c r="AF182">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="AG182" t="s">
-        <v>462</v>
+        <v>1628</v>
       </c>
       <c r="AH182">
         <v>4</v>
@@ -20954,10 +21122,10 @@
         <v>0.22</v>
       </c>
       <c r="AF183">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AG183" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AH183">
         <v>4</v>
@@ -21061,10 +21229,10 @@
         <v>0.3</v>
       </c>
       <c r="AF184">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AG184" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="AH184">
         <v>4</v>
@@ -21165,10 +21333,10 @@
         <v>0.36</v>
       </c>
       <c r="AF185">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="AG185" t="s">
-        <v>91</v>
+        <v>468</v>
       </c>
       <c r="AH185">
         <v>4</v>
@@ -21269,10 +21437,10 @@
         <v>0.16</v>
       </c>
       <c r="AF186">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AG186" t="s">
-        <v>490</v>
+        <v>91</v>
       </c>
       <c r="AH186">
         <v>4</v>
@@ -21373,10 +21541,10 @@
         <v>0.27</v>
       </c>
       <c r="AF187">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="AG187" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="AH187">
         <v>4</v>
@@ -21474,10 +21642,10 @@
         <v>0.21</v>
       </c>
       <c r="AF188">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="AG188" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
       <c r="AH188">
         <v>4</v>
@@ -21576,10 +21744,10 @@
         <v>0.3</v>
       </c>
       <c r="AF189">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="AG189" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="AH189">
         <v>4</v>
@@ -21678,10 +21846,10 @@
         <v>0.4</v>
       </c>
       <c r="AF190">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG190" t="s">
-        <v>803</v>
+        <v>515</v>
       </c>
       <c r="AH190">
         <v>4</v>
@@ -21777,10 +21945,10 @@
         <v>0.17</v>
       </c>
       <c r="AF191">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="AG191" t="s">
-        <v>526</v>
+        <v>803</v>
       </c>
       <c r="AH191">
         <v>4</v>
@@ -21872,10 +22040,10 @@
         <v>0.22</v>
       </c>
       <c r="AF192">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="AG192" t="s">
-        <v>102</v>
+        <v>526</v>
       </c>
       <c r="AH192">
         <v>4</v>
@@ -21970,10 +22138,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AF193">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="AG193" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="AH193">
         <v>4</v>
@@ -22074,10 +22242,10 @@
         <v>0.32</v>
       </c>
       <c r="AF194">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AG194" t="s">
-        <v>801</v>
+        <v>97</v>
       </c>
       <c r="AH194">
         <v>4</v>
@@ -22175,10 +22343,10 @@
         <v>0.19</v>
       </c>
       <c r="AF195">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AG195" t="s">
-        <v>530</v>
+        <v>801</v>
       </c>
       <c r="AH195">
         <v>4</v>
@@ -22279,10 +22447,10 @@
         <v>0.19</v>
       </c>
       <c r="AF196">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="AG196" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="AH196">
         <v>4</v>
@@ -22383,10 +22551,10 @@
         <v>0.24</v>
       </c>
       <c r="AF197">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="AG197" t="s">
-        <v>558</v>
+        <v>541</v>
       </c>
       <c r="AH197">
         <v>4</v>
@@ -22487,10 +22655,10 @@
         <v>0.17</v>
       </c>
       <c r="AF198">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="AG198" t="s">
-        <v>805</v>
+        <v>558</v>
       </c>
       <c r="AH198">
         <v>4</v>
@@ -22588,10 +22756,10 @@
         <v>0.19</v>
       </c>
       <c r="AF199">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AG199" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="AH199">
         <v>4</v>
@@ -22692,10 +22860,10 @@
         <v>0.24</v>
       </c>
       <c r="AF200">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AG200" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="AH200">
         <v>4</v>
@@ -22793,10 +22961,10 @@
         <v>0.36</v>
       </c>
       <c r="AF201">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="AG201" t="s">
-        <v>1136</v>
+        <v>1142</v>
       </c>
       <c r="AH201">
         <v>4</v>
@@ -22894,10 +23062,10 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="AF202">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="AG202" t="s">
-        <v>1135</v>
+        <v>1144</v>
       </c>
       <c r="AH202">
         <v>4</v>
@@ -22992,10 +23160,10 @@
         <v>0.29009999999999997</v>
       </c>
       <c r="AF203">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="AG203" t="s">
-        <v>1142</v>
+        <v>1147</v>
       </c>
       <c r="AH203">
         <v>4</v>
@@ -23093,10 +23261,10 @@
         <v>0.33</v>
       </c>
       <c r="AF204">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="AG204" t="s">
-        <v>1144</v>
+        <v>1148</v>
       </c>
       <c r="AH204">
         <v>4</v>
@@ -23191,10 +23359,10 @@
         <v>0.18</v>
       </c>
       <c r="AF205">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="AG205" t="s">
-        <v>1145</v>
+        <v>1182</v>
       </c>
       <c r="AH205">
         <v>4</v>
@@ -23289,10 +23457,10 @@
         <v>0.29009999999999997</v>
       </c>
       <c r="AF206">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="AG206" t="s">
-        <v>1147</v>
+        <v>1207</v>
       </c>
       <c r="AH206">
         <v>4</v>
@@ -23390,10 +23558,10 @@
         <v>0.15989999999999999</v>
       </c>
       <c r="AF207">
-        <v>261</v>
+        <v>296</v>
       </c>
       <c r="AG207" t="s">
-        <v>1148</v>
+        <v>1205</v>
       </c>
       <c r="AH207">
         <v>4</v>
@@ -23485,16 +23653,16 @@
         <v>0.23010000000000003</v>
       </c>
       <c r="AF208">
-        <v>266</v>
+        <v>13</v>
       </c>
       <c r="AG208" t="s">
-        <v>1158</v>
+        <v>1590</v>
       </c>
       <c r="AH208">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI208" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AK208">
         <v>178</v>
@@ -23581,16 +23749,16 @@
         <v>0.2001</v>
       </c>
       <c r="AF209">
-        <v>271</v>
+        <v>17</v>
       </c>
       <c r="AG209" t="s">
-        <v>1165</v>
+        <v>1593</v>
       </c>
       <c r="AH209">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI209" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AK209">
         <v>179</v>
@@ -23674,16 +23842,16 @@
         <v>0.29009999999999997</v>
       </c>
       <c r="AF210">
-        <v>277</v>
+        <v>21</v>
       </c>
       <c r="AG210" t="s">
-        <v>1171</v>
+        <v>1597</v>
       </c>
       <c r="AH210">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI210" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AK210">
         <v>180</v>
@@ -23772,16 +23940,16 @@
         <v>0.24990000000000001</v>
       </c>
       <c r="AF211">
-        <v>279</v>
+        <v>42</v>
       </c>
       <c r="AG211" t="s">
-        <v>1182</v>
+        <v>1605</v>
       </c>
       <c r="AH211">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI211" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AK211">
         <v>181</v>
@@ -23870,16 +24038,16 @@
         <v>0.1701</v>
       </c>
       <c r="AF212">
-        <v>283</v>
+        <v>50</v>
       </c>
       <c r="AG212" t="s">
-        <v>1207</v>
+        <v>1610</v>
       </c>
       <c r="AH212">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI212" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AK212">
         <v>182</v>
@@ -23971,16 +24139,16 @@
         <v>0.27989999999999998</v>
       </c>
       <c r="AF213">
-        <v>296</v>
+        <v>51</v>
       </c>
       <c r="AG213" t="s">
-        <v>1205</v>
+        <v>1611</v>
       </c>
       <c r="AH213">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI213" s="35">
-        <v>3.2000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AK213">
         <v>183</v>
@@ -24072,10 +24240,10 @@
         <v>0.33</v>
       </c>
       <c r="AF214">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="AG214" t="s">
-        <v>401</v>
+        <v>1623</v>
       </c>
       <c r="AH214">
         <v>5</v>
@@ -24170,10 +24338,10 @@
         <v>0.56010000000000004</v>
       </c>
       <c r="AF215">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="AG215" t="s">
-        <v>16</v>
+        <v>1625</v>
       </c>
       <c r="AH215">
         <v>5</v>
@@ -24271,10 +24439,10 @@
         <v>0.21000000000000002</v>
       </c>
       <c r="AF216">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="AG216" t="s">
-        <v>407</v>
+        <v>469</v>
       </c>
       <c r="AH216">
         <v>5</v>
@@ -24366,10 +24534,10 @@
         <v>0.69989999999999997</v>
       </c>
       <c r="AF217">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="AG217" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="AH217">
         <v>5</v>
@@ -24470,10 +24638,10 @@
         <v>0.24990000000000001</v>
       </c>
       <c r="AF218">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="AG218" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="AH218">
         <v>5</v>
@@ -24571,10 +24739,10 @@
         <v>0.35009999999999997</v>
       </c>
       <c r="AF219">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="AG219" t="s">
-        <v>427</v>
+        <v>493</v>
       </c>
       <c r="AH219">
         <v>5</v>
@@ -24672,10 +24840,10 @@
         <v>0.3201</v>
       </c>
       <c r="AF220">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="AG220" t="s">
-        <v>441</v>
+        <v>582</v>
       </c>
       <c r="AH220">
         <v>5</v>
@@ -24770,10 +24938,10 @@
         <v>0.33</v>
       </c>
       <c r="AF221">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="AG221" t="s">
-        <v>443</v>
+        <v>500</v>
       </c>
       <c r="AH221">
         <v>5</v>
@@ -24868,10 +25036,10 @@
         <v>0.2001</v>
       </c>
       <c r="AF222">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="AG222" t="s">
-        <v>469</v>
+        <v>67</v>
       </c>
       <c r="AH222">
         <v>5</v>
@@ -24969,10 +25137,10 @@
         <v>0.38009999999999999</v>
       </c>
       <c r="AF223">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="AG223" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AH223">
         <v>5</v>
@@ -25064,10 +25232,10 @@
         <v>0.54</v>
       </c>
       <c r="AF224">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="AG224" t="s">
-        <v>493</v>
+        <v>36</v>
       </c>
       <c r="AH224">
         <v>5</v>
@@ -25162,10 +25330,10 @@
         <v>0.15989999999999999</v>
       </c>
       <c r="AF225">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="AG225" t="s">
-        <v>582</v>
+        <v>531</v>
       </c>
       <c r="AH225">
         <v>5</v>
@@ -25257,10 +25425,10 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="AF226">
-        <v>133</v>
+        <v>207</v>
       </c>
       <c r="AG226" t="s">
-        <v>496</v>
+        <v>1638</v>
       </c>
       <c r="AH226">
         <v>5</v>
@@ -25352,10 +25520,10 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="AF227">
-        <v>139</v>
+        <v>222</v>
       </c>
       <c r="AG227" t="s">
-        <v>500</v>
+        <v>802</v>
       </c>
       <c r="AH227">
         <v>5</v>
@@ -25450,10 +25618,10 @@
         <v>0.39990000000000003</v>
       </c>
       <c r="AF228">
-        <v>144</v>
+        <v>240</v>
       </c>
       <c r="AG228" t="s">
-        <v>67</v>
+        <v>806</v>
       </c>
       <c r="AH228">
         <v>5</v>
@@ -25560,10 +25728,10 @@
         <v>0.24</v>
       </c>
       <c r="AF229">
-        <v>157</v>
+        <v>242</v>
       </c>
       <c r="AG229" t="s">
-        <v>38</v>
+        <v>1127</v>
       </c>
       <c r="AH229">
         <v>5</v>
@@ -25670,10 +25838,10 @@
         <v>0.27989999999999998</v>
       </c>
       <c r="AF230">
-        <v>160</v>
+        <v>246</v>
       </c>
       <c r="AG230" t="s">
-        <v>36</v>
+        <v>1133</v>
       </c>
       <c r="AH230">
         <v>5</v>
@@ -25780,10 +25948,10 @@
         <v>0.6</v>
       </c>
       <c r="AF231">
-        <v>183</v>
+        <v>258</v>
       </c>
       <c r="AG231" t="s">
-        <v>94</v>
+        <v>1145</v>
       </c>
       <c r="AH231">
         <v>5</v>
@@ -25887,10 +26055,10 @@
         <v>0.6</v>
       </c>
       <c r="AF232">
-        <v>194</v>
+        <v>262</v>
       </c>
       <c r="AG232" t="s">
-        <v>531</v>
+        <v>1149</v>
       </c>
       <c r="AH232">
         <v>5</v>
@@ -25994,10 +26162,10 @@
         <v>0.42</v>
       </c>
       <c r="AF233">
-        <v>196</v>
+        <v>266</v>
       </c>
       <c r="AG233" t="s">
-        <v>533</v>
+        <v>1158</v>
       </c>
       <c r="AH233">
         <v>5</v>
@@ -26101,10 +26269,10 @@
         <v>0.5</v>
       </c>
       <c r="AF234">
-        <v>198</v>
+        <v>271</v>
       </c>
       <c r="AG234" t="s">
-        <v>535</v>
+        <v>1165</v>
       </c>
       <c r="AH234">
         <v>5</v>
@@ -26211,10 +26379,10 @@
         <v>0.22</v>
       </c>
       <c r="AF235">
-        <v>201</v>
+        <v>275</v>
       </c>
       <c r="AG235" t="s">
-        <v>538</v>
+        <v>1169</v>
       </c>
       <c r="AH235">
         <v>5</v>
@@ -26315,16 +26483,16 @@
         <v>0.38</v>
       </c>
       <c r="AF236">
-        <v>207</v>
+        <v>3</v>
       </c>
       <c r="AG236" t="s">
-        <v>544</v>
+        <v>391</v>
       </c>
       <c r="AH236">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI236" s="35">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK236">
         <v>206</v>
@@ -26422,16 +26590,16 @@
         <v>0.36</v>
       </c>
       <c r="AF237">
-        <v>214</v>
+        <v>9</v>
       </c>
       <c r="AG237" t="s">
-        <v>551</v>
+        <v>397</v>
       </c>
       <c r="AH237">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI237" s="35">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK237">
         <v>207</v>
@@ -26526,16 +26694,16 @@
         <v>0.23</v>
       </c>
       <c r="AF238">
-        <v>222</v>
+        <v>10</v>
       </c>
       <c r="AG238" t="s">
-        <v>802</v>
+        <v>1587</v>
       </c>
       <c r="AH238">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI238" s="35">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK238">
         <v>208</v>
@@ -26633,16 +26801,16 @@
         <v>0.38</v>
       </c>
       <c r="AF239">
-        <v>242</v>
+        <v>16</v>
       </c>
       <c r="AG239" t="s">
-        <v>1127</v>
+        <v>15</v>
       </c>
       <c r="AH239">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI239" s="35">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK239">
         <v>209</v>
@@ -26743,16 +26911,16 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AF240">
-        <v>262</v>
+        <v>22</v>
       </c>
       <c r="AG240" t="s">
-        <v>1149</v>
+        <v>1598</v>
       </c>
       <c r="AH240">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI240" s="35">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK240">
         <v>210</v>
@@ -26850,16 +27018,16 @@
         <v>0.48</v>
       </c>
       <c r="AF241">
-        <v>275</v>
+        <v>24</v>
       </c>
       <c r="AG241" t="s">
-        <v>1169</v>
+        <v>1600</v>
       </c>
       <c r="AH241">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI241" s="35">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK241">
         <v>211</v>
@@ -26954,16 +27122,16 @@
         <v>0.48</v>
       </c>
       <c r="AF242">
-        <v>294</v>
+        <v>27</v>
       </c>
       <c r="AG242" t="s">
-        <v>1201</v>
+        <v>1602</v>
       </c>
       <c r="AH242">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AI242" s="35">
-        <v>4.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="AK242">
         <v>212</v>
@@ -27060,10 +27228,10 @@
         <v>0.88</v>
       </c>
       <c r="AF243">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="AG243" t="s">
-        <v>398</v>
+        <v>1618</v>
       </c>
       <c r="AH243">
         <v>6</v>
@@ -27162,10 +27330,10 @@
         <v>0.45</v>
       </c>
       <c r="AF244">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="AG244" t="s">
-        <v>15</v>
+        <v>464</v>
       </c>
       <c r="AH244">
         <v>6</v>
@@ -27261,10 +27429,10 @@
         <v>0.36</v>
       </c>
       <c r="AF245">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="AG245" t="s">
-        <v>408</v>
+        <v>1632</v>
       </c>
       <c r="AH245">
         <v>6</v>
@@ -27365,10 +27533,10 @@
         <v>0.35</v>
       </c>
       <c r="AF246">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="AG246" t="s">
-        <v>410</v>
+        <v>477</v>
       </c>
       <c r="AH246">
         <v>6</v>
@@ -27469,10 +27637,10 @@
         <v>1.68</v>
       </c>
       <c r="AF247">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="AG247" t="s">
-        <v>12</v>
+        <v>481</v>
       </c>
       <c r="AH247">
         <v>6</v>
@@ -27570,10 +27738,10 @@
         <v>0.5</v>
       </c>
       <c r="AF248">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="AG248" t="s">
-        <v>434</v>
+        <v>482</v>
       </c>
       <c r="AH248">
         <v>6</v>
@@ -27677,10 +27845,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="AF249">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="AG249" t="s">
-        <v>439</v>
+        <v>486</v>
       </c>
       <c r="AH249">
         <v>6</v>
@@ -27781,10 +27949,10 @@
         <v>0.37</v>
       </c>
       <c r="AF250">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="AG250" t="s">
-        <v>464</v>
+        <v>496</v>
       </c>
       <c r="AH250">
         <v>6</v>
@@ -27885,10 +28053,10 @@
         <v>0.39</v>
       </c>
       <c r="AF251">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="AG251" t="s">
-        <v>465</v>
+        <v>66</v>
       </c>
       <c r="AH251">
         <v>6</v>
@@ -27986,10 +28154,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="AF252">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="AG252" t="s">
-        <v>477</v>
+        <v>502</v>
       </c>
       <c r="AH252">
         <v>6</v>
@@ -28079,10 +28247,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AF253">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="AG253" t="s">
-        <v>481</v>
+        <v>506</v>
       </c>
       <c r="AH253">
         <v>6</v>
@@ -28178,10 +28346,10 @@
         <v>0.33</v>
       </c>
       <c r="AF254">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="AG254" t="s">
-        <v>482</v>
+        <v>511</v>
       </c>
       <c r="AH254">
         <v>6</v>
@@ -28280,10 +28448,10 @@
         <v>0.36</v>
       </c>
       <c r="AF255">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="AG255" t="s">
-        <v>486</v>
+        <v>94</v>
       </c>
       <c r="AH255">
         <v>6</v>
@@ -28384,10 +28552,10 @@
         <v>0.3</v>
       </c>
       <c r="AF256">
-        <v>120</v>
+        <v>186</v>
       </c>
       <c r="AG256" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="AH256">
         <v>6</v>
@@ -28491,10 +28659,10 @@
         <v>0.25</v>
       </c>
       <c r="AF257">
-        <v>128</v>
+        <v>196</v>
       </c>
       <c r="AG257" t="s">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="AH257">
         <v>6</v>
@@ -28595,10 +28763,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="AF258">
-        <v>141</v>
+        <v>198</v>
       </c>
       <c r="AG258" t="s">
-        <v>66</v>
+        <v>535</v>
       </c>
       <c r="AH258">
         <v>6</v>
@@ -28699,10 +28867,10 @@
         <v>0.25</v>
       </c>
       <c r="AF259">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="AG259" t="s">
-        <v>502</v>
+        <v>538</v>
       </c>
       <c r="AH259">
         <v>6</v>
@@ -28806,10 +28974,10 @@
         <v>0.6</v>
       </c>
       <c r="AF260">
-        <v>147</v>
+        <v>214</v>
       </c>
       <c r="AG260" t="s">
-        <v>506</v>
+        <v>551</v>
       </c>
       <c r="AH260">
         <v>6</v>
@@ -28910,10 +29078,10 @@
         <v>1.7199999999999998</v>
       </c>
       <c r="AF261">
-        <v>152</v>
+        <v>250</v>
       </c>
       <c r="AG261" t="s">
-        <v>511</v>
+        <v>1135</v>
       </c>
       <c r="AH261">
         <v>6</v>
@@ -29121,10 +29289,10 @@
         <v>0.8899999999999999</v>
       </c>
       <c r="AF263">
-        <v>273</v>
+        <v>294</v>
       </c>
       <c r="AG263" t="s">
-        <v>1167</v>
+        <v>1201</v>
       </c>
       <c r="AH263">
         <v>6</v>
@@ -29231,13 +29399,13 @@
         <v>15</v>
       </c>
       <c r="AG264" t="s">
-        <v>403</v>
+        <v>1592</v>
       </c>
       <c r="AH264">
         <v>7</v>
       </c>
       <c r="AI264" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK264">
         <v>234</v>
@@ -29339,13 +29507,13 @@
         <v>19</v>
       </c>
       <c r="AG265" t="s">
-        <v>405</v>
+        <v>1595</v>
       </c>
       <c r="AH265">
         <v>7</v>
       </c>
       <c r="AI265" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK265">
         <v>235</v>
@@ -29444,13 +29612,13 @@
         <v>25</v>
       </c>
       <c r="AG266" t="s">
-        <v>411</v>
+        <v>1601</v>
       </c>
       <c r="AH266">
         <v>7</v>
       </c>
       <c r="AI266" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK266">
         <v>236</v>
@@ -29552,7 +29720,7 @@
         <v>7</v>
       </c>
       <c r="AI267" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK267">
         <v>237</v>
@@ -29657,7 +29825,7 @@
         <v>7</v>
       </c>
       <c r="AI268" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK268">
         <v>238</v>
@@ -29753,16 +29921,16 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="AF269">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="AG269" t="s">
-        <v>424</v>
+        <v>1616</v>
       </c>
       <c r="AH269">
         <v>7</v>
       </c>
       <c r="AI269" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK269">
         <v>239</v>
@@ -29858,16 +30026,16 @@
         <v>0.45999999999999996</v>
       </c>
       <c r="AF270">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="AG270" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="AH270">
         <v>7</v>
       </c>
       <c r="AI270" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK270">
         <v>240</v>
@@ -29966,16 +30134,16 @@
         <v>0.53</v>
       </c>
       <c r="AF271">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="AG271" t="s">
-        <v>432</v>
+        <v>1090</v>
       </c>
       <c r="AH271">
         <v>7</v>
       </c>
       <c r="AI271" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK271">
         <v>241</v>
@@ -30059,16 +30227,16 @@
         <v>0.65</v>
       </c>
       <c r="AF272">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="AG272" t="s">
-        <v>1090</v>
+        <v>467</v>
       </c>
       <c r="AH272">
         <v>7</v>
       </c>
       <c r="AI272" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK272">
         <v>242</v>
@@ -30152,16 +30320,16 @@
         <v>0.59</v>
       </c>
       <c r="AF273">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="AG273" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="AH273">
         <v>7</v>
       </c>
       <c r="AI273" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK273">
         <v>243</v>
@@ -30245,16 +30413,16 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="AF274">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="AG274" t="s">
-        <v>473</v>
+        <v>63</v>
       </c>
       <c r="AH274">
         <v>7</v>
       </c>
       <c r="AI274" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK274">
         <v>244</v>
@@ -30335,16 +30503,16 @@
         <v>0.77</v>
       </c>
       <c r="AF275">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="AG275" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="AH275">
         <v>7</v>
       </c>
       <c r="AI275" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK275">
         <v>245</v>
@@ -30434,16 +30602,16 @@
         <v>1.31</v>
       </c>
       <c r="AF276">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="AG276" t="s">
-        <v>63</v>
+        <v>518</v>
       </c>
       <c r="AH276">
         <v>7</v>
       </c>
       <c r="AI276" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK276">
         <v>246</v>
@@ -30536,16 +30704,16 @@
         <v>0.62</v>
       </c>
       <c r="AF277">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="AG277" t="s">
-        <v>503</v>
+        <v>523</v>
       </c>
       <c r="AH277">
         <v>7</v>
       </c>
       <c r="AI277" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK277">
         <v>247</v>
@@ -30635,16 +30803,16 @@
         <v>0.69000000000000006</v>
       </c>
       <c r="AF278">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="AG278" t="s">
-        <v>518</v>
+        <v>1639</v>
       </c>
       <c r="AH278">
         <v>7</v>
       </c>
       <c r="AI278" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK278">
         <v>248</v>
@@ -30740,16 +30908,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AF279">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="AG279" t="s">
-        <v>523</v>
+        <v>1642</v>
       </c>
       <c r="AH279">
         <v>7</v>
       </c>
       <c r="AI279" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK279">
         <v>249</v>
@@ -30839,16 +31007,16 @@
         <v>1.45</v>
       </c>
       <c r="AF280">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="AG280" t="s">
-        <v>545</v>
+        <v>563</v>
       </c>
       <c r="AH280">
         <v>7</v>
       </c>
       <c r="AI280" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK280">
         <v>250</v>
@@ -30938,16 +31106,16 @@
         <v>0.52980000000000005</v>
       </c>
       <c r="AF281">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="AG281" t="s">
-        <v>561</v>
+        <v>1132</v>
       </c>
       <c r="AH281">
         <v>7</v>
       </c>
       <c r="AI281" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="AK281">
         <v>251</v>
@@ -31043,16 +31211,16 @@
         <v>0.5202</v>
       </c>
       <c r="AF282">
-        <v>227</v>
+        <v>12</v>
       </c>
       <c r="AG282" t="s">
-        <v>563</v>
+        <v>1589</v>
       </c>
       <c r="AH282">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI282" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK282">
         <v>252</v>
@@ -31145,16 +31313,16 @@
         <v>0.52980000000000005</v>
       </c>
       <c r="AF283">
-        <v>245</v>
+        <v>40</v>
       </c>
       <c r="AG283" t="s">
-        <v>1132</v>
+        <v>424</v>
       </c>
       <c r="AH283">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI283" s="35">
-        <v>5.5999999999999999E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK283">
         <v>253</v>
@@ -31246,16 +31414,16 @@
         <v>0.85019999999999996</v>
       </c>
       <c r="AF284">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="AG284" t="s">
-        <v>400</v>
+        <v>1614</v>
       </c>
       <c r="AH284">
         <v>8</v>
       </c>
       <c r="AI284" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK284">
         <v>254</v>
@@ -31350,13 +31518,13 @@
         <v>61</v>
       </c>
       <c r="AG285" t="s">
-        <v>437</v>
+        <v>1621</v>
       </c>
       <c r="AH285">
         <v>8</v>
       </c>
       <c r="AI285" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK285">
         <v>255</v>
@@ -31458,7 +31626,7 @@
         <v>8</v>
       </c>
       <c r="AI286" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK286">
         <v>256</v>
@@ -31548,13 +31716,13 @@
         <v>96</v>
       </c>
       <c r="AG287" t="s">
-        <v>472</v>
+        <v>1635</v>
       </c>
       <c r="AH287">
         <v>8</v>
       </c>
       <c r="AI287" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK287">
         <v>257</v>
@@ -31653,7 +31821,7 @@
         <v>8</v>
       </c>
       <c r="AI288" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK288">
         <v>258</v>
@@ -31746,16 +31914,16 @@
         <v>0.97020000000000006</v>
       </c>
       <c r="AF289">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="AG289" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
       <c r="AH289">
         <v>8</v>
       </c>
       <c r="AI289" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK289">
         <v>259</v>
@@ -31842,16 +32010,16 @@
         <v>0.86999999999999988</v>
       </c>
       <c r="AF290">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="AG290" t="s">
-        <v>504</v>
+        <v>1072</v>
       </c>
       <c r="AH290">
         <v>8</v>
       </c>
       <c r="AI290" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK290">
         <v>260</v>
@@ -31941,16 +32109,16 @@
         <v>0.85980000000000012</v>
       </c>
       <c r="AF291">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="AG291" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="AH291">
         <v>8</v>
       </c>
       <c r="AI291" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK291">
         <v>261</v>
@@ -32037,16 +32205,16 @@
         <v>3.7002000000000002</v>
       </c>
       <c r="AF292">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="AG292" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="AH292">
         <v>8</v>
       </c>
       <c r="AI292" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK292">
         <v>262</v>
@@ -32139,16 +32307,16 @@
         <v>0.39</v>
       </c>
       <c r="AF293">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="AG293" t="s">
-        <v>70</v>
+        <v>508</v>
       </c>
       <c r="AH293">
         <v>8</v>
       </c>
       <c r="AI293" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK293">
         <v>263</v>
@@ -32238,16 +32406,16 @@
         <v>0.81</v>
       </c>
       <c r="AF294">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="AG294" t="s">
-        <v>574</v>
+        <v>70</v>
       </c>
       <c r="AH294">
         <v>8</v>
       </c>
       <c r="AI294" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK294">
         <v>264</v>
@@ -32337,16 +32505,16 @@
         <v>0.88979999999999992</v>
       </c>
       <c r="AF295">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="AG295" t="s">
-        <v>527</v>
+        <v>574</v>
       </c>
       <c r="AH295">
         <v>8</v>
       </c>
       <c r="AI295" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK295">
         <v>265</v>
@@ -32444,16 +32612,16 @@
         <v>0.59989999999999999</v>
       </c>
       <c r="AF296">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="AG296" t="s">
-        <v>553</v>
+        <v>527</v>
       </c>
       <c r="AH296">
         <v>8</v>
       </c>
       <c r="AI296" s="35">
-        <v>6.4000000000000003E-3</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK296">
         <v>266</v>
@@ -32545,10 +32713,10 @@
         <v>1.2803</v>
       </c>
       <c r="AF297">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AG297" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="AH297">
         <v>9</v>
@@ -32652,10 +32820,10 @@
         <v>0.83019999999999994</v>
       </c>
       <c r="AF298">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="AG298" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="AH298">
         <v>9</v>
@@ -32759,10 +32927,10 @@
         <v>1.9298999999999999</v>
       </c>
       <c r="AF299">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="AG299" t="s">
-        <v>396</v>
+        <v>579</v>
       </c>
       <c r="AH299">
         <v>9</v>
@@ -32863,10 +33031,10 @@
         <v>1.5498000000000001</v>
       </c>
       <c r="AF300">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="AG300" t="s">
-        <v>418</v>
+        <v>1629</v>
       </c>
       <c r="AH300">
         <v>9</v>
@@ -32970,10 +33138,10 @@
         <v>0.49980000000000002</v>
       </c>
       <c r="AF301">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="AG301" t="s">
-        <v>579</v>
+        <v>489</v>
       </c>
       <c r="AH301">
         <v>9</v>
@@ -33071,10 +33239,10 @@
         <v>0.63979999999999992</v>
       </c>
       <c r="AF302">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="AG302" t="s">
-        <v>453</v>
+        <v>580</v>
       </c>
       <c r="AH302">
         <v>9</v>
@@ -33175,10 +33343,10 @@
         <v>0.46970000000000006</v>
       </c>
       <c r="AF303">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="AG303" t="s">
-        <v>455</v>
+        <v>504</v>
       </c>
       <c r="AH303">
         <v>9</v>
@@ -33276,10 +33444,10 @@
         <v>0.86029999999999995</v>
       </c>
       <c r="AF304">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="AG304" t="s">
-        <v>100</v>
+        <v>514</v>
       </c>
       <c r="AH304">
         <v>9</v>
@@ -33375,10 +33543,10 @@
         <v>0.73040000000000005</v>
       </c>
       <c r="AF305">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="AG305" t="s">
-        <v>489</v>
+        <v>525</v>
       </c>
       <c r="AH305">
         <v>9</v>
@@ -33474,10 +33642,10 @@
         <v>6.2504</v>
       </c>
       <c r="AF306">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="AG306" t="s">
-        <v>525</v>
+        <v>553</v>
       </c>
       <c r="AH306">
         <v>9</v>
@@ -33771,16 +33939,16 @@
         <v>1.52</v>
       </c>
       <c r="AF309">
-        <v>28</v>
+        <v>277</v>
       </c>
       <c r="AG309" t="s">
-        <v>412</v>
+        <v>1171</v>
       </c>
       <c r="AH309">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AI309" s="35">
-        <v>7.9000000000000008E-3</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="AK309">
         <v>279</v>
@@ -33870,10 +34038,10 @@
         <v>1.6104000000000001</v>
       </c>
       <c r="AF310">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="AG310" t="s">
-        <v>436</v>
+        <v>389</v>
       </c>
       <c r="AH310">
         <v>10</v>
@@ -33974,10 +34142,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AF311">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="AG311" t="s">
-        <v>463</v>
+        <v>1603</v>
       </c>
       <c r="AH311">
         <v>10</v>
@@ -34075,10 +34243,10 @@
         <v>0.78959999999999997</v>
       </c>
       <c r="AF312">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="AG312" t="s">
-        <v>479</v>
+        <v>1620</v>
       </c>
       <c r="AH312">
         <v>10</v>
@@ -34176,10 +34344,10 @@
         <v>1.3301999999999998</v>
       </c>
       <c r="AF313">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="AG313" t="s">
-        <v>580</v>
+        <v>463</v>
       </c>
       <c r="AH313">
         <v>10</v>
@@ -34280,10 +34448,10 @@
         <v>0.69030000000000002</v>
       </c>
       <c r="AF314">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="AG314" t="s">
-        <v>1072</v>
+        <v>479</v>
       </c>
       <c r="AH314">
         <v>10</v>
@@ -34592,10 +34760,10 @@
         <v>509</v>
       </c>
       <c r="AH317">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AI317" s="35">
-        <v>8.6999999999999994E-3</v>
+        <v>7.9000000000000008E-3</v>
       </c>
       <c r="AK317">
         <v>287</v>
@@ -34684,10 +34852,10 @@
         <v>1.37</v>
       </c>
       <c r="AF318">
-        <v>170</v>
+        <v>107</v>
       </c>
       <c r="AG318" t="s">
-        <v>520</v>
+        <v>100</v>
       </c>
       <c r="AH318">
         <v>11</v>
@@ -34786,16 +34954,16 @@
         <v>2.3595000000000002</v>
       </c>
       <c r="AF319">
-        <v>47</v>
+        <v>273</v>
       </c>
       <c r="AG319" t="s">
-        <v>426</v>
+        <v>1167</v>
       </c>
       <c r="AH319">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AI319" s="35">
-        <v>9.4999999999999998E-3</v>
+        <v>8.6999999999999994E-3</v>
       </c>
       <c r="AK319">
         <v>289</v>
@@ -34891,7 +35059,7 @@
         <v>74</v>
       </c>
       <c r="AG320" t="s">
-        <v>450</v>
+        <v>1627</v>
       </c>
       <c r="AH320">
         <v>12</v>
@@ -34987,10 +35155,10 @@
         <v>1.7199</v>
       </c>
       <c r="AF321">
-        <v>210</v>
+        <v>77</v>
       </c>
       <c r="AG321" t="s">
-        <v>547</v>
+        <v>453</v>
       </c>
       <c r="AH321">
         <v>12</v>
@@ -35086,16 +35254,16 @@
         <v>4.5094000000000003</v>
       </c>
       <c r="AF322">
-        <v>3</v>
+        <v>170</v>
       </c>
       <c r="AG322" t="s">
-        <v>391</v>
+        <v>520</v>
       </c>
       <c r="AH322">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AI322" s="35">
-        <v>1.11E-2</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="AK322">
         <v>292</v>
@@ -35182,16 +35350,16 @@
         <v>3.9000000000000004</v>
       </c>
       <c r="AF323">
-        <v>9</v>
+        <v>210</v>
       </c>
       <c r="AG323" t="s">
-        <v>397</v>
+        <v>547</v>
       </c>
       <c r="AH323">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AI323" s="35">
-        <v>1.11E-2</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="AK323">
         <v>293</v>
@@ -35281,16 +35449,16 @@
         <v>2.3008000000000002</v>
       </c>
       <c r="AF324">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="AG324" t="s">
-        <v>40</v>
+        <v>1607</v>
       </c>
       <c r="AH324">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AI324" s="35">
-        <v>1.11E-2</v>
+        <v>1.03E-2</v>
       </c>
       <c r="AK324">
         <v>294</v>
@@ -35377,16 +35545,16 @@
         <v>2.16</v>
       </c>
       <c r="AF325">
-        <v>6</v>
+        <v>159</v>
       </c>
       <c r="AG325" t="s">
-        <v>394</v>
+        <v>40</v>
       </c>
       <c r="AH325">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AI325" s="35">
-        <v>1.35E-2</v>
+        <v>1.11E-2</v>
       </c>
       <c r="AK325">
         <v>295</v>

</xml_diff>

<commit_message>
Bug fixes and a few cool features!
</commit_message>
<xml_diff>
--- a/PokemonGame/stuff/pokemon game.xlsx
+++ b/PokemonGame/stuff/pokemon game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjkuhnke\git\PokemonGame\PokemonGame\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D88453-59DA-419B-9705-C5025A44AFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C39BC9-8A76-4EF5-B6CA-4C3F309C7987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BD02A17-B686-4FC4-8065-C777F779E0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4748,15 +4748,6 @@
     <t xml:space="preserve">NPC </t>
   </si>
   <si>
-    <t>4. Cinneroph</t>
-  </si>
-  <si>
-    <t>5. Geniova+</t>
-  </si>
-  <si>
-    <t>6. Bronzong</t>
-  </si>
-  <si>
     <t>1. Shocky Spire</t>
   </si>
   <si>
@@ -4775,9 +4766,6 @@
     <t>3. Swalot</t>
   </si>
   <si>
-    <t>7. Hissimitar</t>
-  </si>
-  <si>
     <t>1. Blaster</t>
   </si>
   <si>
@@ -5004,6 +4992,18 @@
   </si>
   <si>
     <t>Letter 2</t>
+  </si>
+  <si>
+    <t>5. Bronzong</t>
+  </si>
+  <si>
+    <t>6. Cinneroph</t>
+  </si>
+  <si>
+    <t>7. Geniova+</t>
+  </si>
+  <si>
+    <t>4. Hissimitar</t>
   </si>
 </sst>
 </file>
@@ -6041,8 +6041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCD2C10-9C1D-4BA8-9034-8E41B08DF934}">
   <dimension ref="A1:AW620"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP39" sqref="AP39"/>
+    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8085,7 +8085,7 @@
         <v>5</v>
       </c>
       <c r="AL31" t="s">
-        <v>1642</v>
+        <v>1638</v>
       </c>
       <c r="AM31">
         <v>0</v>
@@ -8297,16 +8297,16 @@
         <v>415</v>
       </c>
       <c r="N34" t="s">
-        <v>1580</v>
+        <v>1576</v>
       </c>
       <c r="O34" t="s">
         <v>1104</v>
       </c>
       <c r="P34" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="Q34" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="U34" t="s">
         <v>208</v>
@@ -8385,7 +8385,7 @@
         <v>400</v>
       </c>
       <c r="N35" t="s">
-        <v>1581</v>
+        <v>1577</v>
       </c>
       <c r="O35" t="s">
         <v>1105</v>
@@ -8473,10 +8473,10 @@
         <v>400</v>
       </c>
       <c r="N36" t="s">
-        <v>1582</v>
+        <v>1578</v>
       </c>
       <c r="O36" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="P36" t="s">
         <v>1108</v>
@@ -8561,13 +8561,13 @@
         <v>435</v>
       </c>
       <c r="N37" t="s">
-        <v>1583</v>
+        <v>1579</v>
       </c>
       <c r="O37" t="s">
         <v>1106</v>
       </c>
       <c r="P37" t="s">
-        <v>1570</v>
+        <v>1655</v>
       </c>
       <c r="Q37" t="s">
         <v>1111</v>
@@ -8646,13 +8646,13 @@
         <v>400</v>
       </c>
       <c r="N38" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
       <c r="O38" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="P38" t="s">
-        <v>1571</v>
+        <v>1652</v>
       </c>
       <c r="Q38" t="s">
         <v>1112</v>
@@ -8731,13 +8731,13 @@
         <v>500</v>
       </c>
       <c r="N39" t="s">
-        <v>1585</v>
+        <v>1581</v>
       </c>
       <c r="O39" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="P39" t="s">
-        <v>1572</v>
+        <v>1653</v>
       </c>
       <c r="Q39" t="s">
         <v>1113</v>
@@ -8819,7 +8819,7 @@
         <v>1085</v>
       </c>
       <c r="P40" t="s">
-        <v>1579</v>
+        <v>1654</v>
       </c>
       <c r="Q40" t="s">
         <v>1114</v>
@@ -9053,7 +9053,7 @@
         <v>500</v>
       </c>
       <c r="O43" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="P43" t="s">
         <v>1117</v>
@@ -9528,7 +9528,7 @@
         <v>205</v>
       </c>
       <c r="AG49" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
       <c r="AH49">
         <v>1</v>
@@ -9604,7 +9604,7 @@
         <v>206</v>
       </c>
       <c r="AG50" t="s">
-        <v>1636</v>
+        <v>1632</v>
       </c>
       <c r="AH50">
         <v>1</v>
@@ -9762,7 +9762,7 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s">
-        <v>1643</v>
+        <v>1639</v>
       </c>
       <c r="AM52">
         <v>0</v>
@@ -11396,7 +11396,7 @@
         <v>23</v>
       </c>
       <c r="AG69" t="s">
-        <v>1598</v>
+        <v>1594</v>
       </c>
       <c r="AH69">
         <v>2</v>
@@ -11887,7 +11887,7 @@
         <v>41</v>
       </c>
       <c r="AG74" t="s">
-        <v>1603</v>
+        <v>1599</v>
       </c>
       <c r="AH74">
         <v>2</v>
@@ -12140,7 +12140,7 @@
         <v>48</v>
       </c>
       <c r="AG77" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="AH77">
         <v>2</v>
@@ -12213,7 +12213,7 @@
         <v>49</v>
       </c>
       <c r="AG78" t="s">
-        <v>1608</v>
+        <v>1604</v>
       </c>
       <c r="AH78">
         <v>2</v>
@@ -12289,7 +12289,7 @@
         <v>53</v>
       </c>
       <c r="AG79" t="s">
-        <v>1612</v>
+        <v>1608</v>
       </c>
       <c r="AH79">
         <v>2</v>
@@ -12362,7 +12362,7 @@
         <v>55</v>
       </c>
       <c r="AG80" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="AH80">
         <v>2</v>
@@ -12435,7 +12435,7 @@
         <v>59</v>
       </c>
       <c r="AG81" t="s">
-        <v>1618</v>
+        <v>1614</v>
       </c>
       <c r="AH81">
         <v>2</v>
@@ -12733,7 +12733,7 @@
         <v>73</v>
       </c>
       <c r="AG85" t="s">
-        <v>1625</v>
+        <v>1621</v>
       </c>
       <c r="AH85">
         <v>2</v>
@@ -13034,7 +13034,7 @@
         <v>94</v>
       </c>
       <c r="AG89" t="s">
-        <v>1632</v>
+        <v>1628</v>
       </c>
       <c r="AH89">
         <v>2</v>
@@ -13110,7 +13110,7 @@
         <v>95</v>
       </c>
       <c r="AG90" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
       <c r="AH90">
         <v>2</v>
@@ -14992,7 +14992,7 @@
         <v>292</v>
       </c>
       <c r="AL115" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="AM115">
         <v>0</v>
@@ -15065,7 +15065,7 @@
         <v>293</v>
       </c>
       <c r="AL116" t="s">
-        <v>1649</v>
+        <v>1645</v>
       </c>
       <c r="AM116">
         <v>0</v>
@@ -15138,7 +15138,7 @@
         <v>294</v>
       </c>
       <c r="AL117" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
       <c r="AM117">
         <v>0</v>
@@ -15211,7 +15211,7 @@
         <v>295</v>
       </c>
       <c r="AL118" t="s">
-        <v>1651</v>
+        <v>1647</v>
       </c>
       <c r="AM118">
         <v>0</v>
@@ -15357,7 +15357,7 @@
         <v>297</v>
       </c>
       <c r="AL120" t="s">
-        <v>1652</v>
+        <v>1648</v>
       </c>
       <c r="AM120">
         <v>0</v>
@@ -15418,7 +15418,7 @@
         <v>223</v>
       </c>
       <c r="AG121" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="AH121">
         <v>2</v>
@@ -15430,7 +15430,7 @@
         <v>298</v>
       </c>
       <c r="AL121" t="s">
-        <v>1653</v>
+        <v>1649</v>
       </c>
       <c r="AM121">
         <v>0</v>
@@ -15491,7 +15491,7 @@
         <v>224</v>
       </c>
       <c r="AG122" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
       <c r="AH122">
         <v>2</v>
@@ -16665,7 +16665,7 @@
         <v>11</v>
       </c>
       <c r="AG138" t="s">
-        <v>1587</v>
+        <v>1583</v>
       </c>
       <c r="AH138">
         <v>3</v>
@@ -17054,7 +17054,7 @@
         <v>52</v>
       </c>
       <c r="AG143" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="AH143">
         <v>3</v>
@@ -17146,7 +17146,7 @@
         <v>57</v>
       </c>
       <c r="AG144" t="s">
-        <v>1616</v>
+        <v>1612</v>
       </c>
       <c r="AH144">
         <v>3</v>
@@ -17231,7 +17231,7 @@
         <v>66</v>
       </c>
       <c r="AG145" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
       <c r="AH145">
         <v>3</v>
@@ -17341,7 +17341,7 @@
         <v>80</v>
       </c>
       <c r="AG146" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="AH146">
         <v>3</v>
@@ -18616,7 +18616,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="AL158" t="s">
-        <v>1645</v>
+        <v>1641</v>
       </c>
       <c r="AM158">
         <v>0</v>
@@ -18720,7 +18720,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="AL159" t="s">
-        <v>1646</v>
+        <v>1642</v>
       </c>
       <c r="AM159">
         <v>0</v>
@@ -18821,7 +18821,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="AL160" t="s">
-        <v>1655</v>
+        <v>1651</v>
       </c>
       <c r="AM160">
         <v>0</v>
@@ -19980,7 +19980,7 @@
         <v>14</v>
       </c>
       <c r="AG171" t="s">
-        <v>1590</v>
+        <v>1586</v>
       </c>
       <c r="AH171">
         <v>4</v>
@@ -20088,7 +20088,7 @@
         <v>20</v>
       </c>
       <c r="AG172" t="s">
-        <v>1595</v>
+        <v>1591</v>
       </c>
       <c r="AH172">
         <v>4</v>
@@ -20100,7 +20100,7 @@
         <v>91</v>
       </c>
       <c r="AL172" t="s">
-        <v>1644</v>
+        <v>1640</v>
       </c>
       <c r="AM172">
         <v>1</v>
@@ -20187,7 +20187,7 @@
         <v>64</v>
       </c>
       <c r="AG173" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="AH173">
         <v>4</v>
@@ -20496,7 +20496,7 @@
         <v>78</v>
       </c>
       <c r="AG176" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
       <c r="AH176">
         <v>4</v>
@@ -20598,7 +20598,7 @@
         <v>81</v>
       </c>
       <c r="AG177" t="s">
-        <v>1630</v>
+        <v>1626</v>
       </c>
       <c r="AH177">
         <v>4</v>
@@ -21429,7 +21429,7 @@
         <v>107</v>
       </c>
       <c r="AL185" t="s">
-        <v>1647</v>
+        <v>1643</v>
       </c>
       <c r="AM185">
         <v>1</v>
@@ -22950,7 +22950,7 @@
         <v>13</v>
       </c>
       <c r="AG200" t="s">
-        <v>1589</v>
+        <v>1585</v>
       </c>
       <c r="AH200">
         <v>5</v>
@@ -23051,7 +23051,7 @@
         <v>17</v>
       </c>
       <c r="AG201" t="s">
-        <v>1592</v>
+        <v>1588</v>
       </c>
       <c r="AH201">
         <v>5</v>
@@ -23152,7 +23152,7 @@
         <v>18</v>
       </c>
       <c r="AG202" t="s">
-        <v>1593</v>
+        <v>1589</v>
       </c>
       <c r="AH202">
         <v>5</v>
@@ -23354,7 +23354,7 @@
         <v>42</v>
       </c>
       <c r="AG204" t="s">
-        <v>1604</v>
+        <v>1600</v>
       </c>
       <c r="AH204">
         <v>5</v>
@@ -23452,7 +23452,7 @@
         <v>43</v>
       </c>
       <c r="AG205" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="AH205">
         <v>5</v>
@@ -23550,7 +23550,7 @@
         <v>67</v>
       </c>
       <c r="AG206" t="s">
-        <v>1624</v>
+        <v>1620</v>
       </c>
       <c r="AH206">
         <v>5</v>
@@ -24719,7 +24719,7 @@
         <v>10</v>
       </c>
       <c r="AG218" t="s">
-        <v>1586</v>
+        <v>1582</v>
       </c>
       <c r="AH218">
         <v>6</v>
@@ -24918,7 +24918,7 @@
         <v>21</v>
       </c>
       <c r="AG220" t="s">
-        <v>1596</v>
+        <v>1592</v>
       </c>
       <c r="AH220">
         <v>6</v>
@@ -25016,7 +25016,7 @@
         <v>22</v>
       </c>
       <c r="AG221" t="s">
-        <v>1597</v>
+        <v>1593</v>
       </c>
       <c r="AH221">
         <v>6</v>
@@ -25111,7 +25111,7 @@
         <v>27</v>
       </c>
       <c r="AG222" t="s">
-        <v>1601</v>
+        <v>1597</v>
       </c>
       <c r="AH222">
         <v>6</v>
@@ -25212,7 +25212,7 @@
         <v>50</v>
       </c>
       <c r="AG223" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="AH223">
         <v>6</v>
@@ -25307,7 +25307,7 @@
         <v>65</v>
       </c>
       <c r="AG224" t="s">
-        <v>1622</v>
+        <v>1618</v>
       </c>
       <c r="AH224">
         <v>6</v>
@@ -26121,7 +26121,7 @@
         <v>207</v>
       </c>
       <c r="AG232" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="AH232">
         <v>6</v>
@@ -27396,7 +27396,7 @@
         <v>19</v>
       </c>
       <c r="AG244" t="s">
-        <v>1594</v>
+        <v>1590</v>
       </c>
       <c r="AH244">
         <v>7</v>
@@ -27495,7 +27495,7 @@
         <v>25</v>
       </c>
       <c r="AG245" t="s">
-        <v>1600</v>
+        <v>1596</v>
       </c>
       <c r="AH245">
         <v>7</v>
@@ -27599,7 +27599,7 @@
         <v>51</v>
       </c>
       <c r="AG246" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
       <c r="AH246">
         <v>7</v>
@@ -27703,7 +27703,7 @@
         <v>54</v>
       </c>
       <c r="AG247" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="AH247">
         <v>7</v>
@@ -27804,7 +27804,7 @@
         <v>56</v>
       </c>
       <c r="AG248" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="AH248">
         <v>7</v>
@@ -29675,7 +29675,7 @@
         <v>15</v>
       </c>
       <c r="AG266" t="s">
-        <v>1591</v>
+        <v>1587</v>
       </c>
       <c r="AH266">
         <v>8</v>
@@ -29780,7 +29780,7 @@
         <v>24</v>
       </c>
       <c r="AG267" t="s">
-        <v>1599</v>
+        <v>1595</v>
       </c>
       <c r="AH267">
         <v>8</v>
@@ -30086,7 +30086,7 @@
         <v>58</v>
       </c>
       <c r="AG270" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="AH270">
         <v>8</v>
@@ -31680,7 +31680,7 @@
         <v>208</v>
       </c>
       <c r="AG286" t="s">
-        <v>1638</v>
+        <v>1634</v>
       </c>
       <c r="AH286">
         <v>8</v>
@@ -31776,7 +31776,7 @@
         <v>225</v>
       </c>
       <c r="AG287" t="s">
-        <v>1641</v>
+        <v>1637</v>
       </c>
       <c r="AH287">
         <v>8</v>
@@ -32169,7 +32169,7 @@
         <v>12</v>
       </c>
       <c r="AG291" t="s">
-        <v>1588</v>
+        <v>1584</v>
       </c>
       <c r="AH291">
         <v>9</v>
@@ -32265,7 +32265,7 @@
         <v>28</v>
       </c>
       <c r="AG292" t="s">
-        <v>1602</v>
+        <v>1598</v>
       </c>
       <c r="AH292">
         <v>9</v>
@@ -32660,7 +32660,7 @@
         <v>61</v>
       </c>
       <c r="AG296" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
       <c r="AH296">
         <v>9</v>
@@ -32865,7 +32865,7 @@
         <v>89</v>
       </c>
       <c r="AG298" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="AH298">
         <v>9</v>
@@ -32969,7 +32969,7 @@
         <v>96</v>
       </c>
       <c r="AG299" t="s">
-        <v>1634</v>
+        <v>1630</v>
       </c>
       <c r="AH299">
         <v>9</v>
@@ -33876,7 +33876,7 @@
         <v>79</v>
       </c>
       <c r="AG308" t="s">
-        <v>1628</v>
+        <v>1624</v>
       </c>
       <c r="AH308">
         <v>10</v>
@@ -34472,7 +34472,7 @@
         <v>60</v>
       </c>
       <c r="AG314" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
       <c r="AH314">
         <v>11</v>
@@ -35071,7 +35071,7 @@
         <v>74</v>
       </c>
       <c r="AG320" t="s">
-        <v>1626</v>
+        <v>1622</v>
       </c>
       <c r="AH320">
         <v>13</v>
@@ -35473,7 +35473,7 @@
         <v>47</v>
       </c>
       <c r="AG324" t="s">
-        <v>1606</v>
+        <v>1602</v>
       </c>
       <c r="AH324">
         <v>14</v>
@@ -36877,7 +36877,7 @@
         <v>845</v>
       </c>
       <c r="Z343" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="AK343">
         <v>33</v>

</xml_diff>